<commit_message>
finalizando step 2 - queda testearlo
</commit_message>
<xml_diff>
--- a/bookings-db/output_files/hotels/hotels.xlsx
+++ b/bookings-db/output_files/hotels/hotels.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -595,6 +595,1221 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>6562</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Regal Chambers</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>{'Country': 'France', 'City': 'Nice', 'ZipCode': '13739', 'Address': '7525 Clark Grove Apt. 928'}</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>{'OccupancyPeakSeasonWeight': 93, 'OccupancyOffSeasonWeight': 30, 'OccupancyBaseDiscountPercentage': 21, 'ExtraBedChargePercentage': 27, 'MealPlanWeights': {'room_only': {'name': 'Room Only', 'weight': 0.1}, 'room_and_breakfast': {'name': 'Room and Breakfast', 'weight': 0.53}, 'all_inclusive': {'name': 'All Inclusive', 'weight': 0.0}, 'half_board': {'name': 'Half Board', 'weight': 0.12}, 'full_board': {'name': 'Full Board', 'weight': 0.25}}, 'MealPlanPrices': {'Room Only': 1.0, 'Room and Breakfast': 1.11, 'All Inclusive': 2.15, 'Half Board': 1.38, 'Full Board': 1.6}, 'PromotionPriceDiscount': 29}</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>[{'RoomId': '01-001', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 92.0, 'PricePeakSeason': 161.92}, {'RoomId': '01-002', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 92.0, 'PricePeakSeason': 161.92}, {'RoomId': '01-003', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 40.0, 'PricePeakSeason': 70.4}, {'RoomId': '01-004', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 40.0, 'PricePeakSeason': 70.4}, {'RoomId': '01-005', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 138.0, 'PricePeakSeason': 242.88}, {'RoomId': '01-006', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 40.0, 'PricePeakSeason': 70.4}, {'RoomId': '01-007', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 138.0, 'PricePeakSeason': 242.88}, {'RoomId': '01-008', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 192.28, 'PricePeakSeason': 338.41}, {'RoomId': '01-009', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 92.0, 'PricePeakSeason': 161.92}, {'RoomId': '01-010', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 138.0, 'PricePeakSeason': 242.88}, {'RoomId': '01-011', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 138.0, 'PricePeakSeason': 242.88}, {'RoomId': '01-012', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 83.6, 'PricePeakSeason': 147.14}, {'RoomId': '01-013', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 192.28, 'PricePeakSeason': 338.41}, {'RoomId': '01-014', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 192.28, 'PricePeakSeason': 338.41}, {'RoomId': '01-015', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 92.0, 'PricePeakSeason': 161.92}, {'RoomId': '01-016', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 40.0, 'PricePeakSeason': 70.4}, {'RoomId': '01-017', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 92.0, 'PricePeakSeason': 161.92}, {'RoomId': '01-018', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 83.6, 'PricePeakSeason': 147.14}, {'RoomId': '02-001', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 138.0, 'PricePeakSeason': 242.88}, {'RoomId': '02-002', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 192.28, 'PricePeakSeason': 338.41}, {'RoomId': '02-003', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 192.28, 'PricePeakSeason': 338.41}, {'RoomId': '02-004', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 92.0, 'PricePeakSeason': 161.92}, {'RoomId': '02-005', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 192.28, 'PricePeakSeason': 338.41}, {'RoomId': '02-006', 'Floor': '02', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 288.42, 'PricePeakSeason': 507.62}, {'RoomId': '02-007', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 92.0, 'PricePeakSeason': 161.92}, {'RoomId': '02-008', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 138.0, 'PricePeakSeason': 242.88}, {'RoomId': '02-009', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 138.0, 'PricePeakSeason': 242.88}, {'RoomId': '02-010', 'Floor': '02', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 288.42, 'PricePeakSeason': 507.62}, {'RoomId': '02-011', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 92.0, 'PricePeakSeason': 161.92}, {'RoomId': '02-012', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 192.28, 'PricePeakSeason': 338.41}, {'RoomId': '02-013', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 92.0, 'PricePeakSeason': 161.92}, {'RoomId': '02-014', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 192.28, 'PricePeakSeason': 338.41}, {'RoomId': '02-015', 'Floor': '02', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 288.42, 'PricePeakSeason': 507.62}, {'RoomId': '02-016', 'Floor': '02', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 83.6, 'PricePeakSeason': 147.14}, {'RoomId': '02-017', 'Floor': '02', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 83.6, 'PricePeakSeason': 147.14}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>6513</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Sovereign Suites</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>{'Country': 'France', 'City': 'Nice', 'ZipCode': '96069', 'Address': '76483 Cameron Trail'}</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>{'OccupancyPeakSeasonWeight': 86, 'OccupancyOffSeasonWeight': 23, 'OccupancyBaseDiscountPercentage': 30, 'ExtraBedChargePercentage': 25, 'MealPlanWeights': {'room_only': {'name': 'Room Only', 'weight': 0.14}, 'room_and_breakfast': {'name': 'Room and Breakfast', 'weight': 0.53}, 'all_inclusive': {'name': 'All Inclusive', 'weight': 0.04}, 'half_board': {'name': 'Half Board', 'weight': 0.16}, 'full_board': {'name': 'Full Board', 'weight': 0.13}}, 'MealPlanPrices': {'Room Only': 1.0, 'Room and Breakfast': 1.17, 'All Inclusive': 2.02, 'Half Board': 1.36, 'Full Board': 1.7}, 'PromotionPriceDiscount': 30}</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>[{'RoomId': '01-001', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 89.0, 'PricePeakSeason': 169.1}, {'RoomId': '01-002', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 42.0, 'PricePeakSeason': 79.8}, {'RoomId': '01-003', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 160.2, 'PricePeakSeason': 304.38}, {'RoomId': '01-004', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 42.0, 'PricePeakSeason': 79.8}, {'RoomId': '01-005', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 89.0, 'PricePeakSeason': 169.1}, {'RoomId': '01-006', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 89.0, 'PricePeakSeason': 169.1}, {'RoomId': '01-007', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 89.0, 'PricePeakSeason': 169.1}, {'RoomId': '01-008', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 89.0, 'PricePeakSeason': 169.1}, {'RoomId': '01-009', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 89.0, 'PricePeakSeason': 169.1}, {'RoomId': '01-010', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 42.0, 'PricePeakSeason': 79.8}, {'RoomId': '01-011', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 89.0, 'PricePeakSeason': 169.1}, {'RoomId': '01-012', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 89.0, 'PricePeakSeason': 169.1}, {'RoomId': '01-013', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 89.0, 'PricePeakSeason': 169.1}, {'RoomId': '01-014', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 89.0, 'PricePeakSeason': 169.1}, {'RoomId': '01-015', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 133.5, 'PricePeakSeason': 253.65}, {'RoomId': '01-016', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 89.0, 'PricePeakSeason': 169.1}, {'RoomId': '01-017', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 42.0, 'PricePeakSeason': 79.8}, {'RoomId': '01-018', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 240.3, 'PricePeakSeason': 456.57}, {'RoomId': '01-019', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 133.5, 'PricePeakSeason': 253.65}, {'RoomId': '01-020', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 89.0, 'PricePeakSeason': 169.1}, {'RoomId': '01-021', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 133.5, 'PricePeakSeason': 253.65}, {'RoomId': '01-022', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 75.6, 'PricePeakSeason': 143.64}, {'RoomId': '01-023', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 89.0, 'PricePeakSeason': 169.1}, {'RoomId': '01-024', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 89.0, 'PricePeakSeason': 169.1}, {'RoomId': '01-025', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 133.5, 'PricePeakSeason': 253.65}, {'RoomId': '01-026', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 42.0, 'PricePeakSeason': 79.8}, {'RoomId': '01-027', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 160.2, 'PricePeakSeason': 304.38}, {'RoomId': '01-028', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 240.3, 'PricePeakSeason': 456.57}, {'RoomId': '01-029', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 240.3, 'PricePeakSeason': 456.57}, {'RoomId': '01-030', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 160.2, 'PricePeakSeason': 304.38}, {'RoomId': '01-031', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 89.0, 'PricePeakSeason': 169.1}, {'RoomId': '01-032', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 42.0, 'PricePeakSeason': 79.8}, {'RoomId': '01-033', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 89.0, 'PricePeakSeason': 169.1}, {'RoomId': '01-034', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 160.2, 'PricePeakSeason': 304.38}, {'RoomId': '01-035', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 42.0, 'PricePeakSeason': 79.8}, {'RoomId': '01-036', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 42.0, 'PricePeakSeason': 79.8}, {'RoomId': '01-037', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 75.6, 'PricePeakSeason': 143.64}, {'RoomId': '02-001', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 42.0, 'PricePeakSeason': 79.8}, {'RoomId': '02-002', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 160.2, 'PricePeakSeason': 304.38}, {'RoomId': '02-003', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 42.0, 'PricePeakSeason': 79.8}, {'RoomId': '02-004', 'Floor': '02', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 240.3, 'PricePeakSeason': 456.57}, {'RoomId': '02-005', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 89.0, 'PricePeakSeason': 169.1}, {'RoomId': '02-006', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 42.0, 'PricePeakSeason': 79.8}, {'RoomId': '02-007', 'Floor': '02', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 240.3, 'PricePeakSeason': 456.57}, {'RoomId': '02-008', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 160.2, 'PricePeakSeason': 304.38}, {'RoomId': '02-009', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 160.2, 'PricePeakSeason': 304.38}, {'RoomId': '02-010', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 42.0, 'PricePeakSeason': 79.8}, {'RoomId': '02-011', 'Floor': '02', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 75.6, 'PricePeakSeason': 143.64}, {'RoomId': '02-012', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 89.0, 'PricePeakSeason': 169.1}, {'RoomId': '02-013', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 133.5, 'PricePeakSeason': 253.65}, {'RoomId': '02-014', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 42.0, 'PricePeakSeason': 79.8}, {'RoomId': '02-015', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 89.0, 'PricePeakSeason': 169.1}, {'RoomId': '02-016', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 89.0, 'PricePeakSeason': 169.1}, {'RoomId': '02-017', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 160.2, 'PricePeakSeason': 304.38}, {'RoomId': '02-018', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 89.0, 'PricePeakSeason': 169.1}, {'RoomId': '02-019', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 89.0, 'PricePeakSeason': 169.1}, {'RoomId': '02-020', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 89.0, 'PricePeakSeason': 169.1}, {'RoomId': '02-021', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 160.2, 'PricePeakSeason': 304.38}, {'RoomId': '02-022', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 89.0, 'PricePeakSeason': 169.1}, {'RoomId': '02-023', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 89.0, 'PricePeakSeason': 169.1}, {'RoomId': '02-024', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 89.0, 'PricePeakSeason': 169.1}, {'RoomId': '02-025', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 42.0, 'PricePeakSeason': 79.8}, {'RoomId': '02-026', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 133.5, 'PricePeakSeason': 253.65}, {'RoomId': '02-027', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 89.0, 'PricePeakSeason': 169.1}, {'RoomId': '02-028', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 89.0, 'PricePeakSeason': 169.1}, {'RoomId': '02-029', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 133.5, 'PricePeakSeason': 253.65}, {'RoomId': '02-030', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 89.0, 'PricePeakSeason': 169.1}, {'RoomId': '02-031', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 89.0, 'PricePeakSeason': 169.1}, {'RoomId': '02-032', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 160.2, 'PricePeakSeason': 304.38}, {'RoomId': '02-033', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 160.2, 'PricePeakSeason': 304.38}, {'RoomId': '02-034', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 160.2, 'PricePeakSeason': 304.38}, {'RoomId': '02-035', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 42.0, 'PricePeakSeason': 79.8}, {'RoomId': '02-036', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 89.0, 'PricePeakSeason': 169.1}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>9784</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Noble Abode</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>{'Country': 'France', 'City': 'Paris', 'ZipCode': '07832', 'Address': '56413 Lewis Parks'}</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>{'OccupancyPeakSeasonWeight': 98, 'OccupancyOffSeasonWeight': 21, 'OccupancyBaseDiscountPercentage': 26, 'ExtraBedChargePercentage': 20, 'MealPlanWeights': {'room_only': {'name': 'Room Only', 'weight': 0.17}, 'room_and_breakfast': {'name': 'Room and Breakfast', 'weight': 0.37}, 'all_inclusive': {'name': 'All Inclusive', 'weight': 0.03}, 'half_board': {'name': 'Half Board', 'weight': 0.22}, 'full_board': {'name': 'Full Board', 'weight': 0.21}}, 'MealPlanPrices': {'Room Only': 1.0, 'Room and Breakfast': 1.14, 'All Inclusive': 2.03, 'Half Board': 1.42, 'Full Board': 1.5}, 'PromotionPriceDiscount': 20}</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>[{'RoomId': '01-001', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 233.59, 'PricePeakSeason': 399.44}, {'RoomId': '01-002', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 87.0, 'PricePeakSeason': 148.77}, {'RoomId': '01-003', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 233.59, 'PricePeakSeason': 399.44}, {'RoomId': '01-004', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 130.5, 'PricePeakSeason': 223.16}, {'RoomId': '01-005', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 130.5, 'PricePeakSeason': 223.16}, {'RoomId': '01-006', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 87.0, 'PricePeakSeason': 148.77}, {'RoomId': '01-007', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 155.73, 'PricePeakSeason': 266.3}, {'RoomId': '01-008', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 87.0, 'PricePeakSeason': 148.77}, {'RoomId': '01-009', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 87.0, 'PricePeakSeason': 148.77}, {'RoomId': '01-010', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 53.0, 'PricePeakSeason': 90.63}, {'RoomId': '01-011', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 87.0, 'PricePeakSeason': 148.77}, {'RoomId': '01-012', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 87.0, 'PricePeakSeason': 148.77}, {'RoomId': '01-013', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 87.0, 'PricePeakSeason': 148.77}, {'RoomId': '01-014', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 130.5, 'PricePeakSeason': 223.16}, {'RoomId': '01-015', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 87.0, 'PricePeakSeason': 148.77}, {'RoomId': '01-016', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 53.0, 'PricePeakSeason': 90.63}, {'RoomId': '01-017', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 233.59, 'PricePeakSeason': 399.44}, {'RoomId': '01-018', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 53.0, 'PricePeakSeason': 90.63}, {'RoomId': '01-019', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 87.0, 'PricePeakSeason': 148.77}, {'RoomId': '01-020', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 155.73, 'PricePeakSeason': 266.3}, {'RoomId': '01-021', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 53.0, 'PricePeakSeason': 90.63}, {'RoomId': '01-022', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 87.0, 'PricePeakSeason': 148.77}, {'RoomId': '01-023', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 87.0, 'PricePeakSeason': 148.77}, {'RoomId': '01-024', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 87.0, 'PricePeakSeason': 148.77}, {'RoomId': '01-025', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 87.0, 'PricePeakSeason': 148.77}, {'RoomId': '01-026', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 94.87, 'PricePeakSeason': 162.23}, {'RoomId': '01-027', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 130.5, 'PricePeakSeason': 223.16}, {'RoomId': '01-028', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 130.5, 'PricePeakSeason': 223.16}, {'RoomId': '01-029', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 130.5, 'PricePeakSeason': 223.16}, {'RoomId': '01-030', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 130.5, 'PricePeakSeason': 223.16}, {'RoomId': '01-031', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 87.0, 'PricePeakSeason': 148.77}, {'RoomId': '01-032', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 87.0, 'PricePeakSeason': 148.77}, {'RoomId': '01-033', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 130.5, 'PricePeakSeason': 223.16}, {'RoomId': '01-034', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 87.0, 'PricePeakSeason': 148.77}, {'RoomId': '01-035', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 53.0, 'PricePeakSeason': 90.63}, {'RoomId': '01-036', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 87.0, 'PricePeakSeason': 148.77}, {'RoomId': '01-037', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 53.0, 'PricePeakSeason': 90.63}, {'RoomId': '01-038', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 130.5, 'PricePeakSeason': 223.16}, {'RoomId': '01-039', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 87.0, 'PricePeakSeason': 148.77}, {'RoomId': '01-040', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 130.5, 'PricePeakSeason': 223.16}, {'RoomId': '01-041', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 155.73, 'PricePeakSeason': 266.3}, {'RoomId': '01-042', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 94.87, 'PricePeakSeason': 162.23}, {'RoomId': '01-043', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 87.0, 'PricePeakSeason': 148.77}, {'RoomId': '01-044', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 87.0, 'PricePeakSeason': 148.77}, {'RoomId': '01-045', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 87.0, 'PricePeakSeason': 148.77}, {'RoomId': '01-046', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 155.73, 'PricePeakSeason': 266.3}, {'RoomId': '01-047', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 53.0, 'PricePeakSeason': 90.63}, {'RoomId': '01-048', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 53.0, 'PricePeakSeason': 90.63}, {'RoomId': '01-049', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 87.0, 'PricePeakSeason': 148.77}, {'RoomId': '01-050', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 155.73, 'PricePeakSeason': 266.3}, {'RoomId': '01-051', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 87.0, 'PricePeakSeason': 148.77}, {'RoomId': '01-052', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 87.0, 'PricePeakSeason': 148.77}, {'RoomId': '01-053', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 53.0, 'PricePeakSeason': 90.63}, {'RoomId': '01-054', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 130.5, 'PricePeakSeason': 223.16}, {'RoomId': '01-055', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 155.73, 'PricePeakSeason': 266.3}, {'RoomId': '01-056', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 53.0, 'PricePeakSeason': 90.63}, {'RoomId': '01-057', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 53.0, 'PricePeakSeason': 90.63}, {'RoomId': '01-058', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 233.59, 'PricePeakSeason': 399.44}, {'RoomId': '01-059', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 87.0, 'PricePeakSeason': 148.77}, {'RoomId': '01-060', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 87.0, 'PricePeakSeason': 148.77}, {'RoomId': '01-061', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 87.0, 'PricePeakSeason': 148.77}, {'RoomId': '01-062', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 130.5, 'PricePeakSeason': 223.16}, {'RoomId': '01-063', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 130.5, 'PricePeakSeason': 223.16}, {'RoomId': '01-064', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 130.5, 'PricePeakSeason': 223.16}, {'RoomId': '01-065', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 53.0, 'PricePeakSeason': 90.63}, {'RoomId': '01-066', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 87.0, 'PricePeakSeason': 148.77}, {'RoomId': '01-067', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 87.0, 'PricePeakSeason': 148.77}, {'RoomId': '01-068', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 87.0, 'PricePeakSeason': 148.77}, {'RoomId': '01-069', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 53.0, 'PricePeakSeason': 90.63}, {'RoomId': '01-070', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 87.0, 'PricePeakSeason': 148.77}, {'RoomId': '01-071', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 87.0, 'PricePeakSeason': 148.77}, {'RoomId': '01-072', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 130.5, 'PricePeakSeason': 223.16}, {'RoomId': '01-073', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 53.0, 'PricePeakSeason': 90.63}, {'RoomId': '01-074', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 233.59, 'PricePeakSeason': 399.44}, {'RoomId': '01-075', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 155.73, 'PricePeakSeason': 266.3}, {'RoomId': '01-076', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 87.0, 'PricePeakSeason': 148.77}, {'RoomId': '01-077', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 53.0, 'PricePeakSeason': 90.63}, {'RoomId': '01-078', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 53.0, 'PricePeakSeason': 90.63}, {'RoomId': '01-079', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 87.0, 'PricePeakSeason': 148.77}, {'RoomId': '01-080', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 87.0, 'PricePeakSeason': 148.77}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2816</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Heritage House</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>{'Country': 'France', 'City': 'Cannes', 'ZipCode': '52357', 'Address': '42388 Burgess Meadow Suite 532'}</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>{'OccupancyPeakSeasonWeight': 81, 'OccupancyOffSeasonWeight': 27, 'OccupancyBaseDiscountPercentage': 22, 'ExtraBedChargePercentage': 22, 'MealPlanWeights': {'room_only': {'name': 'Room Only', 'weight': 0.09}, 'room_and_breakfast': {'name': 'Room and Breakfast', 'weight': 0.46}, 'all_inclusive': {'name': 'All Inclusive', 'weight': 0.01}, 'half_board': {'name': 'Half Board', 'weight': 0.21}, 'full_board': {'name': 'Full Board', 'weight': 0.23}}, 'MealPlanPrices': {'Room Only': 1.0, 'Room and Breakfast': 1.2, 'All Inclusive': 2.1, 'Half Board': 1.49, 'Full Board': 1.54}, 'PromotionPriceDiscount': 29}</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>[{'RoomId': '01-001', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 59.0, 'PricePeakSeason': 100.89}, {'RoomId': '01-002', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.0, 'PricePeakSeason': 165.87}, {'RoomId': '01-003', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.0, 'PricePeakSeason': 165.87}, {'RoomId': '01-004', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 145.5, 'PricePeakSeason': 248.81}, {'RoomId': '01-005', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 59.0, 'PricePeakSeason': 100.89}, {'RoomId': '01-006', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.0, 'PricePeakSeason': 165.87}, {'RoomId': '01-007', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 59.0, 'PricePeakSeason': 100.89}, {'RoomId': '01-008', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 59.0, 'PricePeakSeason': 100.89}, {'RoomId': '01-009', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 172.66, 'PricePeakSeason': 295.25}, {'RoomId': '01-010', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.0, 'PricePeakSeason': 165.87}, {'RoomId': '01-011', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.0, 'PricePeakSeason': 165.87}, {'RoomId': '01-012', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 172.66, 'PricePeakSeason': 295.25}, {'RoomId': '01-013', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 172.66, 'PricePeakSeason': 295.25}, {'RoomId': '01-014', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 172.66, 'PricePeakSeason': 295.25}, {'RoomId': '01-015', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.0, 'PricePeakSeason': 165.87}, {'RoomId': '01-016', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.0, 'PricePeakSeason': 165.87}, {'RoomId': '01-017', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.0, 'PricePeakSeason': 165.87}, {'RoomId': '01-018', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.0, 'PricePeakSeason': 165.87}, {'RoomId': '01-019', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.0, 'PricePeakSeason': 165.87}, {'RoomId': '01-020', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.0, 'PricePeakSeason': 165.87}, {'RoomId': '01-021', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 105.02, 'PricePeakSeason': 179.58}, {'RoomId': '01-022', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.0, 'PricePeakSeason': 165.87}, {'RoomId': '01-023', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 145.5, 'PricePeakSeason': 248.81}, {'RoomId': '01-024', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 59.0, 'PricePeakSeason': 100.89}, {'RoomId': '01-025', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 172.66, 'PricePeakSeason': 295.25}, {'RoomId': '01-026', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.0, 'PricePeakSeason': 165.87}, {'RoomId': '01-027', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 145.5, 'PricePeakSeason': 248.81}, {'RoomId': '01-028', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 145.5, 'PricePeakSeason': 248.81}, {'RoomId': '01-029', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 258.99, 'PricePeakSeason': 442.87}, {'RoomId': '01-030', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.0, 'PricePeakSeason': 165.87}, {'RoomId': '01-031', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.0, 'PricePeakSeason': 165.87}, {'RoomId': '01-032', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 172.66, 'PricePeakSeason': 295.25}, {'RoomId': '01-033', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.0, 'PricePeakSeason': 165.87}, {'RoomId': '01-034', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 172.66, 'PricePeakSeason': 295.25}, {'RoomId': '01-035', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.0, 'PricePeakSeason': 165.87}, {'RoomId': '01-036', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.0, 'PricePeakSeason': 165.87}, {'RoomId': '01-037', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.0, 'PricePeakSeason': 165.87}, {'RoomId': '01-038', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.0, 'PricePeakSeason': 165.87}, {'RoomId': '01-039', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 145.5, 'PricePeakSeason': 248.81}, {'RoomId': '01-040', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 172.66, 'PricePeakSeason': 295.25}, {'RoomId': '01-041', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 59.0, 'PricePeakSeason': 100.89}, {'RoomId': '01-042', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 145.5, 'PricePeakSeason': 248.81}, {'RoomId': '01-043', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.0, 'PricePeakSeason': 165.87}, {'RoomId': '01-044', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 59.0, 'PricePeakSeason': 100.89}, {'RoomId': '01-045', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 59.0, 'PricePeakSeason': 100.89}, {'RoomId': '01-046', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.0, 'PricePeakSeason': 165.87}, {'RoomId': '01-047', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 59.0, 'PricePeakSeason': 100.89}, {'RoomId': '01-048', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 145.5, 'PricePeakSeason': 248.81}, {'RoomId': '01-049', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 258.99, 'PricePeakSeason': 442.87}, {'RoomId': '01-050', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.0, 'PricePeakSeason': 165.87}, {'RoomId': '01-051', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 59.0, 'PricePeakSeason': 100.89}, {'RoomId': '01-052', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 145.5, 'PricePeakSeason': 248.81}, {'RoomId': '01-053', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.0, 'PricePeakSeason': 165.87}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>6173</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Legacy Lodge</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>{'Country': 'France', 'City': 'Paris', 'ZipCode': '67285', 'Address': '01226 Paul Ranch Suite 848'}</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>{'OccupancyPeakSeasonWeight': 86, 'OccupancyOffSeasonWeight': 22, 'OccupancyBaseDiscountPercentage': 28, 'ExtraBedChargePercentage': 28, 'MealPlanWeights': {'room_only': {'name': 'Room Only', 'weight': 0.13}, 'room_and_breakfast': {'name': 'Room and Breakfast', 'weight': 0.51}, 'all_inclusive': {'name': 'All Inclusive', 'weight': 0.05}, 'half_board': {'name': 'Half Board', 'weight': 0.15}, 'full_board': {'name': 'Full Board', 'weight': 0.16}}, 'MealPlanPrices': {'Room Only': 1.0, 'Room and Breakfast': 1.15, 'All Inclusive': 2.08, 'Half Board': 1.3, 'Full Board': 1.61}, 'PromotionPriceDiscount': 12}</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>[{'RoomId': '01-001', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.5, 'PricePeakSeason': 168.21}, {'RoomId': '01-002', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 113.4, 'PricePeakSeason': 201.85}, {'RoomId': '01-003', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 146.0, 'PricePeakSeason': 259.88}, {'RoomId': '01-004', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 262.8, 'PricePeakSeason': 467.78}, {'RoomId': '01-005', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.5, 'PricePeakSeason': 168.21}, {'RoomId': '01-006', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.5, 'PricePeakSeason': 168.21}, {'RoomId': '01-007', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.5, 'PricePeakSeason': 168.21}, {'RoomId': '01-008', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.5, 'PricePeakSeason': 168.21}, {'RoomId': '01-009', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 63.0, 'PricePeakSeason': 112.14}, {'RoomId': '01-010', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 146.0, 'PricePeakSeason': 259.88}, {'RoomId': '01-011', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.5, 'PricePeakSeason': 168.21}, {'RoomId': '01-012', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 146.0, 'PricePeakSeason': 259.88}, {'RoomId': '01-013', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.5, 'PricePeakSeason': 168.21}, {'RoomId': '01-014', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 63.0, 'PricePeakSeason': 112.14}, {'RoomId': '02-001', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.5, 'PricePeakSeason': 168.21}, {'RoomId': '02-002', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 146.0, 'PricePeakSeason': 259.88}, {'RoomId': '02-003', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 146.0, 'PricePeakSeason': 259.88}, {'RoomId': '02-004', 'Floor': '02', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 262.8, 'PricePeakSeason': 467.78}, {'RoomId': '02-005', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 170.1, 'PricePeakSeason': 302.78}, {'RoomId': '02-006', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.5, 'PricePeakSeason': 168.21}, {'RoomId': '02-007', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 63.0, 'PricePeakSeason': 112.14}, {'RoomId': '02-008', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.5, 'PricePeakSeason': 168.21}, {'RoomId': '02-009', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.5, 'PricePeakSeason': 168.21}, {'RoomId': '02-010', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 63.0, 'PricePeakSeason': 112.14}, {'RoomId': '02-011', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 146.0, 'PricePeakSeason': 259.88}, {'RoomId': '02-012', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 146.0, 'PricePeakSeason': 259.88}, {'RoomId': '02-013', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.5, 'PricePeakSeason': 168.21}, {'RoomId': '02-014', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 146.0, 'PricePeakSeason': 259.88}, {'RoomId': '03-001', 'Floor': '03', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 63.0, 'PricePeakSeason': 112.14}, {'RoomId': '03-002', 'Floor': '03', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 146.0, 'PricePeakSeason': 259.88}, {'RoomId': '03-003', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.5, 'PricePeakSeason': 168.21}, {'RoomId': '03-004', 'Floor': '03', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 113.4, 'PricePeakSeason': 201.85}, {'RoomId': '03-005', 'Floor': '03', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 63.0, 'PricePeakSeason': 112.14}, {'RoomId': '03-006', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.5, 'PricePeakSeason': 168.21}, {'RoomId': '03-007', 'Floor': '03', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 146.0, 'PricePeakSeason': 259.88}, {'RoomId': '03-008', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.5, 'PricePeakSeason': 168.21}, {'RoomId': '03-009', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.5, 'PricePeakSeason': 168.21}, {'RoomId': '03-010', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.5, 'PricePeakSeason': 168.21}, {'RoomId': '03-011', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.5, 'PricePeakSeason': 168.21}, {'RoomId': '03-012', 'Floor': '03', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 63.0, 'PricePeakSeason': 112.14}, {'RoomId': '03-013', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.5, 'PricePeakSeason': 168.21}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>5650</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Landmark Hotel</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>{'Country': 'France', 'City': 'Cannes', 'ZipCode': '02005', 'Address': '845 Kelly Estate'}</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>{'OccupancyPeakSeasonWeight': 85, 'OccupancyOffSeasonWeight': 27, 'OccupancyBaseDiscountPercentage': 25, 'ExtraBedChargePercentage': 28, 'MealPlanWeights': {'room_only': {'name': 'Room Only', 'weight': 0.16}, 'room_and_breakfast': {'name': 'Room and Breakfast', 'weight': 0.46}, 'all_inclusive': {'name': 'All Inclusive', 'weight': 0.02}, 'half_board': {'name': 'Half Board', 'weight': 0.19}, 'full_board': {'name': 'Full Board', 'weight': 0.17}}, 'MealPlanPrices': {'Room Only': 1.0, 'Room and Breakfast': 1.2, 'All Inclusive': 2.09, 'Half Board': 1.49, 'Full Board': 1.67}, 'PromotionPriceDiscount': 12}</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>[{'RoomId': '01-001', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 91.5, 'PricePeakSeason': 176.6}, {'RoomId': '01-002', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 91.5, 'PricePeakSeason': 176.6}, {'RoomId': '01-003', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 91.5, 'PricePeakSeason': 176.6}, {'RoomId': '01-004', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 91.5, 'PricePeakSeason': 176.6}, {'RoomId': '01-005', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 61.0, 'PricePeakSeason': 117.73}, {'RoomId': '01-006', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 137.25, 'PricePeakSeason': 264.89}, {'RoomId': '01-007', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 137.25, 'PricePeakSeason': 264.89}, {'RoomId': '01-008', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 61.0, 'PricePeakSeason': 117.73}, {'RoomId': '01-009', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 151.89, 'PricePeakSeason': 293.15}, {'RoomId': '01-010', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 91.5, 'PricePeakSeason': 176.6}, {'RoomId': '01-011', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 227.84, 'PricePeakSeason': 439.73}, {'RoomId': '01-012', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 91.5, 'PricePeakSeason': 176.6}, {'RoomId': '01-013', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 227.84, 'PricePeakSeason': 439.73}, {'RoomId': '01-014', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 227.84, 'PricePeakSeason': 439.73}, {'RoomId': '01-015', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 227.84, 'PricePeakSeason': 439.73}, {'RoomId': '01-016', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 137.25, 'PricePeakSeason': 264.89}, {'RoomId': '01-017', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 91.5, 'PricePeakSeason': 176.6}, {'RoomId': '01-018', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 61.0, 'PricePeakSeason': 117.73}, {'RoomId': '01-019', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 91.5, 'PricePeakSeason': 176.6}, {'RoomId': '01-020', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 91.5, 'PricePeakSeason': 176.6}, {'RoomId': '01-021', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 91.5, 'PricePeakSeason': 176.6}, {'RoomId': '01-022', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 91.5, 'PricePeakSeason': 176.6}, {'RoomId': '01-023', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 91.5, 'PricePeakSeason': 176.6}, {'RoomId': '01-024', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 61.0, 'PricePeakSeason': 117.73}, {'RoomId': '02-001', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 227.84, 'PricePeakSeason': 439.73}, {'RoomId': '02-002', 'Floor': '02', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 151.89, 'PricePeakSeason': 293.15}, {'RoomId': '02-003', 'Floor': '02', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 341.75, 'PricePeakSeason': 659.58}, {'RoomId': '02-004', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 91.5, 'PricePeakSeason': 176.6}, {'RoomId': '02-005', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 91.5, 'PricePeakSeason': 176.6}, {'RoomId': '02-006', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 137.25, 'PricePeakSeason': 264.89}, {'RoomId': '02-007', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 91.5, 'PricePeakSeason': 176.6}, {'RoomId': '02-008', 'Floor': '02', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 151.89, 'PricePeakSeason': 293.15}, {'RoomId': '02-009', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 91.5, 'PricePeakSeason': 176.6}, {'RoomId': '02-010', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 91.5, 'PricePeakSeason': 176.6}, {'RoomId': '02-011', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 91.5, 'PricePeakSeason': 176.6}, {'RoomId': '02-012', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 137.25, 'PricePeakSeason': 264.89}, {'RoomId': '02-013', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 91.5, 'PricePeakSeason': 176.6}, {'RoomId': '02-014', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 91.5, 'PricePeakSeason': 176.6}, {'RoomId': '02-015', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 91.5, 'PricePeakSeason': 176.6}, {'RoomId': '02-016', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 61.0, 'PricePeakSeason': 117.73}, {'RoomId': '02-017', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 227.84, 'PricePeakSeason': 439.73}, {'RoomId': '02-018', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 91.5, 'PricePeakSeason': 176.6}, {'RoomId': '02-019', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 61.0, 'PricePeakSeason': 117.73}, {'RoomId': '02-020', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 137.25, 'PricePeakSeason': 264.89}, {'RoomId': '02-021', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 137.25, 'PricePeakSeason': 264.89}, {'RoomId': '02-022', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 61.0, 'PricePeakSeason': 117.73}, {'RoomId': '02-023', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 227.84, 'PricePeakSeason': 439.73}, {'RoomId': '02-024', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 227.84, 'PricePeakSeason': 439.73}, {'RoomId': '03-001', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 91.5, 'PricePeakSeason': 176.6}, {'RoomId': '03-002', 'Floor': '03', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 227.84, 'PricePeakSeason': 439.73}, {'RoomId': '03-003', 'Floor': '03', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 61.0, 'PricePeakSeason': 117.73}, {'RoomId': '03-004', 'Floor': '03', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 137.25, 'PricePeakSeason': 264.89}, {'RoomId': '03-005', 'Floor': '03', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 227.84, 'PricePeakSeason': 439.73}, {'RoomId': '03-006', 'Floor': '03', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 227.84, 'PricePeakSeason': 439.73}, {'RoomId': '03-007', 'Floor': '03', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 227.84, 'PricePeakSeason': 439.73}, {'RoomId': '03-008', 'Floor': '03', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 61.0, 'PricePeakSeason': 117.73}, {'RoomId': '03-009', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 91.5, 'PricePeakSeason': 176.6}, {'RoomId': '03-010', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 91.5, 'PricePeakSeason': 176.6}, {'RoomId': '03-011', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 91.5, 'PricePeakSeason': 176.6}, {'RoomId': '03-012', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 91.5, 'PricePeakSeason': 176.6}, {'RoomId': '03-013', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 91.5, 'PricePeakSeason': 176.6}, {'RoomId': '03-014', 'Floor': '03', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 227.84, 'PricePeakSeason': 439.73}, {'RoomId': '03-015', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 91.5, 'PricePeakSeason': 176.6}, {'RoomId': '03-016', 'Floor': '03', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 151.89, 'PricePeakSeason': 293.15}, {'RoomId': '03-017', 'Floor': '03', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 227.84, 'PricePeakSeason': 439.73}, {'RoomId': '03-018', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 91.5, 'PricePeakSeason': 176.6}, {'RoomId': '03-019', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 91.5, 'PricePeakSeason': 176.6}, {'RoomId': '03-020', 'Floor': '03', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 227.84, 'PricePeakSeason': 439.73}, {'RoomId': '03-021', 'Floor': '03', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 137.25, 'PricePeakSeason': 264.89}, {'RoomId': '03-022', 'Floor': '03', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 137.25, 'PricePeakSeason': 264.89}, {'RoomId': '03-023', 'Floor': '03', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 61.0, 'PricePeakSeason': 117.73}, {'RoomId': '03-024', 'Floor': '03', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 61.0, 'PricePeakSeason': 117.73}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>8235</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Apex Tower</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>{'Country': 'France', 'City': 'Cannes', 'ZipCode': '59971', 'Address': '482 Monica Hills'}</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>{'OccupancyPeakSeasonWeight': 94, 'OccupancyOffSeasonWeight': 35, 'OccupancyBaseDiscountPercentage': 20, 'ExtraBedChargePercentage': 22, 'MealPlanWeights': {'room_only': {'name': 'Room Only', 'weight': 0.14}, 'room_and_breakfast': {'name': 'Room and Breakfast', 'weight': 0.43}, 'all_inclusive': {'name': 'All Inclusive', 'weight': 0.09}, 'half_board': {'name': 'Half Board', 'weight': 0.18}, 'full_board': {'name': 'Full Board', 'weight': 0.16}}, 'MealPlanPrices': {'Room Only': 1.0, 'Room and Breakfast': 1.17, 'All Inclusive': 2.17, 'Half Board': 1.4, 'Full Board': 1.67}, 'PromotionPriceDiscount': 21}</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>[{'RoomId': '01-001', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 182.4, 'PricePeakSeason': 277.25}, {'RoomId': '01-002', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 76.0, 'PricePeakSeason': 115.52}, {'RoomId': '01-003', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 173.28}, {'RoomId': '01-004', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 171.0, 'PricePeakSeason': 259.92}, {'RoomId': '01-005', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 173.28}, {'RoomId': '01-006', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 173.28}, {'RoomId': '01-007', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 182.4, 'PricePeakSeason': 277.25}, {'RoomId': '01-008', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 173.28}, {'RoomId': '01-009', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 173.28}, {'RoomId': '01-010', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 173.28}, {'RoomId': '01-011', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 171.0, 'PricePeakSeason': 259.92}, {'RoomId': '01-012', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 171.0, 'PricePeakSeason': 259.92}, {'RoomId': '01-013', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 173.28}, {'RoomId': '01-014', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 182.4, 'PricePeakSeason': 277.25}, {'RoomId': '01-015', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 173.28}, {'RoomId': '01-016', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 173.28}, {'RoomId': '01-017', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 76.0, 'PricePeakSeason': 115.52}, {'RoomId': '01-018', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 273.6, 'PricePeakSeason': 415.87}, {'RoomId': '01-019', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 171.0, 'PricePeakSeason': 259.92}, {'RoomId': '01-020', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 182.4, 'PricePeakSeason': 277.25}, {'RoomId': '01-021', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 182.4, 'PricePeakSeason': 277.25}, {'RoomId': '01-022', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 76.0, 'PricePeakSeason': 115.52}, {'RoomId': '01-023', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 182.4, 'PricePeakSeason': 277.25}, {'RoomId': '02-001', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 182.4, 'PricePeakSeason': 277.25}, {'RoomId': '02-002', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 173.28}, {'RoomId': '02-003', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 173.28}, {'RoomId': '02-004', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 76.0, 'PricePeakSeason': 115.52}, {'RoomId': '02-005', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 173.28}, {'RoomId': '02-006', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 182.4, 'PricePeakSeason': 277.25}, {'RoomId': '02-007', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 76.0, 'PricePeakSeason': 115.52}, {'RoomId': '02-008', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 76.0, 'PricePeakSeason': 115.52}, {'RoomId': '02-009', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 173.28}, {'RoomId': '02-010', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 76.0, 'PricePeakSeason': 115.52}, {'RoomId': '02-011', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 173.28}, {'RoomId': '02-012', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 173.28}, {'RoomId': '02-013', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 173.28}, {'RoomId': '02-014', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 173.28}, {'RoomId': '02-015', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 182.4, 'PricePeakSeason': 277.25}, {'RoomId': '02-016', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 76.0, 'PricePeakSeason': 115.52}, {'RoomId': '02-017', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 171.0, 'PricePeakSeason': 259.92}, {'RoomId': '02-018', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 173.28}, {'RoomId': '02-019', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 173.28}, {'RoomId': '02-020', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 76.0, 'PricePeakSeason': 115.52}, {'RoomId': '02-021', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 173.28}, {'RoomId': '02-022', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 182.4, 'PricePeakSeason': 277.25}, {'RoomId': '03-001', 'Floor': '03', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 171.0, 'PricePeakSeason': 259.92}, {'RoomId': '03-002', 'Floor': '03', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 171.0, 'PricePeakSeason': 259.92}, {'RoomId': '03-003', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 173.28}, {'RoomId': '03-004', 'Floor': '03', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 182.4, 'PricePeakSeason': 277.25}, {'RoomId': '03-005', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 173.28}, {'RoomId': '03-006', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 173.28}, {'RoomId': '03-007', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 173.28}, {'RoomId': '03-008', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 173.28}, {'RoomId': '03-009', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 173.28}, {'RoomId': '03-010', 'Floor': '03', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 171.0, 'PricePeakSeason': 259.92}, {'RoomId': '03-011', 'Floor': '03', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 182.4, 'PricePeakSeason': 277.25}, {'RoomId': '03-012', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 173.28}, {'RoomId': '03-013', 'Floor': '03', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 273.6, 'PricePeakSeason': 415.87}, {'RoomId': '03-014', 'Floor': '03', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 76.0, 'PricePeakSeason': 115.52}, {'RoomId': '03-015', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 173.28}, {'RoomId': '03-016', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 173.28}, {'RoomId': '03-017', 'Floor': '03', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 182.4, 'PricePeakSeason': 277.25}, {'RoomId': '03-018', 'Floor': '03', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 182.4, 'PricePeakSeason': 277.25}, {'RoomId': '03-019', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 173.28}, {'RoomId': '03-020', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 173.28}, {'RoomId': '03-021', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 173.28}, {'RoomId': '03-022', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 173.28}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>4332</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Zenith Point</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>{'Country': 'France', 'City': 'Paris', 'ZipCode': '84249', 'Address': '52880 Burns Creek'}</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>{'OccupancyPeakSeasonWeight': 87, 'OccupancyOffSeasonWeight': 23, 'OccupancyBaseDiscountPercentage': 22, 'ExtraBedChargePercentage': 22, 'MealPlanWeights': {'room_only': {'name': 'Room Only', 'weight': 0.14}, 'room_and_breakfast': {'name': 'Room and Breakfast', 'weight': 0.53}, 'all_inclusive': {'name': 'All Inclusive', 'weight': 0.0}, 'half_board': {'name': 'Half Board', 'weight': 0.16}, 'full_board': {'name': 'Full Board', 'weight': 0.17}}, 'MealPlanPrices': {'Room Only': 1.0, 'Room and Breakfast': 1.15, 'All Inclusive': 2.09, 'Half Board': 1.48, 'Full Board': 1.68}, 'PromotionPriceDiscount': 10}</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>[{'RoomId': '01-001', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.0, 'PricePeakSeason': 159.8}, {'RoomId': '01-002', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 199.28, 'PricePeakSeason': 338.78}, {'RoomId': '01-003', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.0, 'PricePeakSeason': 159.8}, {'RoomId': '01-004', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 145.0, 'PricePeakSeason': 246.5}, {'RoomId': '01-005', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.0, 'PricePeakSeason': 159.8}, {'RoomId': '01-006', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 53.0, 'PricePeakSeason': 90.1}, {'RoomId': '01-007', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 145.0, 'PricePeakSeason': 246.5}, {'RoomId': '01-008', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 145.0, 'PricePeakSeason': 246.5}, {'RoomId': '01-009', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.0, 'PricePeakSeason': 159.8}, {'RoomId': '01-010', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.0, 'PricePeakSeason': 159.8}, {'RoomId': '01-011', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.0, 'PricePeakSeason': 159.8}, {'RoomId': '01-012', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 53.0, 'PricePeakSeason': 90.1}, {'RoomId': '01-013', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.0, 'PricePeakSeason': 159.8}, {'RoomId': '01-014', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 145.0, 'PricePeakSeason': 246.5}, {'RoomId': '01-015', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.0, 'PricePeakSeason': 159.8}, {'RoomId': '01-016', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.0, 'PricePeakSeason': 159.8}, {'RoomId': '01-017', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.0, 'PricePeakSeason': 159.8}, {'RoomId': '01-018', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 145.0, 'PricePeakSeason': 246.5}, {'RoomId': '01-019', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 112.36, 'PricePeakSeason': 191.01}, {'RoomId': '01-020', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 145.0, 'PricePeakSeason': 246.5}, {'RoomId': '01-021', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.0, 'PricePeakSeason': 159.8}, {'RoomId': '01-022', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.0, 'PricePeakSeason': 159.8}, {'RoomId': '01-023', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 53.0, 'PricePeakSeason': 90.1}, {'RoomId': '02-001', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.0, 'PricePeakSeason': 159.8}, {'RoomId': '02-002', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.0, 'PricePeakSeason': 159.8}, {'RoomId': '02-003', 'Floor': '02', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 112.36, 'PricePeakSeason': 191.01}, {'RoomId': '02-004', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 199.28, 'PricePeakSeason': 338.78}, {'RoomId': '02-005', 'Floor': '02', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 307.4, 'PricePeakSeason': 522.58}, {'RoomId': '02-006', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.0, 'PricePeakSeason': 159.8}, {'RoomId': '02-007', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 53.0, 'PricePeakSeason': 90.1}, {'RoomId': '02-008', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 145.0, 'PricePeakSeason': 246.5}, {'RoomId': '02-009', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 53.0, 'PricePeakSeason': 90.1}, {'RoomId': '02-010', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.0, 'PricePeakSeason': 159.8}, {'RoomId': '02-011', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 199.28, 'PricePeakSeason': 338.78}, {'RoomId': '02-012', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.0, 'PricePeakSeason': 159.8}, {'RoomId': '02-013', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 145.0, 'PricePeakSeason': 246.5}, {'RoomId': '02-014', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.0, 'PricePeakSeason': 159.8}, {'RoomId': '02-015', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.0, 'PricePeakSeason': 159.8}, {'RoomId': '02-016', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.0, 'PricePeakSeason': 159.8}, {'RoomId': '02-017', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.0, 'PricePeakSeason': 159.8}, {'RoomId': '02-018', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.0, 'PricePeakSeason': 159.8}, {'RoomId': '02-019', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.0, 'PricePeakSeason': 159.8}, {'RoomId': '02-020', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.0, 'PricePeakSeason': 159.8}, {'RoomId': '02-021', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.0, 'PricePeakSeason': 159.8}, {'RoomId': '02-022', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.0, 'PricePeakSeason': 159.8}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>4286</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Meridian Suites</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>{'Country': 'France', 'City': 'Cannes', 'ZipCode': '48077', 'Address': '03911 Cabrera Trace Apt. 278'}</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>{'OccupancyPeakSeasonWeight': 75, 'OccupancyOffSeasonWeight': 27, 'OccupancyBaseDiscountPercentage': 23, 'ExtraBedChargePercentage': 21, 'MealPlanWeights': {'room_only': {'name': 'Room Only', 'weight': 0.13}, 'room_and_breakfast': {'name': 'Room and Breakfast', 'weight': 0.38}, 'all_inclusive': {'name': 'All Inclusive', 'weight': 0.07}, 'half_board': {'name': 'Half Board', 'weight': 0.29}, 'full_board': {'name': 'Full Board', 'weight': 0.13}}, 'MealPlanPrices': {'Room Only': 1.0, 'Room and Breakfast': 1.16, 'All Inclusive': 2.14, 'Half Board': 1.37, 'Full Board': 1.67}, 'PromotionPriceDiscount': 16}</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>[{'RoomId': '01-001', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 59.0, 'PricePeakSeason': 99.12}, {'RoomId': '01-002', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 217.14, 'PricePeakSeason': 364.8}, {'RoomId': '01-003', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 141.0, 'PricePeakSeason': 236.88}, {'RoomId': '01-004', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.0, 'PricePeakSeason': 157.92}, {'RoomId': '01-005', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 217.14, 'PricePeakSeason': 364.8}, {'RoomId': '01-006', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 325.71, 'PricePeakSeason': 547.19}, {'RoomId': '01-007', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 217.14, 'PricePeakSeason': 364.8}, {'RoomId': '01-008', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 141.0, 'PricePeakSeason': 236.88}, {'RoomId': '01-009', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.0, 'PricePeakSeason': 157.92}, {'RoomId': '01-010', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 141.0, 'PricePeakSeason': 236.88}, {'RoomId': '01-011', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 141.0, 'PricePeakSeason': 236.88}, {'RoomId': '01-012', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 136.29, 'PricePeakSeason': 228.97}, {'RoomId': '01-013', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 59.0, 'PricePeakSeason': 99.12}, {'RoomId': '01-014', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 217.14, 'PricePeakSeason': 364.8}, {'RoomId': '01-015', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 217.14, 'PricePeakSeason': 364.8}, {'RoomId': '01-016', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 141.0, 'PricePeakSeason': 236.88}, {'RoomId': '01-017', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 59.0, 'PricePeakSeason': 99.12}, {'RoomId': '01-018', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.0, 'PricePeakSeason': 157.92}, {'RoomId': '01-019', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.0, 'PricePeakSeason': 157.92}, {'RoomId': '01-020', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 217.14, 'PricePeakSeason': 364.8}, {'RoomId': '01-021', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.0, 'PricePeakSeason': 157.92}, {'RoomId': '01-022', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 59.0, 'PricePeakSeason': 99.12}, {'RoomId': '01-023', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.0, 'PricePeakSeason': 157.92}, {'RoomId': '01-024', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 217.14, 'PricePeakSeason': 364.8}, {'RoomId': '01-025', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 141.0, 'PricePeakSeason': 236.88}, {'RoomId': '01-026', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 217.14, 'PricePeakSeason': 364.8}, {'RoomId': '01-027', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 59.0, 'PricePeakSeason': 99.12}, {'RoomId': '01-028', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.0, 'PricePeakSeason': 157.92}, {'RoomId': '01-029', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 325.71, 'PricePeakSeason': 547.19}, {'RoomId': '01-030', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 141.0, 'PricePeakSeason': 236.88}, {'RoomId': '01-031', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 141.0, 'PricePeakSeason': 236.88}, {'RoomId': '01-032', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 59.0, 'PricePeakSeason': 99.12}, {'RoomId': '01-033', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 325.71, 'PricePeakSeason': 547.19}, {'RoomId': '01-034', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 141.0, 'PricePeakSeason': 236.88}, {'RoomId': '01-035', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 141.0, 'PricePeakSeason': 236.88}, {'RoomId': '01-036', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 59.0, 'PricePeakSeason': 99.12}, {'RoomId': '01-037', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 325.71, 'PricePeakSeason': 547.19}, {'RoomId': '01-038', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 325.71, 'PricePeakSeason': 547.19}, {'RoomId': '01-039', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.0, 'PricePeakSeason': 157.92}, {'RoomId': '01-040', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.0, 'PricePeakSeason': 157.92}, {'RoomId': '01-041', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.0, 'PricePeakSeason': 157.92}, {'RoomId': '01-042', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 59.0, 'PricePeakSeason': 99.12}, {'RoomId': '01-043', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 325.71, 'PricePeakSeason': 547.19}, {'RoomId': '01-044', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.0, 'PricePeakSeason': 157.92}, {'RoomId': '01-045', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 325.71, 'PricePeakSeason': 547.19}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>0925</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Nexus Hotel</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>{'Country': 'France', 'City': 'Cannes', 'ZipCode': '22144', 'Address': '963 Jennifer Locks Suite 787'}</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>{'OccupancyPeakSeasonWeight': 90, 'OccupancyOffSeasonWeight': 25, 'OccupancyBaseDiscountPercentage': 28, 'ExtraBedChargePercentage': 30, 'MealPlanWeights': {'room_only': {'name': 'Room Only', 'weight': 0.18}, 'room_and_breakfast': {'name': 'Room and Breakfast', 'weight': 0.42}, 'all_inclusive': {'name': 'All Inclusive', 'weight': 0.07}, 'half_board': {'name': 'Half Board', 'weight': 0.1}, 'full_board': {'name': 'Full Board', 'weight': 0.23}}, 'MealPlanPrices': {'Room Only': 1.0, 'Room and Breakfast': 1.1, 'All Inclusive': 2.13, 'Half Board': 1.34, 'Full Board': 1.7}, 'PromotionPriceDiscount': 17}</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>[{'RoomId': '01-001', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 150.97}, {'RoomId': '01-002', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 123.75, 'PricePeakSeason': 226.46}, {'RoomId': '01-003', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 289.57, 'PricePeakSeason': 529.91}, {'RoomId': '01-004', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 150.97}, {'RoomId': '01-005', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 123.75, 'PricePeakSeason': 226.46}, {'RoomId': '01-006', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 193.05, 'PricePeakSeason': 353.28}, {'RoomId': '01-007', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 150.97}, {'RoomId': '01-008', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 55.0, 'PricePeakSeason': 100.65}, {'RoomId': '01-009', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 150.97}, {'RoomId': '01-010', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 123.75, 'PricePeakSeason': 226.46}, {'RoomId': '01-011', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 150.97}, {'RoomId': '01-012', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 289.57, 'PricePeakSeason': 529.91}, {'RoomId': '01-013', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 123.75, 'PricePeakSeason': 226.46}, {'RoomId': '01-014', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 55.0, 'PricePeakSeason': 100.65}, {'RoomId': '01-015', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 55.0, 'PricePeakSeason': 100.65}, {'RoomId': '01-016', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 123.75, 'PricePeakSeason': 226.46}, {'RoomId': '02-001', 'Floor': '02', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 128.7, 'PricePeakSeason': 235.52}, {'RoomId': '02-002', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 55.0, 'PricePeakSeason': 100.65}, {'RoomId': '02-003', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 150.97}, {'RoomId': '02-004', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 123.75, 'PricePeakSeason': 226.46}, {'RoomId': '02-005', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 150.97}, {'RoomId': '02-006', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 150.97}, {'RoomId': '02-007', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 123.75, 'PricePeakSeason': 226.46}, {'RoomId': '02-008', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 123.75, 'PricePeakSeason': 226.46}, {'RoomId': '02-009', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 123.75, 'PricePeakSeason': 226.46}, {'RoomId': '02-010', 'Floor': '02', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 128.7, 'PricePeakSeason': 235.52}, {'RoomId': '02-011', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 193.05, 'PricePeakSeason': 353.28}, {'RoomId': '02-012', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 150.97}, {'RoomId': '02-013', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 123.75, 'PricePeakSeason': 226.46}, {'RoomId': '02-014', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 150.97}, {'RoomId': '02-015', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 150.97}, {'RoomId': '02-016', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 150.97}, {'RoomId': '03-001', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 150.97}, {'RoomId': '03-002', 'Floor': '03', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 123.75, 'PricePeakSeason': 226.46}, {'RoomId': '03-003', 'Floor': '03', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 123.75, 'PricePeakSeason': 226.46}, {'RoomId': '03-004', 'Floor': '03', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 193.05, 'PricePeakSeason': 353.28}, {'RoomId': '03-005', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 150.97}, {'RoomId': '03-006', 'Floor': '03', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 55.0, 'PricePeakSeason': 100.65}, {'RoomId': '03-007', 'Floor': '03', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 123.75, 'PricePeakSeason': 226.46}, {'RoomId': '03-008', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 150.97}, {'RoomId': '03-009', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 150.97}, {'RoomId': '03-010', 'Floor': '03', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 123.75, 'PricePeakSeason': 226.46}, {'RoomId': '03-011', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 150.97}, {'RoomId': '03-012', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 150.97}, {'RoomId': '03-013', 'Floor': '03', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 289.57, 'PricePeakSeason': 529.91}, {'RoomId': '03-014', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 150.97}, {'RoomId': '03-015', 'Floor': '03', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 123.75, 'PricePeakSeason': 226.46}, {'RoomId': '03-016', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 150.97}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>1114</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Vertex Residences</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>{'Country': 'France', 'City': 'Paris', 'ZipCode': '16361', 'Address': '15098 Brianna Avenue'}</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>{'OccupancyPeakSeasonWeight': 87, 'OccupancyOffSeasonWeight': 33, 'OccupancyBaseDiscountPercentage': 22, 'ExtraBedChargePercentage': 30, 'MealPlanWeights': {'room_only': {'name': 'Room Only', 'weight': 0.17}, 'room_and_breakfast': {'name': 'Room and Breakfast', 'weight': 0.42}, 'all_inclusive': {'name': 'All Inclusive', 'weight': 0.08}, 'half_board': {'name': 'Half Board', 'weight': 0.17}, 'full_board': {'name': 'Full Board', 'weight': 0.16}}, 'MealPlanPrices': {'Room Only': 1.0, 'Room and Breakfast': 1.11, 'All Inclusive': 2.08, 'Half Board': 1.34, 'Full Board': 1.62}, 'PromotionPriceDiscount': 30}</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>[{'RoomId': '01-001', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 105.0, 'PricePeakSeason': 157.5}, {'RoomId': '01-002', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 105.0, 'PricePeakSeason': 157.5}, {'RoomId': '01-003', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 105.0, 'PricePeakSeason': 157.5}, {'RoomId': '01-004', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 105.0, 'PricePeakSeason': 157.5}, {'RoomId': '01-005', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 157.5, 'PricePeakSeason': 236.25}, {'RoomId': '01-006', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 157.5, 'PricePeakSeason': 236.25}, {'RoomId': '01-007', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 105.0, 'PricePeakSeason': 157.5}, {'RoomId': '01-008', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 159.6, 'PricePeakSeason': 239.4}, {'RoomId': '01-009', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 157.5, 'PricePeakSeason': 236.25}, {'RoomId': '01-010', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 157.5, 'PricePeakSeason': 236.25}, {'RoomId': '01-011', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 105.0, 'PricePeakSeason': 157.5}, {'RoomId': '01-012', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 159.6, 'PricePeakSeason': 239.4}, {'RoomId': '01-013', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 106.4, 'PricePeakSeason': 159.6}, {'RoomId': '01-014', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 159.6, 'PricePeakSeason': 239.4}, {'RoomId': '01-015', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 105.0, 'PricePeakSeason': 157.5}, {'RoomId': '01-016', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 105.0, 'PricePeakSeason': 157.5}, {'RoomId': '01-017', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 159.6, 'PricePeakSeason': 239.4}, {'RoomId': '01-018', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 157.5, 'PricePeakSeason': 236.25}, {'RoomId': '01-019', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 159.6, 'PricePeakSeason': 239.4}, {'RoomId': '01-020', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 239.4, 'PricePeakSeason': 359.1}, {'RoomId': '01-021', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 239.4, 'PricePeakSeason': 359.1}, {'RoomId': '01-022', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 157.5, 'PricePeakSeason': 236.25}, {'RoomId': '02-001', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 159.6, 'PricePeakSeason': 239.4}, {'RoomId': '02-002', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 157.5, 'PricePeakSeason': 236.25}, {'RoomId': '02-003', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 159.6, 'PricePeakSeason': 239.4}, {'RoomId': '02-004', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 105.0, 'PricePeakSeason': 157.5}, {'RoomId': '02-005', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 157.5, 'PricePeakSeason': 236.25}, {'RoomId': '02-006', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 105.0, 'PricePeakSeason': 157.5}, {'RoomId': '02-007', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 157.5, 'PricePeakSeason': 236.25}, {'RoomId': '02-008', 'Floor': '02', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 239.4, 'PricePeakSeason': 359.1}, {'RoomId': '02-009', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 105.0, 'PricePeakSeason': 157.5}, {'RoomId': '02-010', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 157.5, 'PricePeakSeason': 236.25}, {'RoomId': '02-011', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 159.6, 'PricePeakSeason': 239.4}, {'RoomId': '02-012', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 105.0, 'PricePeakSeason': 157.5}, {'RoomId': '02-013', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 159.6, 'PricePeakSeason': 239.4}, {'RoomId': '02-014', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 157.5, 'PricePeakSeason': 236.25}, {'RoomId': '02-015', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 70.0, 'PricePeakSeason': 105.0}, {'RoomId': '02-016', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 70.0, 'PricePeakSeason': 105.0}, {'RoomId': '02-017', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 105.0, 'PricePeakSeason': 157.5}, {'RoomId': '02-018', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 157.5, 'PricePeakSeason': 236.25}, {'RoomId': '02-019', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 105.0, 'PricePeakSeason': 157.5}, {'RoomId': '02-020', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 159.6, 'PricePeakSeason': 239.4}, {'RoomId': '02-021', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 105.0, 'PricePeakSeason': 157.5}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2528</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Luminary Hotel</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>{'Country': 'France', 'City': 'Nice', 'ZipCode': '09806', 'Address': '10518 Joshua Oval'}</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>{'OccupancyPeakSeasonWeight': 92, 'OccupancyOffSeasonWeight': 38, 'OccupancyBaseDiscountPercentage': 29, 'ExtraBedChargePercentage': 23, 'MealPlanWeights': {'room_only': {'name': 'Room Only', 'weight': 0.13}, 'room_and_breakfast': {'name': 'Room and Breakfast', 'weight': 0.39}, 'all_inclusive': {'name': 'All Inclusive', 'weight': 0.08}, 'half_board': {'name': 'Half Board', 'weight': 0.21}, 'full_board': {'name': 'Full Board', 'weight': 0.19}}, 'MealPlanPrices': {'Room Only': 1.0, 'Room and Breakfast': 1.1, 'All Inclusive': 2.15, 'Half Board': 1.33, 'Full Board': 1.59}, 'PromotionPriceDiscount': 23}</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>[{'RoomId': '01-001', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 72.0, 'PricePeakSeason': 128.16}, {'RoomId': '01-002', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 48.0, 'PricePeakSeason': 85.44}, {'RoomId': '01-003', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 72.0, 'PricePeakSeason': 128.16}, {'RoomId': '01-004', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 111.0, 'PricePeakSeason': 197.58}, {'RoomId': '01-005', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 72.0, 'PricePeakSeason': 128.16}, {'RoomId': '01-006', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 72.0, 'PricePeakSeason': 128.16}, {'RoomId': '01-007', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 111.0, 'PricePeakSeason': 197.58}, {'RoomId': '01-008', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 72.0, 'PricePeakSeason': 128.16}, {'RoomId': '01-009', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 48.0, 'PricePeakSeason': 85.44}, {'RoomId': '01-010', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 72.0, 'PricePeakSeason': 128.16}, {'RoomId': '01-011', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 48.0, 'PricePeakSeason': 85.44}, {'RoomId': '01-012', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 72.0, 'PricePeakSeason': 128.16}, {'RoomId': '01-013', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 72.0, 'PricePeakSeason': 128.16}, {'RoomId': '01-014', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 147.6, 'PricePeakSeason': 262.73}, {'RoomId': '01-015', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 72.0, 'PricePeakSeason': 128.16}, {'RoomId': '01-016', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 48.0, 'PricePeakSeason': 85.44}, {'RoomId': '01-017', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 72.0, 'PricePeakSeason': 128.16}, {'RoomId': '01-018', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 72.0, 'PricePeakSeason': 128.16}, {'RoomId': '01-019', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 72.0, 'PricePeakSeason': 128.16}, {'RoomId': '01-020', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 111.0, 'PricePeakSeason': 197.58}, {'RoomId': '01-021', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 72.0, 'PricePeakSeason': 128.16}, {'RoomId': '01-022', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 72.0, 'PricePeakSeason': 128.16}, {'RoomId': '01-023', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 72.0, 'PricePeakSeason': 128.16}, {'RoomId': '01-024', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 72.0, 'PricePeakSeason': 128.16}, {'RoomId': '01-025', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 72.0, 'PricePeakSeason': 128.16}, {'RoomId': '01-026', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 111.0, 'PricePeakSeason': 197.58}, {'RoomId': '01-027', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 72.0, 'PricePeakSeason': 128.16}, {'RoomId': '01-028', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 111.0, 'PricePeakSeason': 197.58}, {'RoomId': '01-029', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 111.0, 'PricePeakSeason': 197.58}, {'RoomId': '01-030', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 111.0, 'PricePeakSeason': 197.58}, {'RoomId': '01-031', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 72.0, 'PricePeakSeason': 128.16}, {'RoomId': '01-032', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 72.0, 'PricePeakSeason': 128.16}, {'RoomId': '01-033', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 98.4, 'PricePeakSeason': 175.15}, {'RoomId': '01-034', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 111.0, 'PricePeakSeason': 197.58}, {'RoomId': '01-035', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 111.0, 'PricePeakSeason': 197.58}, {'RoomId': '01-036', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 72.0, 'PricePeakSeason': 128.16}, {'RoomId': '01-037', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 72.0, 'PricePeakSeason': 128.16}, {'RoomId': '01-038', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 48.0, 'PricePeakSeason': 85.44}, {'RoomId': '01-039', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 72.0, 'PricePeakSeason': 128.16}, {'RoomId': '01-040', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 72.0, 'PricePeakSeason': 128.16}, {'RoomId': '01-041', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 72.0, 'PricePeakSeason': 128.16}, {'RoomId': '01-042', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 227.55, 'PricePeakSeason': 405.04}, {'RoomId': '01-043', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 48.0, 'PricePeakSeason': 85.44}, {'RoomId': '01-044', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 147.6, 'PricePeakSeason': 262.73}, {'RoomId': '01-045', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 72.0, 'PricePeakSeason': 128.16}, {'RoomId': '01-046', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 98.4, 'PricePeakSeason': 175.15}, {'RoomId': '01-047', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 72.0, 'PricePeakSeason': 128.16}, {'RoomId': '01-048', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 72.0, 'PricePeakSeason': 128.16}, {'RoomId': '01-049', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 72.0, 'PricePeakSeason': 128.16}, {'RoomId': '01-050', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 111.0, 'PricePeakSeason': 197.58}, {'RoomId': '01-051', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 111.0, 'PricePeakSeason': 197.58}, {'RoomId': '01-052', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 48.0, 'PricePeakSeason': 85.44}, {'RoomId': '01-053', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 72.0, 'PricePeakSeason': 128.16}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>1407</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Solstice Plaza</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>{'Country': 'France', 'City': 'Cannes', 'ZipCode': '28581', 'Address': '997 Kristen Valley'}</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>{'OccupancyPeakSeasonWeight': 89, 'OccupancyOffSeasonWeight': 35, 'OccupancyBaseDiscountPercentage': 22, 'ExtraBedChargePercentage': 21, 'MealPlanWeights': {'room_only': {'name': 'Room Only', 'weight': 0.16}, 'room_and_breakfast': {'name': 'Room and Breakfast', 'weight': 0.57}, 'all_inclusive': {'name': 'All Inclusive', 'weight': 0.02}, 'half_board': {'name': 'Half Board', 'weight': 0.11}, 'full_board': {'name': 'Full Board', 'weight': 0.14}}, 'MealPlanPrices': {'Room Only': 1.0, 'Room and Breakfast': 1.12, 'All Inclusive': 2.14, 'Half Board': 1.48, 'Full Board': 1.65}, 'PromotionPriceDiscount': 27}</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>[{'RoomId': '01-001', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 78.0, 'PricePeakSeason': 138.84}, {'RoomId': '01-002', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 109.94, 'PricePeakSeason': 195.69}, {'RoomId': '01-003', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 186.42, 'PricePeakSeason': 331.83}, {'RoomId': '01-004', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 46.0, 'PricePeakSeason': 81.88}, {'RoomId': '01-005', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 109.94, 'PricePeakSeason': 195.69}, {'RoomId': '01-006', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 46.0, 'PricePeakSeason': 81.88}, {'RoomId': '01-007', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 146.0, 'PricePeakSeason': 259.88}, {'RoomId': '01-008', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 78.0, 'PricePeakSeason': 138.84}, {'RoomId': '01-009', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 78.0, 'PricePeakSeason': 138.84}, {'RoomId': '01-010', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 46.0, 'PricePeakSeason': 81.88}, {'RoomId': '01-011', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 46.0, 'PricePeakSeason': 81.88}, {'RoomId': '01-012', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 78.0, 'PricePeakSeason': 138.84}, {'RoomId': '01-013', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 46.0, 'PricePeakSeason': 81.88}, {'RoomId': '01-014', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 348.94, 'PricePeakSeason': 621.11}, {'RoomId': '01-015', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 46.0, 'PricePeakSeason': 81.88}, {'RoomId': '01-016', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 109.94, 'PricePeakSeason': 195.69}, {'RoomId': '01-017', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 78.0, 'PricePeakSeason': 138.84}, {'RoomId': '01-018', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 146.0, 'PricePeakSeason': 259.88}, {'RoomId': '01-019', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 78.0, 'PricePeakSeason': 138.84}, {'RoomId': '01-020', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 78.0, 'PricePeakSeason': 138.84}, {'RoomId': '02-001', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 78.0, 'PricePeakSeason': 138.84}, {'RoomId': '02-002', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 186.42, 'PricePeakSeason': 331.83}, {'RoomId': '02-003', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 186.42, 'PricePeakSeason': 331.83}, {'RoomId': '02-004', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 78.0, 'PricePeakSeason': 138.84}, {'RoomId': '02-005', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 46.0, 'PricePeakSeason': 81.88}, {'RoomId': '02-006', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 78.0, 'PricePeakSeason': 138.84}, {'RoomId': '02-007', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 78.0, 'PricePeakSeason': 138.84}, {'RoomId': '02-008', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 78.0, 'PricePeakSeason': 138.84}, {'RoomId': '02-009', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 78.0, 'PricePeakSeason': 138.84}, {'RoomId': '02-010', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 78.0, 'PricePeakSeason': 138.84}, {'RoomId': '02-011', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 78.0, 'PricePeakSeason': 138.84}, {'RoomId': '02-012', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 186.42, 'PricePeakSeason': 331.83}, {'RoomId': '02-013', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 46.0, 'PricePeakSeason': 81.88}, {'RoomId': '02-014', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 78.0, 'PricePeakSeason': 138.84}, {'RoomId': '02-015', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 78.0, 'PricePeakSeason': 138.84}, {'RoomId': '02-016', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 46.0, 'PricePeakSeason': 81.88}, {'RoomId': '02-017', 'Floor': '02', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 348.94, 'PricePeakSeason': 621.11}, {'RoomId': '02-018', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 78.0, 'PricePeakSeason': 138.84}, {'RoomId': '02-019', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 78.0, 'PricePeakSeason': 138.84}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>8370</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Equinox Suites</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>{'Country': 'France', 'City': 'Cannes', 'ZipCode': '53855', 'Address': '16566 Shields Center'}</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>{'OccupancyPeakSeasonWeight': 79, 'OccupancyOffSeasonWeight': 38, 'OccupancyBaseDiscountPercentage': 27, 'ExtraBedChargePercentage': 25, 'MealPlanWeights': {'room_only': {'name': 'Room Only', 'weight': 0.16}, 'room_and_breakfast': {'name': 'Room and Breakfast', 'weight': 0.43}, 'all_inclusive': {'name': 'All Inclusive', 'weight': 0.0}, 'half_board': {'name': 'Half Board', 'weight': 0.19}, 'full_board': {'name': 'Full Board', 'weight': 0.22}}, 'MealPlanPrices': {'Room Only': 1.0, 'Room and Breakfast': 1.11, 'All Inclusive': 2.05, 'Half Board': 1.44, 'Full Board': 1.64}, 'PromotionPriceDiscount': 10}</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>[{'RoomId': '01-001', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 102.0, 'PricePeakSeason': 159.12}, {'RoomId': '01-002', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 153.0, 'PricePeakSeason': 238.68}, {'RoomId': '01-003', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 102.0, 'PricePeakSeason': 159.12}, {'RoomId': '01-004', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 68.0, 'PricePeakSeason': 106.08}, {'RoomId': '01-005', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 68.0, 'PricePeakSeason': 106.08}, {'RoomId': '01-006', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 68.0, 'PricePeakSeason': 106.08}, {'RoomId': '01-007', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 102.0, 'PricePeakSeason': 159.12}, {'RoomId': '01-008', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 102.0, 'PricePeakSeason': 159.12}, {'RoomId': '01-009', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 102.0, 'PricePeakSeason': 159.12}, {'RoomId': '01-010', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 153.0, 'PricePeakSeason': 238.68}, {'RoomId': '01-011', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 102.0, 'PricePeakSeason': 159.12}, {'RoomId': '01-012', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 102.0, 'PricePeakSeason': 159.12}, {'RoomId': '01-013', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 153.0, 'PricePeakSeason': 238.68}, {'RoomId': '02-001', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 102.0, 'PricePeakSeason': 159.12}, {'RoomId': '02-002', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 208.08, 'PricePeakSeason': 324.6}, {'RoomId': '02-003', 'Floor': '02', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 312.12, 'PricePeakSeason': 486.91}, {'RoomId': '02-004', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 102.0, 'PricePeakSeason': 159.12}, {'RoomId': '02-005', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 68.0, 'PricePeakSeason': 106.08}, {'RoomId': '02-006', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 102.0, 'PricePeakSeason': 159.12}, {'RoomId': '02-007', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 68.0, 'PricePeakSeason': 106.08}, {'RoomId': '02-008', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 102.0, 'PricePeakSeason': 159.12}, {'RoomId': '02-009', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 153.0, 'PricePeakSeason': 238.68}, {'RoomId': '02-010', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 68.0, 'PricePeakSeason': 106.08}, {'RoomId': '02-011', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 102.0, 'PricePeakSeason': 159.12}, {'RoomId': '02-012', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 68.0, 'PricePeakSeason': 106.08}, {'RoomId': '03-001', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 102.0, 'PricePeakSeason': 159.12}, {'RoomId': '03-002', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 102.0, 'PricePeakSeason': 159.12}, {'RoomId': '03-003', 'Floor': '03', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 153.0, 'PricePeakSeason': 238.68}, {'RoomId': '03-004', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 102.0, 'PricePeakSeason': 159.12}, {'RoomId': '03-005', 'Floor': '03', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 153.0, 'PricePeakSeason': 238.68}, {'RoomId': '03-006', 'Floor': '03', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 68.0, 'PricePeakSeason': 106.08}, {'RoomId': '03-007', 'Floor': '03', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 208.08, 'PricePeakSeason': 324.6}, {'RoomId': '03-008', 'Floor': '03', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 153.0, 'PricePeakSeason': 238.68}, {'RoomId': '03-009', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 102.0, 'PricePeakSeason': 159.12}, {'RoomId': '03-010', 'Floor': '03', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 312.12, 'PricePeakSeason': 486.91}, {'RoomId': '03-011', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 102.0, 'PricePeakSeason': 159.12}, {'RoomId': '03-012', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 102.0, 'PricePeakSeason': 159.12}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>7010</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Azure Retreat</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>{'Country': 'France', 'City': 'Cannes', 'ZipCode': '88760', 'Address': '65133 Amanda Dam'}</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>{'OccupancyPeakSeasonWeight': 86, 'OccupancyOffSeasonWeight': 37, 'OccupancyBaseDiscountPercentage': 30, 'ExtraBedChargePercentage': 22, 'MealPlanWeights': {'room_only': {'name': 'Room Only', 'weight': 0.17}, 'room_and_breakfast': {'name': 'Room and Breakfast', 'weight': 0.56}, 'all_inclusive': {'name': 'All Inclusive', 'weight': 0.08}, 'half_board': {'name': 'Half Board', 'weight': 0.09}, 'full_board': {'name': 'Full Board', 'weight': 0.1}}, 'MealPlanPrices': {'Room Only': 1.0, 'Room and Breakfast': 1.13, 'All Inclusive': 2.01, 'Half Board': 1.31, 'Full Board': 1.62}, 'PromotionPriceDiscount': 26}</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>[{'RoomId': '01-001', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 84.0, 'PricePeakSeason': 160.44}, {'RoomId': '01-002', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 84.0, 'PricePeakSeason': 160.44}, {'RoomId': '01-003', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 84.0, 'PricePeakSeason': 160.44}, {'RoomId': '01-004', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 56.0, 'PricePeakSeason': 106.96}, {'RoomId': '01-005', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 56.0, 'PricePeakSeason': 106.96}, {'RoomId': '01-006', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 84.0, 'PricePeakSeason': 160.44}, {'RoomId': '01-007', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 84.0, 'PricePeakSeason': 160.44}, {'RoomId': '01-008', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 296.1, 'PricePeakSeason': 565.55}, {'RoomId': '01-009', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 56.0, 'PricePeakSeason': 106.96}, {'RoomId': '01-010', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 84.0, 'PricePeakSeason': 160.44}, {'RoomId': '01-011', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 56.0, 'PricePeakSeason': 106.96}, {'RoomId': '01-012', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 84.0, 'PricePeakSeason': 160.44}, {'RoomId': '01-013', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 84.0, 'PricePeakSeason': 160.44}, {'RoomId': '01-014', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 56.0, 'PricePeakSeason': 106.96}, {'RoomId': '01-015', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 131.6, 'PricePeakSeason': 251.36}, {'RoomId': '01-016', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 56.0, 'PricePeakSeason': 106.96}, {'RoomId': '01-017', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 84.0, 'PricePeakSeason': 160.44}, {'RoomId': '01-018', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 84.0, 'PricePeakSeason': 160.44}, {'RoomId': '01-019', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 84.0, 'PricePeakSeason': 160.44}, {'RoomId': '01-020', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 84.0, 'PricePeakSeason': 160.44}, {'RoomId': '01-021', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 56.0, 'PricePeakSeason': 106.96}, {'RoomId': '01-022', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 84.0, 'PricePeakSeason': 160.44}, {'RoomId': '01-023', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 126.0, 'PricePeakSeason': 240.66}, {'RoomId': '01-024', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 56.0, 'PricePeakSeason': 106.96}, {'RoomId': '01-025', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 56.0, 'PricePeakSeason': 106.96}, {'RoomId': '01-026', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 84.0, 'PricePeakSeason': 160.44}, {'RoomId': '01-027', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 84.0, 'PricePeakSeason': 160.44}, {'RoomId': '01-028', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 84.0, 'PricePeakSeason': 160.44}, {'RoomId': '01-029', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 84.0, 'PricePeakSeason': 160.44}, {'RoomId': '01-030', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 84.0, 'PricePeakSeason': 160.44}, {'RoomId': '01-031', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 84.0, 'PricePeakSeason': 160.44}, {'RoomId': '01-032', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 126.0, 'PricePeakSeason': 240.66}, {'RoomId': '01-033', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 197.4, 'PricePeakSeason': 377.03}, {'RoomId': '01-034', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 84.0, 'PricePeakSeason': 160.44}, {'RoomId': '01-035', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 84.0, 'PricePeakSeason': 160.44}, {'RoomId': '01-036', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 296.1, 'PricePeakSeason': 565.55}, {'RoomId': '01-037', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 131.6, 'PricePeakSeason': 251.36}, {'RoomId': '01-038', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 197.4, 'PricePeakSeason': 377.03}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>4694</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Crimson Manor</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>{'Country': 'France', 'City': 'Nice', 'ZipCode': '55797', 'Address': '7317 Brent Plains'}</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>{'OccupancyPeakSeasonWeight': 84, 'OccupancyOffSeasonWeight': 39, 'OccupancyBaseDiscountPercentage': 20, 'ExtraBedChargePercentage': 23, 'MealPlanWeights': {'room_only': {'name': 'Room Only', 'weight': 0.2}, 'room_and_breakfast': {'name': 'Room and Breakfast', 'weight': 0.44}, 'all_inclusive': {'name': 'All Inclusive', 'weight': 0.01}, 'half_board': {'name': 'Half Board', 'weight': 0.16}, 'full_board': {'name': 'Full Board', 'weight': 0.19}}, 'MealPlanPrices': {'Room Only': 1.0, 'Room and Breakfast': 1.2, 'All Inclusive': 2.09, 'Half Board': 1.38, 'Full Board': 1.55}, 'PromotionPriceDiscount': 10}</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>[{'RoomId': '01-001', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.0, 'PricePeakSeason': 150.88}, {'RoomId': '01-002', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.0, 'PricePeakSeason': 150.88}, {'RoomId': '01-003', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.0, 'PricePeakSeason': 150.88}, {'RoomId': '01-004', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 123.0, 'PricePeakSeason': 226.32}, {'RoomId': '01-005', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.0, 'PricePeakSeason': 150.88}, {'RoomId': '01-006', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 76.05, 'PricePeakSeason': 139.93}, {'RoomId': '01-007', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 45.0, 'PricePeakSeason': 82.8}, {'RoomId': '01-008', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.0, 'PricePeakSeason': 150.88}, {'RoomId': '01-009', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 45.0, 'PricePeakSeason': 82.8}, {'RoomId': '01-010', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 45.0, 'PricePeakSeason': 82.8}, {'RoomId': '01-011', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.0, 'PricePeakSeason': 150.88}, {'RoomId': '01-012', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.0, 'PricePeakSeason': 150.88}, {'RoomId': '01-013', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.0, 'PricePeakSeason': 150.88}, {'RoomId': '01-014', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 123.0, 'PricePeakSeason': 226.32}, {'RoomId': '01-015', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 45.0, 'PricePeakSeason': 82.8}, {'RoomId': '01-016', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 138.58, 'PricePeakSeason': 254.99}, {'RoomId': '01-017', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.0, 'PricePeakSeason': 150.88}, {'RoomId': '01-018', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 123.0, 'PricePeakSeason': 226.32}, {'RoomId': '01-019', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.0, 'PricePeakSeason': 150.88}, {'RoomId': '01-020', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 45.0, 'PricePeakSeason': 82.8}, {'RoomId': '01-021', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 76.05, 'PricePeakSeason': 139.93}, {'RoomId': '01-022', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.0, 'PricePeakSeason': 150.88}, {'RoomId': '01-023', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 138.58, 'PricePeakSeason': 254.99}, {'RoomId': '01-024', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.0, 'PricePeakSeason': 150.88}, {'RoomId': '01-025', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 123.0, 'PricePeakSeason': 226.32}, {'RoomId': '02-001', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 45.0, 'PricePeakSeason': 82.8}, {'RoomId': '02-002', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 123.0, 'PricePeakSeason': 226.32}, {'RoomId': '02-003', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 123.0, 'PricePeakSeason': 226.32}, {'RoomId': '02-004', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.0, 'PricePeakSeason': 150.88}, {'RoomId': '02-005', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.0, 'PricePeakSeason': 150.88}, {'RoomId': '02-006', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.0, 'PricePeakSeason': 150.88}, {'RoomId': '02-007', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 138.58, 'PricePeakSeason': 254.99}, {'RoomId': '02-008', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 138.58, 'PricePeakSeason': 254.99}, {'RoomId': '02-009', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.0, 'PricePeakSeason': 150.88}, {'RoomId': '02-010', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 45.0, 'PricePeakSeason': 82.8}, {'RoomId': '02-011', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 45.0, 'PricePeakSeason': 82.8}, {'RoomId': '02-012', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 123.0, 'PricePeakSeason': 226.32}, {'RoomId': '02-013', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 138.58, 'PricePeakSeason': 254.99}, {'RoomId': '02-014', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 45.0, 'PricePeakSeason': 82.8}, {'RoomId': '02-015', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.0, 'PricePeakSeason': 150.88}, {'RoomId': '02-016', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.0, 'PricePeakSeason': 150.88}, {'RoomId': '02-017', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.0, 'PricePeakSeason': 150.88}, {'RoomId': '02-018', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 123.0, 'PricePeakSeason': 226.32}, {'RoomId': '02-019', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 138.58, 'PricePeakSeason': 254.99}, {'RoomId': '02-020', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.0, 'PricePeakSeason': 150.88}, {'RoomId': '02-021', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 45.0, 'PricePeakSeason': 82.8}, {'RoomId': '02-022', 'Floor': '02', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 76.05, 'PricePeakSeason': 139.93}, {'RoomId': '02-023', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.0, 'PricePeakSeason': 150.88}, {'RoomId': '02-024', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 45.0, 'PricePeakSeason': 82.8}, {'RoomId': '02-025', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.0, 'PricePeakSeason': 150.88}, {'RoomId': '03-001', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.0, 'PricePeakSeason': 150.88}, {'RoomId': '03-002', 'Floor': '03', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 45.0, 'PricePeakSeason': 82.8}, {'RoomId': '03-003', 'Floor': '03', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 138.58, 'PricePeakSeason': 254.99}, {'RoomId': '03-004', 'Floor': '03', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 207.87, 'PricePeakSeason': 382.48}, {'RoomId': '03-005', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.0, 'PricePeakSeason': 150.88}, {'RoomId': '03-006', 'Floor': '03', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 45.0, 'PricePeakSeason': 82.8}, {'RoomId': '03-007', 'Floor': '03', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 138.58, 'PricePeakSeason': 254.99}, {'RoomId': '03-008', 'Floor': '03', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 138.58, 'PricePeakSeason': 254.99}, {'RoomId': '03-009', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.0, 'PricePeakSeason': 150.88}, {'RoomId': '03-010', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.0, 'PricePeakSeason': 150.88}, {'RoomId': '03-011', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.0, 'PricePeakSeason': 150.88}, {'RoomId': '03-012', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.0, 'PricePeakSeason': 150.88}, {'RoomId': '03-013', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.0, 'PricePeakSeason': 150.88}, {'RoomId': '03-014', 'Floor': '03', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 207.87, 'PricePeakSeason': 382.48}, {'RoomId': '03-015', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.0, 'PricePeakSeason': 150.88}, {'RoomId': '03-016', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.0, 'PricePeakSeason': 150.88}, {'RoomId': '03-017', 'Floor': '03', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 123.0, 'PricePeakSeason': 226.32}, {'RoomId': '03-018', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.0, 'PricePeakSeason': 150.88}, {'RoomId': '03-019', 'Floor': '03', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 45.0, 'PricePeakSeason': 82.8}, {'RoomId': '03-020', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.0, 'PricePeakSeason': 150.88}, {'RoomId': '03-021', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.0, 'PricePeakSeason': 150.88}, {'RoomId': '03-022', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.0, 'PricePeakSeason': 150.88}, {'RoomId': '03-023', 'Floor': '03', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 123.0, 'PricePeakSeason': 226.32}, {'RoomId': '03-024', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.0, 'PricePeakSeason': 150.88}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>6626</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Seraphina Hotel</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>{'Country': 'France', 'City': 'Cannes', 'ZipCode': '02435', 'Address': '26773 Barrera Expressway'}</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>{'OccupancyPeakSeasonWeight': 85, 'OccupancyOffSeasonWeight': 34, 'OccupancyBaseDiscountPercentage': 20, 'ExtraBedChargePercentage': 24, 'MealPlanWeights': {'room_only': {'name': 'Room Only', 'weight': 0.1}, 'room_and_breakfast': {'name': 'Room and Breakfast', 'weight': 0.44}, 'all_inclusive': {'name': 'All Inclusive', 'weight': 0.03}, 'half_board': {'name': 'Half Board', 'weight': 0.22}, 'full_board': {'name': 'Full Board', 'weight': 0.21}}, 'MealPlanPrices': {'Room Only': 1.0, 'Room and Breakfast': 1.16, 'All Inclusive': 2.14, 'Half Board': 1.43, 'Full Board': 1.55}, 'PromotionPriceDiscount': 23}</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>[{'RoomId': '01-001', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 160.38}, {'RoomId': '01-002', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 160.38}, {'RoomId': '01-003', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 160.38}, {'RoomId': '01-004', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 43.0, 'PricePeakSeason': 69.66}, {'RoomId': '01-005', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 148.5, 'PricePeakSeason': 240.57}, {'RoomId': '01-006', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 43.0, 'PricePeakSeason': 69.66}, {'RoomId': '01-007', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 164.34, 'PricePeakSeason': 266.23}, {'RoomId': '01-008', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 43.0, 'PricePeakSeason': 69.66}, {'RoomId': '01-009', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 43.0, 'PricePeakSeason': 69.66}, {'RoomId': '01-010', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 160.38}, {'RoomId': '01-011', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 43.0, 'PricePeakSeason': 69.66}, {'RoomId': '01-012', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 43.0, 'PricePeakSeason': 69.66}, {'RoomId': '01-013', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 43.0, 'PricePeakSeason': 69.66}, {'RoomId': '01-014', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 148.5, 'PricePeakSeason': 240.57}, {'RoomId': '01-015', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 160.38}, {'RoomId': '01-016', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 160.38}, {'RoomId': '01-017', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 160.38}, {'RoomId': '01-018', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 160.38}, {'RoomId': '01-019', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 43.0, 'PricePeakSeason': 69.66}, {'RoomId': '01-020', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 160.38}, {'RoomId': '01-021', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 160.38}, {'RoomId': '01-022', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 148.5, 'PricePeakSeason': 240.57}, {'RoomId': '01-023', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 160.38}, {'RoomId': '01-024', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 160.38}, {'RoomId': '01-025', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 164.34, 'PricePeakSeason': 266.23}, {'RoomId': '01-026', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 43.0, 'PricePeakSeason': 69.66}, {'RoomId': '01-027', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 43.0, 'PricePeakSeason': 69.66}, {'RoomId': '01-028', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 160.38}, {'RoomId': '01-029', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 148.5, 'PricePeakSeason': 240.57}, {'RoomId': '01-030', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 160.38}, {'RoomId': '01-031', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 246.51, 'PricePeakSeason': 399.35}, {'RoomId': '01-032', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 160.38}, {'RoomId': '01-033', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 160.38}, {'RoomId': '01-034', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 71.38, 'PricePeakSeason': 115.64}, {'RoomId': '01-035', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 71.38, 'PricePeakSeason': 115.64}, {'RoomId': '01-036', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 160.38}, {'RoomId': '01-037', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 160.38}, {'RoomId': '01-038', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 43.0, 'PricePeakSeason': 69.66}, {'RoomId': '01-039', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 160.38}, {'RoomId': '01-040', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 148.5, 'PricePeakSeason': 240.57}, {'RoomId': '01-041', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 160.38}, {'RoomId': '01-042', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 164.34, 'PricePeakSeason': 266.23}, {'RoomId': '01-043', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 43.0, 'PricePeakSeason': 69.66}, {'RoomId': '01-044', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 246.51, 'PricePeakSeason': 399.35}, {'RoomId': '01-045', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 160.38}, {'RoomId': '01-046', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 43.0, 'PricePeakSeason': 69.66}, {'RoomId': '01-047', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 43.0, 'PricePeakSeason': 69.66}, {'RoomId': '01-048', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 43.0, 'PricePeakSeason': 69.66}, {'RoomId': '01-049', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 71.38, 'PricePeakSeason': 115.64}, {'RoomId': '01-050', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 160.38}, {'RoomId': '01-051', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 164.34, 'PricePeakSeason': 266.23}, {'RoomId': '01-052', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 43.0, 'PricePeakSeason': 69.66}, {'RoomId': '01-053', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 148.5, 'PricePeakSeason': 240.57}, {'RoomId': '01-054', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 160.38}, {'RoomId': '01-055', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 148.5, 'PricePeakSeason': 240.57}, {'RoomId': '01-056', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 148.5, 'PricePeakSeason': 240.57}, {'RoomId': '01-057', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 43.0, 'PricePeakSeason': 69.66}, {'RoomId': '01-058', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 43.0, 'PricePeakSeason': 69.66}, {'RoomId': '01-059', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 148.5, 'PricePeakSeason': 240.57}, {'RoomId': '01-060', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 148.5, 'PricePeakSeason': 240.57}, {'RoomId': '01-061', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 43.0, 'PricePeakSeason': 69.66}, {'RoomId': '01-062', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 164.34, 'PricePeakSeason': 266.23}, {'RoomId': '01-063', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 164.34, 'PricePeakSeason': 266.23}, {'RoomId': '01-064', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 160.38}, {'RoomId': '01-065', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 160.38}, {'RoomId': '01-066', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 43.0, 'PricePeakSeason': 69.66}, {'RoomId': '01-067', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 148.5, 'PricePeakSeason': 240.57}, {'RoomId': '01-068', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 164.34, 'PricePeakSeason': 266.23}, {'RoomId': '01-069', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 246.51, 'PricePeakSeason': 399.35}, {'RoomId': '01-070', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 160.38}, {'RoomId': '01-071', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 246.51, 'PricePeakSeason': 399.35}, {'RoomId': '01-072', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 160.38}, {'RoomId': '01-073', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 71.38, 'PricePeakSeason': 115.64}, {'RoomId': '01-074', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 43.0, 'PricePeakSeason': 69.66}, {'RoomId': '01-075', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 71.38, 'PricePeakSeason': 115.64}, {'RoomId': '01-076', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 43.0, 'PricePeakSeason': 69.66}, {'RoomId': '01-077', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 160.38}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>8079</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Elysian Suites</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>{'Country': 'France', 'City': 'Nice', 'ZipCode': '50173', 'Address': '4746 Moore Hill'}</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>{'OccupancyPeakSeasonWeight': 87, 'OccupancyOffSeasonWeight': 30, 'OccupancyBaseDiscountPercentage': 23, 'ExtraBedChargePercentage': 20, 'MealPlanWeights': {'room_only': {'name': 'Room Only', 'weight': 0.14}, 'room_and_breakfast': {'name': 'Room and Breakfast', 'weight': 0.49}, 'all_inclusive': {'name': 'All Inclusive', 'weight': 0.07}, 'half_board': {'name': 'Half Board', 'weight': 0.08}, 'full_board': {'name': 'Full Board', 'weight': 0.22}}, 'MealPlanPrices': {'Room Only': 1.0, 'Room and Breakfast': 1.14, 'All Inclusive': 2.08, 'Half Board': 1.45, 'Full Board': 1.53}, 'PromotionPriceDiscount': 17}</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>[{'RoomId': '01-001', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 78.0, 'PricePeakSeason': 131.04}, {'RoomId': '01-002', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 78.0, 'PricePeakSeason': 131.04}, {'RoomId': '01-003', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 77.0, 'PricePeakSeason': 129.36}, {'RoomId': '01-004', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 117.0, 'PricePeakSeason': 196.56}, {'RoomId': '01-005', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 120.12, 'PricePeakSeason': 201.8}, {'RoomId': '01-006', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 180.18, 'PricePeakSeason': 302.7}, {'RoomId': '01-007', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 78.0, 'PricePeakSeason': 131.04}, {'RoomId': '01-008', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 78.0, 'PricePeakSeason': 131.04}, {'RoomId': '01-009', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 50.0, 'PricePeakSeason': 84.0}, {'RoomId': '01-010', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 117.0, 'PricePeakSeason': 196.56}, {'RoomId': '01-011', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 78.0, 'PricePeakSeason': 131.04}, {'RoomId': '01-012', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 120.12, 'PricePeakSeason': 201.8}, {'RoomId': '01-013', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 78.0, 'PricePeakSeason': 131.04}, {'RoomId': '01-014', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 78.0, 'PricePeakSeason': 131.04}, {'RoomId': '01-015', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 78.0, 'PricePeakSeason': 131.04}, {'RoomId': '01-016', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 50.0, 'PricePeakSeason': 84.0}, {'RoomId': '01-017', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 117.0, 'PricePeakSeason': 196.56}, {'RoomId': '01-018', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 78.0, 'PricePeakSeason': 131.04}, {'RoomId': '01-019', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 50.0, 'PricePeakSeason': 84.0}, {'RoomId': '01-020', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 117.0, 'PricePeakSeason': 196.56}, {'RoomId': '01-021', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 50.0, 'PricePeakSeason': 84.0}, {'RoomId': '01-022', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 78.0, 'PricePeakSeason': 131.04}, {'RoomId': '01-023', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 120.12, 'PricePeakSeason': 201.8}, {'RoomId': '01-024', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 78.0, 'PricePeakSeason': 131.04}, {'RoomId': '01-025', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 78.0, 'PricePeakSeason': 131.04}, {'RoomId': '01-026', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 50.0, 'PricePeakSeason': 84.0}, {'RoomId': '01-027', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 78.0, 'PricePeakSeason': 131.04}, {'RoomId': '01-028', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 120.12, 'PricePeakSeason': 201.8}, {'RoomId': '01-029', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 78.0, 'PricePeakSeason': 131.04}, {'RoomId': '01-030', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 78.0, 'PricePeakSeason': 131.04}, {'RoomId': '01-031', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 78.0, 'PricePeakSeason': 131.04}, {'RoomId': '01-032', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 50.0, 'PricePeakSeason': 84.0}, {'RoomId': '02-001', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 78.0, 'PricePeakSeason': 131.04}, {'RoomId': '02-002', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 117.0, 'PricePeakSeason': 196.56}, {'RoomId': '02-003', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 117.0, 'PricePeakSeason': 196.56}, {'RoomId': '02-004', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 50.0, 'PricePeakSeason': 84.0}, {'RoomId': '02-005', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 78.0, 'PricePeakSeason': 131.04}, {'RoomId': '02-006', 'Floor': '02', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 77.0, 'PricePeakSeason': 129.36}, {'RoomId': '02-007', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 78.0, 'PricePeakSeason': 131.04}, {'RoomId': '02-008', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 117.0, 'PricePeakSeason': 196.56}, {'RoomId': '02-009', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 117.0, 'PricePeakSeason': 196.56}, {'RoomId': '02-010', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 117.0, 'PricePeakSeason': 196.56}, {'RoomId': '02-011', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 50.0, 'PricePeakSeason': 84.0}, {'RoomId': '02-012', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 50.0, 'PricePeakSeason': 84.0}, {'RoomId': '02-013', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 78.0, 'PricePeakSeason': 131.04}, {'RoomId': '02-014', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 117.0, 'PricePeakSeason': 196.56}, {'RoomId': '02-015', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 78.0, 'PricePeakSeason': 131.04}, {'RoomId': '02-016', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 78.0, 'PricePeakSeason': 131.04}, {'RoomId': '02-017', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 50.0, 'PricePeakSeason': 84.0}, {'RoomId': '02-018', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 78.0, 'PricePeakSeason': 131.04}, {'RoomId': '02-019', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 120.12, 'PricePeakSeason': 201.8}, {'RoomId': '02-020', 'Floor': '02', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 77.0, 'PricePeakSeason': 129.36}, {'RoomId': '02-021', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 78.0, 'PricePeakSeason': 131.04}, {'RoomId': '02-022', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 50.0, 'PricePeakSeason': 84.0}, {'RoomId': '02-023', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 78.0, 'PricePeakSeason': 131.04}, {'RoomId': '02-024', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 117.0, 'PricePeakSeason': 196.56}, {'RoomId': '02-025', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 50.0, 'PricePeakSeason': 84.0}, {'RoomId': '02-026', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 117.0, 'PricePeakSeason': 196.56}, {'RoomId': '02-027', 'Floor': '02', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 180.18, 'PricePeakSeason': 302.7}, {'RoomId': '02-028', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 120.12, 'PricePeakSeason': 201.8}, {'RoomId': '02-029', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 78.0, 'PricePeakSeason': 131.04}, {'RoomId': '02-030', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 50.0, 'PricePeakSeason': 84.0}, {'RoomId': '02-031', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 78.0, 'PricePeakSeason': 131.04}, {'RoomId': '02-032', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 78.0, 'PricePeakSeason': 131.04}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2202</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Valerian Residences</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>{'Country': 'France', 'City': 'Cannes', 'ZipCode': '29035', 'Address': '805 Brendan Neck'}</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>{'OccupancyPeakSeasonWeight': 96, 'OccupancyOffSeasonWeight': 30, 'OccupancyBaseDiscountPercentage': 30, 'ExtraBedChargePercentage': 21, 'MealPlanWeights': {'room_only': {'name': 'Room Only', 'weight': 0.12}, 'room_and_breakfast': {'name': 'Room and Breakfast', 'weight': 0.35}, 'all_inclusive': {'name': 'All Inclusive', 'weight': 0.09}, 'half_board': {'name': 'Half Board', 'weight': 0.17}, 'full_board': {'name': 'Full Board', 'weight': 0.27}}, 'MealPlanPrices': {'Room Only': 1.0, 'Room and Breakfast': 1.14, 'All Inclusive': 2.18, 'Half Board': 1.39, 'Full Board': 1.64}, 'PromotionPriceDiscount': 13}</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>[{'RoomId': '01-001', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 244.53, 'PricePeakSeason': 447.49}, {'RoomId': '01-002', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 66.0, 'PricePeakSeason': 120.78}, {'RoomId': '01-003', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 181.17}, {'RoomId': '01-004', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 181.17}, {'RoomId': '01-005', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 163.02, 'PricePeakSeason': 298.33}, {'RoomId': '01-006', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 181.17}, {'RoomId': '01-007', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 181.17}, {'RoomId': '01-008', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 148.5, 'PricePeakSeason': 271.75}, {'RoomId': '01-009', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 181.17}, {'RoomId': '01-010', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 181.17}, {'RoomId': '01-011', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 66.0, 'PricePeakSeason': 120.78}, {'RoomId': '01-012', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 181.17}, {'RoomId': '01-013', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 66.0, 'PricePeakSeason': 120.78}, {'RoomId': '01-014', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 244.53, 'PricePeakSeason': 447.49}, {'RoomId': '01-015', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 66.0, 'PricePeakSeason': 120.78}, {'RoomId': '01-016', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 244.53, 'PricePeakSeason': 447.49}, {'RoomId': '01-017', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 181.17}, {'RoomId': '01-018', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 66.0, 'PricePeakSeason': 120.78}, {'RoomId': '01-019', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 148.5, 'PricePeakSeason': 271.75}, {'RoomId': '01-020', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 244.53, 'PricePeakSeason': 447.49}, {'RoomId': '02-001', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 181.17}, {'RoomId': '02-002', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 66.0, 'PricePeakSeason': 120.78}, {'RoomId': '02-003', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 181.17}, {'RoomId': '02-004', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 148.5, 'PricePeakSeason': 271.75}, {'RoomId': '02-005', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 181.17}, {'RoomId': '02-006', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 181.17}, {'RoomId': '02-007', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 181.17}, {'RoomId': '02-008', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 244.53, 'PricePeakSeason': 447.49}, {'RoomId': '02-009', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 181.17}, {'RoomId': '02-010', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 181.17}, {'RoomId': '02-011', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 181.17}, {'RoomId': '02-012', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 181.17}, {'RoomId': '02-013', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 181.17}, {'RoomId': '02-014', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 181.17}, {'RoomId': '02-015', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 181.17}, {'RoomId': '02-016', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 181.17}, {'RoomId': '02-017', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 66.0, 'PricePeakSeason': 120.78}, {'RoomId': '02-018', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 244.53, 'PricePeakSeason': 447.49}, {'RoomId': '02-019', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 244.53, 'PricePeakSeason': 447.49}, {'RoomId': '03-001', 'Floor': '03', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 148.5, 'PricePeakSeason': 271.75}, {'RoomId': '03-002', 'Floor': '03', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 66.0, 'PricePeakSeason': 120.78}, {'RoomId': '03-003', 'Floor': '03', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 148.5, 'PricePeakSeason': 271.75}, {'RoomId': '03-004', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 181.17}, {'RoomId': '03-005', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 181.17}, {'RoomId': '03-006', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 181.17}, {'RoomId': '03-007', 'Floor': '03', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 148.5, 'PricePeakSeason': 271.75}, {'RoomId': '03-008', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 181.17}, {'RoomId': '03-009', 'Floor': '03', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 66.0, 'PricePeakSeason': 120.78}, {'RoomId': '03-010', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 181.17}, {'RoomId': '03-011', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 181.17}, {'RoomId': '03-012', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 181.17}, {'RoomId': '03-013', 'Floor': '03', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 148.5, 'PricePeakSeason': 271.75}, {'RoomId': '03-014', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 181.17}, {'RoomId': '03-015', 'Floor': '03', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 244.53, 'PricePeakSeason': 447.49}, {'RoomId': '03-016', 'Floor': '03', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 163.02, 'PricePeakSeason': 298.33}, {'RoomId': '03-017', 'Floor': '03', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 66.0, 'PricePeakSeason': 120.78}, {'RoomId': '03-018', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 181.17}, {'RoomId': '03-019', 'Floor': '03', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 66.0, 'PricePeakSeason': 120.78}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>7710</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Avant-Garde Hotel</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>{'Country': 'France', 'City': 'Cannes', 'ZipCode': '66410', 'Address': '81219 Emma Freeway'}</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>{'OccupancyPeakSeasonWeight': 95, 'OccupancyOffSeasonWeight': 25, 'OccupancyBaseDiscountPercentage': 25, 'ExtraBedChargePercentage': 25, 'MealPlanWeights': {'room_only': {'name': 'Room Only', 'weight': 0.15}, 'room_and_breakfast': {'name': 'Room and Breakfast', 'weight': 0.49}, 'all_inclusive': {'name': 'All Inclusive', 'weight': 0.02}, 'half_board': {'name': 'Half Board', 'weight': 0.2}, 'full_board': {'name': 'Full Board', 'weight': 0.14}}, 'MealPlanPrices': {'Room Only': 1.0, 'Room and Breakfast': 1.12, 'All Inclusive': 2.03, 'Half Board': 1.42, 'Full Board': 1.62}, 'PromotionPriceDiscount': 24}</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>[{'RoomId': '01-001', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 129.28, 'PricePeakSeason': 197.8}, {'RoomId': '01-002', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 193.92, 'PricePeakSeason': 296.7}, {'RoomId': '01-003', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 290.88, 'PricePeakSeason': 445.05}, {'RoomId': '01-004', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 129.28, 'PricePeakSeason': 197.8}, {'RoomId': '01-005', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 129.28, 'PricePeakSeason': 197.8}, {'RoomId': '01-006', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 146.88}, {'RoomId': '01-007', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 193.92, 'PricePeakSeason': 296.7}, {'RoomId': '01-008', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 146.88}, {'RoomId': '01-009', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 146.88}, {'RoomId': '01-010', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 64.0, 'PricePeakSeason': 97.92}, {'RoomId': '01-011', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 193.92, 'PricePeakSeason': 296.7}, {'RoomId': '01-012', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 146.88}, {'RoomId': '01-013', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 146.88}, {'RoomId': '01-014', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 64.0, 'PricePeakSeason': 97.92}, {'RoomId': '01-015', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 146.88}, {'RoomId': '01-016', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 290.88, 'PricePeakSeason': 445.05}, {'RoomId': '01-017', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 193.92, 'PricePeakSeason': 296.7}, {'RoomId': '01-018', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 64.0, 'PricePeakSeason': 97.92}, {'RoomId': '01-019', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 129.28, 'PricePeakSeason': 197.8}, {'RoomId': '01-020', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 193.92, 'PricePeakSeason': 296.7}, {'RoomId': '01-021', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 146.88}, {'RoomId': '01-022', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 64.0, 'PricePeakSeason': 97.92}, {'RoomId': '01-023', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 144.0, 'PricePeakSeason': 220.32}, {'RoomId': '01-024', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 146.88}, {'RoomId': '01-025', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 146.88}, {'RoomId': '01-026', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 64.0, 'PricePeakSeason': 97.92}, {'RoomId': '01-027', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 193.92, 'PricePeakSeason': 296.7}, {'RoomId': '01-028', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 129.28, 'PricePeakSeason': 197.8}, {'RoomId': '01-029', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 193.92, 'PricePeakSeason': 296.7}, {'RoomId': '01-030', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 64.0, 'PricePeakSeason': 97.92}, {'RoomId': '01-031', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 129.28, 'PricePeakSeason': 197.8}, {'RoomId': '01-032', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 146.88}, {'RoomId': '01-033', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 146.88}, {'RoomId': '01-034', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 193.92, 'PricePeakSeason': 296.7}, {'RoomId': '01-035', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 146.88}, {'RoomId': '01-036', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 146.88}, {'RoomId': '01-037', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 64.0, 'PricePeakSeason': 97.92}, {'RoomId': '01-038', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 129.28, 'PricePeakSeason': 197.8}, {'RoomId': '01-039', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 146.88}, {'RoomId': '01-040', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 64.0, 'PricePeakSeason': 97.92}, {'RoomId': '01-041', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 129.28, 'PricePeakSeason': 197.8}, {'RoomId': '01-042', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 64.0, 'PricePeakSeason': 97.92}, {'RoomId': '01-043', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 64.0, 'PricePeakSeason': 97.92}, {'RoomId': '01-044', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 146.88}, {'RoomId': '01-045', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 193.92, 'PricePeakSeason': 296.7}, {'RoomId': '01-046', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 193.92, 'PricePeakSeason': 296.7}, {'RoomId': '01-047', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 146.88}, {'RoomId': '01-048', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 193.92, 'PricePeakSeason': 296.7}, {'RoomId': '01-049', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 146.88}, {'RoomId': '01-050', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 290.88, 'PricePeakSeason': 445.05}, {'RoomId': '01-051', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 146.88}, {'RoomId': '01-052', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 146.88}, {'RoomId': '01-053', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 193.92, 'PricePeakSeason': 296.7}, {'RoomId': '01-054', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 64.0, 'PricePeakSeason': 97.92}, {'RoomId': '01-055', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 64.0, 'PricePeakSeason': 97.92}, {'RoomId': '01-056', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 146.88}, {'RoomId': '01-057', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 144.0, 'PricePeakSeason': 220.32}, {'RoomId': '01-058', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 129.28, 'PricePeakSeason': 197.8}, {'RoomId': '01-059', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 290.88, 'PricePeakSeason': 445.05}, {'RoomId': '01-060', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 146.88}, {'RoomId': '01-061', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 129.28, 'PricePeakSeason': 197.8}, {'RoomId': '01-062', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 146.88}, {'RoomId': '01-063', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 193.92, 'PricePeakSeason': 296.7}, {'RoomId': '01-064', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 146.88}, {'RoomId': '01-065', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 64.0, 'PricePeakSeason': 97.92}, {'RoomId': '01-066', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 290.88, 'PricePeakSeason': 445.05}, {'RoomId': '01-067', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 64.0, 'PricePeakSeason': 97.92}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>4454</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Emerald Grove</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>{'Country': 'France', 'City': 'Cannes', 'ZipCode': '53424', 'Address': '399 Christine Manor'}</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>{'OccupancyPeakSeasonWeight': 93, 'OccupancyOffSeasonWeight': 25, 'OccupancyBaseDiscountPercentage': 22, 'ExtraBedChargePercentage': 21, 'MealPlanWeights': {'room_only': {'name': 'Room Only', 'weight': 0.13}, 'room_and_breakfast': {'name': 'Room and Breakfast', 'weight': 0.44}, 'all_inclusive': {'name': 'All Inclusive', 'weight': 0.08}, 'half_board': {'name': 'Half Board', 'weight': 0.18}, 'full_board': {'name': 'Full Board', 'weight': 0.17}}, 'MealPlanPrices': {'Room Only': 1.0, 'Room and Breakfast': 1.14, 'All Inclusive': 2.12, 'Half Board': 1.4, 'Full Board': 1.59}, 'PromotionPriceDiscount': 24}</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>[{'RoomId': '01-001', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 168.75, 'PricePeakSeason': 303.75}, {'RoomId': '01-002', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 75.0, 'PricePeakSeason': 135.0}, {'RoomId': '01-003', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 50.0, 'PricePeakSeason': 90.0}, {'RoomId': '01-004', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 168.75, 'PricePeakSeason': 303.75}, {'RoomId': '01-005', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 112.5, 'PricePeakSeason': 202.5}, {'RoomId': '01-006', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 112.5, 'PricePeakSeason': 202.5}, {'RoomId': '01-007', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 50.0, 'PricePeakSeason': 90.0}, {'RoomId': '01-008', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 75.0, 'PricePeakSeason': 135.0}, {'RoomId': '01-009', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 168.75, 'PricePeakSeason': 303.75}, {'RoomId': '01-010', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 168.75, 'PricePeakSeason': 303.75}, {'RoomId': '01-011', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 126.0, 'PricePeakSeason': 226.8}, {'RoomId': '01-012', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 168.75, 'PricePeakSeason': 303.75}, {'RoomId': '01-013', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 75.0, 'PricePeakSeason': 135.0}, {'RoomId': '01-014', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 75.0, 'PricePeakSeason': 135.0}, {'RoomId': '01-015', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 75.0, 'PricePeakSeason': 135.0}, {'RoomId': '01-016', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 168.75, 'PricePeakSeason': 303.75}, {'RoomId': '01-017', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 168.75, 'PricePeakSeason': 303.75}, {'RoomId': '01-018', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 112.5, 'PricePeakSeason': 202.5}, {'RoomId': '01-019', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 112.5, 'PricePeakSeason': 202.5}, {'RoomId': '01-020', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 168.75, 'PricePeakSeason': 303.75}, {'RoomId': '01-021', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 112.5, 'PricePeakSeason': 202.5}, {'RoomId': '01-022', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 75.0, 'PricePeakSeason': 135.0}, {'RoomId': '01-023', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 112.5, 'PricePeakSeason': 202.5}, {'RoomId': '01-024', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 75.0, 'PricePeakSeason': 135.0}, {'RoomId': '01-025', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 75.0, 'PricePeakSeason': 135.0}, {'RoomId': '01-026', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 75.0, 'PricePeakSeason': 135.0}, {'RoomId': '01-027', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 75.0, 'PricePeakSeason': 135.0}, {'RoomId': '01-028', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 50.0, 'PricePeakSeason': 90.0}, {'RoomId': '01-029', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 75.0, 'PricePeakSeason': 135.0}, {'RoomId': '01-030', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 75.0, 'PricePeakSeason': 135.0}, {'RoomId': '01-031', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 50.0, 'PricePeakSeason': 90.0}, {'RoomId': '01-032', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 75.0, 'PricePeakSeason': 135.0}, {'RoomId': '01-033', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 168.75, 'PricePeakSeason': 303.75}, {'RoomId': '01-034', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 50.0, 'PricePeakSeason': 90.0}, {'RoomId': '01-035', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 283.5, 'PricePeakSeason': 510.3}, {'RoomId': '01-036', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 50.0, 'PricePeakSeason': 90.0}, {'RoomId': '01-037', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 75.0, 'PricePeakSeason': 135.0}, {'RoomId': '01-038', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 75.0, 'PricePeakSeason': 135.0}, {'RoomId': '01-039', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 75.0, 'PricePeakSeason': 135.0}, {'RoomId': '01-040', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 112.5, 'PricePeakSeason': 202.5}, {'RoomId': '01-041', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 168.75, 'PricePeakSeason': 303.75}, {'RoomId': '01-042', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 75.0, 'PricePeakSeason': 135.0}, {'RoomId': '01-043', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 168.75, 'PricePeakSeason': 303.75}, {'RoomId': '01-044', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 75.0, 'PricePeakSeason': 135.0}, {'RoomId': '01-045', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 50.0, 'PricePeakSeason': 90.0}, {'RoomId': '01-046', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 75.0, 'PricePeakSeason': 135.0}, {'RoomId': '01-047', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 112.5, 'PricePeakSeason': 202.5}, {'RoomId': '01-048', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 112.5, 'PricePeakSeason': 202.5}, {'RoomId': '01-049', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 168.75, 'PricePeakSeason': 303.75}, {'RoomId': '01-050', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 75.0, 'PricePeakSeason': 135.0}, {'RoomId': '01-051', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 112.5, 'PricePeakSeason': 202.5}, {'RoomId': '01-052', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 126.0, 'PricePeakSeason': 226.8}, {'RoomId': '01-053', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 168.75, 'PricePeakSeason': 303.75}, {'RoomId': '01-054', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 168.75, 'PricePeakSeason': 303.75}, {'RoomId': '01-055', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 283.5, 'PricePeakSeason': 510.3}, {'RoomId': '01-056', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 75.0, 'PricePeakSeason': 135.0}, {'RoomId': '01-057', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 50.0, 'PricePeakSeason': 90.0}, {'RoomId': '01-058', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 168.75, 'PricePeakSeason': 303.75}, {'RoomId': '01-059', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 75.0, 'PricePeakSeason': 135.0}, {'RoomId': '01-060', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 112.5, 'PricePeakSeason': 202.5}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2186</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Sapphire Coast</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>{'Country': 'France', 'City': 'Nice', 'ZipCode': '86664', 'Address': '3534 Anderson Rue Suite 751'}</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>{'OccupancyPeakSeasonWeight': 92, 'OccupancyOffSeasonWeight': 37, 'OccupancyBaseDiscountPercentage': 20, 'ExtraBedChargePercentage': 30, 'MealPlanWeights': {'room_only': {'name': 'Room Only', 'weight': 0.1}, 'room_and_breakfast': {'name': 'Room and Breakfast', 'weight': 0.43}, 'all_inclusive': {'name': 'All Inclusive', 'weight': 0.07}, 'half_board': {'name': 'Half Board', 'weight': 0.24}, 'full_board': {'name': 'Full Board', 'weight': 0.16}}, 'MealPlanPrices': {'Room Only': 1.0, 'Room and Breakfast': 1.13, 'All Inclusive': 2.17, 'Half Board': 1.43, 'Full Board': 1.7}, 'PromotionPriceDiscount': 12}</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>[{'RoomId': '01-001', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 112.5, 'PricePeakSeason': 183.38}, {'RoomId': '01-002', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 112.5, 'PricePeakSeason': 183.38}, {'RoomId': '01-003', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 196.88, 'PricePeakSeason': 320.91}, {'RoomId': '01-004', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 196.88, 'PricePeakSeason': 320.91}, {'RoomId': '01-005', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 196.88, 'PricePeakSeason': 320.91}, {'RoomId': '01-006', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 112.5, 'PricePeakSeason': 183.38}, {'RoomId': '01-007', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 112.5, 'PricePeakSeason': 183.38}, {'RoomId': '01-008', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 112.5, 'PricePeakSeason': 183.38}, {'RoomId': '01-009', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 295.31, 'PricePeakSeason': 481.36}, {'RoomId': '01-010', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 168.75, 'PricePeakSeason': 275.06}, {'RoomId': '01-011', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 196.88, 'PricePeakSeason': 320.91}, {'RoomId': '01-012', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 75.0, 'PricePeakSeason': 122.25}, {'RoomId': '01-013', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 75.0, 'PricePeakSeason': 122.25}, {'RoomId': '01-014', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 131.25, 'PricePeakSeason': 213.94}, {'RoomId': '01-015', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 112.5, 'PricePeakSeason': 183.38}, {'RoomId': '01-016', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 196.88, 'PricePeakSeason': 320.91}, {'RoomId': '01-017', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 112.5, 'PricePeakSeason': 183.38}, {'RoomId': '01-018', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 168.75, 'PricePeakSeason': 275.06}, {'RoomId': '01-019', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 168.75, 'PricePeakSeason': 275.06}, {'RoomId': '01-020', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 295.31, 'PricePeakSeason': 481.36}, {'RoomId': '01-021', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 196.88, 'PricePeakSeason': 320.91}, {'RoomId': '01-022', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 168.75, 'PricePeakSeason': 275.06}, {'RoomId': '01-023', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 196.88, 'PricePeakSeason': 320.91}, {'RoomId': '02-001', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 168.75, 'PricePeakSeason': 275.06}, {'RoomId': '02-002', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 168.75, 'PricePeakSeason': 275.06}, {'RoomId': '02-003', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 196.88, 'PricePeakSeason': 320.91}, {'RoomId': '02-004', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 75.0, 'PricePeakSeason': 122.25}, {'RoomId': '02-005', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 112.5, 'PricePeakSeason': 183.38}, {'RoomId': '02-006', 'Floor': '02', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 295.31, 'PricePeakSeason': 481.36}, {'RoomId': '02-007', 'Floor': '02', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 295.31, 'PricePeakSeason': 481.36}, {'RoomId': '02-008', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 196.88, 'PricePeakSeason': 320.91}, {'RoomId': '02-009', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 196.88, 'PricePeakSeason': 320.91}, {'RoomId': '02-010', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 168.75, 'PricePeakSeason': 275.06}, {'RoomId': '02-011', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 196.88, 'PricePeakSeason': 320.91}, {'RoomId': '02-012', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 112.5, 'PricePeakSeason': 183.38}, {'RoomId': '02-013', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 75.0, 'PricePeakSeason': 122.25}, {'RoomId': '02-014', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 112.5, 'PricePeakSeason': 183.38}, {'RoomId': '02-015', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 112.5, 'PricePeakSeason': 183.38}, {'RoomId': '02-016', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 112.5, 'PricePeakSeason': 183.38}, {'RoomId': '02-017', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 112.5, 'PricePeakSeason': 183.38}, {'RoomId': '02-018', 'Floor': '02', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 131.25, 'PricePeakSeason': 213.94}, {'RoomId': '02-019', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 112.5, 'PricePeakSeason': 183.38}, {'RoomId': '02-020', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 168.75, 'PricePeakSeason': 275.06}, {'RoomId': '02-021', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 112.5, 'PricePeakSeason': 183.38}, {'RoomId': '02-022', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 112.5, 'PricePeakSeason': 183.38}, {'RoomId': '02-023', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 168.75, 'PricePeakSeason': 275.06}, {'RoomId': '03-001', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 112.5, 'PricePeakSeason': 183.38}, {'RoomId': '03-002', 'Floor': '03', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 75.0, 'PricePeakSeason': 122.25}, {'RoomId': '03-003', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 112.5, 'PricePeakSeason': 183.38}, {'RoomId': '03-004', 'Floor': '03', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 75.0, 'PricePeakSeason': 122.25}, {'RoomId': '03-005', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 112.5, 'PricePeakSeason': 183.38}, {'RoomId': '03-006', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 112.5, 'PricePeakSeason': 183.38}, {'RoomId': '03-007', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 112.5, 'PricePeakSeason': 183.38}, {'RoomId': '03-008', 'Floor': '03', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 168.75, 'PricePeakSeason': 275.06}, {'RoomId': '03-009', 'Floor': '03', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 295.31, 'PricePeakSeason': 481.36}, {'RoomId': '03-010', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 112.5, 'PricePeakSeason': 183.38}, {'RoomId': '03-011', 'Floor': '03', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 168.75, 'PricePeakSeason': 275.06}, {'RoomId': '03-012', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 112.5, 'PricePeakSeason': 183.38}, {'RoomId': '03-013', 'Floor': '03', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 196.88, 'PricePeakSeason': 320.91}, {'RoomId': '03-014', 'Floor': '03', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 168.75, 'PricePeakSeason': 275.06}, {'RoomId': '03-015', 'Floor': '03', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 196.88, 'PricePeakSeason': 320.91}, {'RoomId': '03-016', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 112.5, 'PricePeakSeason': 183.38}, {'RoomId': '03-017', 'Floor': '03', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 295.31, 'PricePeakSeason': 481.36}, {'RoomId': '03-018', 'Floor': '03', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 168.75, 'PricePeakSeason': 275.06}, {'RoomId': '03-019', 'Floor': '03', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 75.0, 'PricePeakSeason': 122.25}, {'RoomId': '03-020', 'Floor': '03', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 131.25, 'PricePeakSeason': 213.94}, {'RoomId': '03-021', 'Floor': '03', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 168.75, 'PricePeakSeason': 275.06}, {'RoomId': '03-022', 'Floor': '03', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 168.75, 'PricePeakSeason': 275.06}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2520</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Golden Peak</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>{'Country': 'France', 'City': 'Nice', 'ZipCode': '01721', 'Address': '911 William Curve Suite 135'}</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>{'OccupancyPeakSeasonWeight': 95, 'OccupancyOffSeasonWeight': 30, 'OccupancyBaseDiscountPercentage': 21, 'ExtraBedChargePercentage': 28, 'MealPlanWeights': {'room_only': {'name': 'Room Only', 'weight': 0.15}, 'room_and_breakfast': {'name': 'Room and Breakfast', 'weight': 0.37}, 'all_inclusive': {'name': 'All Inclusive', 'weight': 0.07}, 'half_board': {'name': 'Half Board', 'weight': 0.21}, 'full_board': {'name': 'Full Board', 'weight': 0.2}}, 'MealPlanPrices': {'Room Only': 1.0, 'Room and Breakfast': 1.2, 'All Inclusive': 2.12, 'Half Board': 1.41, 'Full Board': 1.68}, 'PromotionPriceDiscount': 30}</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>[{'RoomId': '01-001', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 198.36}, {'RoomId': '01-002', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 198.36}, {'RoomId': '01-003', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 76.0, 'PricePeakSeason': 132.24}, {'RoomId': '01-004', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 76.0, 'PricePeakSeason': 132.24}, {'RoomId': '01-005', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 76.0, 'PricePeakSeason': 132.24}, {'RoomId': '01-006', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 198.36}, {'RoomId': '01-007', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 198.36}, {'RoomId': '01-008', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 198.36}, {'RoomId': '01-009', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 171.0, 'PricePeakSeason': 297.54}, {'RoomId': '01-010', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 198.36}, {'RoomId': '01-011', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 76.0, 'PricePeakSeason': 132.24}, {'RoomId': '01-012', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 198.36}, {'RoomId': '01-013', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 171.0, 'PricePeakSeason': 297.54}, {'RoomId': '01-014', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 198.36}, {'RoomId': '01-015', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 171.0, 'PricePeakSeason': 297.54}, {'RoomId': '01-016', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 345.42, 'PricePeakSeason': 601.03}, {'RoomId': '01-017', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 171.0, 'PricePeakSeason': 297.54}, {'RoomId': '01-018', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 171.0, 'PricePeakSeason': 297.54}, {'RoomId': '01-019', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 76.0, 'PricePeakSeason': 132.24}, {'RoomId': '01-020', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 198.36}, {'RoomId': '01-021', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 76.0, 'PricePeakSeason': 132.24}, {'RoomId': '01-022', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 198.36}, {'RoomId': '01-023', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 76.0, 'PricePeakSeason': 132.24}, {'RoomId': '01-024', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 345.42, 'PricePeakSeason': 601.03}, {'RoomId': '01-025', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 76.0, 'PricePeakSeason': 132.24}, {'RoomId': '01-026', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 198.36}, {'RoomId': '01-027', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 198.36}, {'RoomId': '01-028', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 76.0, 'PricePeakSeason': 132.24}, {'RoomId': '01-029', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 171.0, 'PricePeakSeason': 297.54}, {'RoomId': '01-030', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 198.36}, {'RoomId': '01-031', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 198.36}, {'RoomId': '01-032', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 76.0, 'PricePeakSeason': 132.24}, {'RoomId': '01-033', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 171.0, 'PricePeakSeason': 297.54}, {'RoomId': '01-034', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 198.36}, {'RoomId': '01-035', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 198.36}, {'RoomId': '01-036', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 76.0, 'PricePeakSeason': 132.24}, {'RoomId': '01-037', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 198.36}, {'RoomId': '01-038', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 198.36}, {'RoomId': '01-039', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 198.36}, {'RoomId': '01-040', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 171.0, 'PricePeakSeason': 297.54}, {'RoomId': '01-041', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 198.36}, {'RoomId': '01-042', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 198.36}, {'RoomId': '01-043', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 198.36}, {'RoomId': '01-044', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 198.36}, {'RoomId': '01-045', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 198.36}, {'RoomId': '01-046', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 198.36}, {'RoomId': '01-047', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 76.0, 'PricePeakSeason': 132.24}, {'RoomId': '01-048', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 76.0, 'PricePeakSeason': 132.24}, {'RoomId': '01-049', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 198.36}, {'RoomId': '01-050', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 153.52, 'PricePeakSeason': 267.12}, {'RoomId': '01-051', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 198.36}, {'RoomId': '01-052', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 171.0, 'PricePeakSeason': 297.54}, {'RoomId': '01-053', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 198.36}, {'RoomId': '01-054', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 198.36}, {'RoomId': '01-055', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 76.0, 'PricePeakSeason': 132.24}, {'RoomId': '01-056', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 198.36}, {'RoomId': '01-057', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 230.28, 'PricePeakSeason': 400.69}, {'RoomId': '01-058', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 76.0, 'PricePeakSeason': 132.24}, {'RoomId': '01-059', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 171.0, 'PricePeakSeason': 297.54}, {'RoomId': '01-060', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 171.0, 'PricePeakSeason': 297.54}, {'RoomId': '01-061', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 198.36}, {'RoomId': '01-062', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 198.36}, {'RoomId': '01-063', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 198.36}, {'RoomId': '01-064', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 345.42, 'PricePeakSeason': 601.03}, {'RoomId': '01-065', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 198.36}, {'RoomId': '01-066', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 76.0, 'PricePeakSeason': 132.24}, {'RoomId': '01-067', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 198.36}, {'RoomId': '01-068', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 76.0, 'PricePeakSeason': 132.24}, {'RoomId': '01-069', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 171.0, 'PricePeakSeason': 297.54}, {'RoomId': '01-070', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 198.36}, {'RoomId': '01-071', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 198.36}, {'RoomId': '01-072', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 198.36}, {'RoomId': '01-073', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 198.36}, {'RoomId': '01-074', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 171.0, 'PricePeakSeason': 297.54}, {'RoomId': '01-075', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 153.52, 'PricePeakSeason': 267.12}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>1276</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Silver Stream</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>{'Country': 'France', 'City': 'Nice', 'ZipCode': '37854', 'Address': '8498 Elizabeth Plaza'}</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>{'OccupancyPeakSeasonWeight': 84, 'OccupancyOffSeasonWeight': 39, 'OccupancyBaseDiscountPercentage': 28, 'ExtraBedChargePercentage': 26, 'MealPlanWeights': {'room_only': {'name': 'Room Only', 'weight': 0.16}, 'room_and_breakfast': {'name': 'Room and Breakfast', 'weight': 0.38}, 'all_inclusive': {'name': 'All Inclusive', 'weight': 0.09}, 'half_board': {'name': 'Half Board', 'weight': 0.12}, 'full_board': {'name': 'Full Board', 'weight': 0.25}}, 'MealPlanPrices': {'Room Only': 1.0, 'Room and Breakfast': 1.16, 'All Inclusive': 2.2, 'Half Board': 1.36, 'Full Board': 1.6}, 'PromotionPriceDiscount': 23}</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>[{'RoomId': '01-001', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 78.0, 'PricePeakSeason': 138.84}, {'RoomId': '01-002', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 130.26, 'PricePeakSeason': 231.86}, {'RoomId': '01-003', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 117.0, 'PricePeakSeason': 208.26}, {'RoomId': '01-004', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 130.26, 'PricePeakSeason': 231.86}, {'RoomId': '01-005', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 175.5, 'PricePeakSeason': 312.39}, {'RoomId': '01-006', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 195.39, 'PricePeakSeason': 347.79}, {'RoomId': '01-007', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 78.0, 'PricePeakSeason': 138.84}, {'RoomId': '01-008', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 175.5, 'PricePeakSeason': 312.39}, {'RoomId': '01-009', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 78.0, 'PricePeakSeason': 138.84}, {'RoomId': '01-010', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 78.0, 'PricePeakSeason': 138.84}, {'RoomId': '01-011', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 130.26, 'PricePeakSeason': 231.86}, {'RoomId': '01-012', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 78.0, 'PricePeakSeason': 138.84}, {'RoomId': '01-013', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 78.0, 'PricePeakSeason': 138.84}, {'RoomId': '01-014', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 195.39, 'PricePeakSeason': 347.79}, {'RoomId': '01-015', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 78.0, 'PricePeakSeason': 138.84}, {'RoomId': '01-016', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 195.39, 'PricePeakSeason': 347.79}, {'RoomId': '01-017', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 78.0, 'PricePeakSeason': 138.84}, {'RoomId': '01-018', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 175.5, 'PricePeakSeason': 312.39}, {'RoomId': '01-019', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 130.26, 'PricePeakSeason': 231.86}, {'RoomId': '01-020', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 195.39, 'PricePeakSeason': 347.79}, {'RoomId': '01-021', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 293.08, 'PricePeakSeason': 521.68}, {'RoomId': '01-022', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 117.0, 'PricePeakSeason': 208.26}, {'RoomId': '02-001', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 117.0, 'PricePeakSeason': 208.26}, {'RoomId': '02-002', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 117.0, 'PricePeakSeason': 208.26}, {'RoomId': '02-003', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 78.0, 'PricePeakSeason': 138.84}, {'RoomId': '02-004', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 78.0, 'PricePeakSeason': 138.84}, {'RoomId': '02-005', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 175.5, 'PricePeakSeason': 312.39}, {'RoomId': '02-006', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 117.0, 'PricePeakSeason': 208.26}, {'RoomId': '02-007', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 78.0, 'PricePeakSeason': 138.84}, {'RoomId': '02-008', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 117.0, 'PricePeakSeason': 208.26}, {'RoomId': '02-009', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 175.5, 'PricePeakSeason': 312.39}, {'RoomId': '02-010', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 78.0, 'PricePeakSeason': 138.84}, {'RoomId': '02-011', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 78.0, 'PricePeakSeason': 138.84}, {'RoomId': '02-012', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 175.5, 'PricePeakSeason': 312.39}, {'RoomId': '02-013', 'Floor': '02', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 293.08, 'PricePeakSeason': 521.68}, {'RoomId': '02-014', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 195.39, 'PricePeakSeason': 347.79}, {'RoomId': '02-015', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 78.0, 'PricePeakSeason': 138.84}, {'RoomId': '02-016', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 78.0, 'PricePeakSeason': 138.84}, {'RoomId': '02-017', 'Floor': '02', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 293.08, 'PricePeakSeason': 521.68}, {'RoomId': '02-018', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 117.0, 'PricePeakSeason': 208.26}, {'RoomId': '02-019', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 195.39, 'PricePeakSeason': 347.79}, {'RoomId': '02-020', 'Floor': '02', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 130.26, 'PricePeakSeason': 231.86}, {'RoomId': '02-021', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 117.0, 'PricePeakSeason': 208.26}, {'RoomId': '02-022', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 175.5, 'PricePeakSeason': 312.39}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>5936</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Diamond Falls</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>{'Country': 'France', 'City': 'Paris', 'ZipCode': '39741', 'Address': '41182 Campbell Fords'}</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>{'OccupancyPeakSeasonWeight': 86, 'OccupancyOffSeasonWeight': 26, 'OccupancyBaseDiscountPercentage': 29, 'ExtraBedChargePercentage': 24, 'MealPlanWeights': {'room_only': {'name': 'Room Only', 'weight': 0.11}, 'room_and_breakfast': {'name': 'Room and Breakfast', 'weight': 0.47000000000000003}, 'all_inclusive': {'name': 'All Inclusive', 'weight': 0.08}, 'half_board': {'name': 'Half Board', 'weight': 0.12}, 'full_board': {'name': 'Full Board', 'weight': 0.22}}, 'MealPlanPrices': {'Room Only': 1.0, 'Room and Breakfast': 1.13, 'All Inclusive': 2.08, 'Half Board': 1.36, 'Full Board': 1.57}, 'PromotionPriceDiscount': 16}</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>[{'RoomId': '01-001', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 151.59}, {'RoomId': '01-002', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 151.59}, {'RoomId': '01-003', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 151.59}, {'RoomId': '01-004', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 151.59}, {'RoomId': '01-005', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 151.59}, {'RoomId': '01-006', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 228.78, 'PricePeakSeason': 372.91}, {'RoomId': '01-007', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 228.78, 'PricePeakSeason': 372.91}, {'RoomId': '01-008', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 57.0, 'PricePeakSeason': 92.91}, {'RoomId': '01-009', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 151.59}, {'RoomId': '01-010', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 151.59}, {'RoomId': '01-011', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 151.59}, {'RoomId': '01-012', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 139.5, 'PricePeakSeason': 227.38}, {'RoomId': '01-013', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 57.0, 'PricePeakSeason': 92.91}, {'RoomId': '01-014', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 139.5, 'PricePeakSeason': 227.38}, {'RoomId': '01-015', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 57.0, 'PricePeakSeason': 92.91}, {'RoomId': '01-016', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 57.0, 'PricePeakSeason': 92.91}, {'RoomId': '01-017', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 151.59}, {'RoomId': '01-018', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 228.78, 'PricePeakSeason': 372.91}, {'RoomId': '01-019', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 151.59}, {'RoomId': '01-020', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 139.5, 'PricePeakSeason': 227.38}, {'RoomId': '01-021', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 228.78, 'PricePeakSeason': 372.91}, {'RoomId': '01-022', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 57.0, 'PricePeakSeason': 92.91}, {'RoomId': '01-023', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 139.5, 'PricePeakSeason': 227.38}, {'RoomId': '01-024', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 57.0, 'PricePeakSeason': 92.91}, {'RoomId': '01-025', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 151.59}, {'RoomId': '01-026', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 57.0, 'PricePeakSeason': 92.91}, {'RoomId': '01-027', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 151.59}, {'RoomId': '01-028', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 57.0, 'PricePeakSeason': 92.91}, {'RoomId': '01-029', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 228.78, 'PricePeakSeason': 372.91}, {'RoomId': '02-001', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 151.59}, {'RoomId': '02-002', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 151.59}, {'RoomId': '02-003', 'Floor': '02', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 140.22, 'PricePeakSeason': 228.56}, {'RoomId': '02-004', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 151.59}, {'RoomId': '02-005', 'Floor': '02', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 343.17, 'PricePeakSeason': 559.37}, {'RoomId': '02-006', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 139.5, 'PricePeakSeason': 227.38}, {'RoomId': '02-007', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 151.59}, {'RoomId': '02-008', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 139.5, 'PricePeakSeason': 227.38}, {'RoomId': '02-009', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 151.59}, {'RoomId': '02-010', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 57.0, 'PricePeakSeason': 92.91}, {'RoomId': '02-011', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 151.59}, {'RoomId': '02-012', 'Floor': '02', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 343.17, 'PricePeakSeason': 559.37}, {'RoomId': '02-013', 'Floor': '02', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 343.17, 'PricePeakSeason': 559.37}, {'RoomId': '02-014', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 228.78, 'PricePeakSeason': 372.91}, {'RoomId': '02-015', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 139.5, 'PricePeakSeason': 227.38}, {'RoomId': '02-016', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 151.59}, {'RoomId': '02-017', 'Floor': '02', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 343.17, 'PricePeakSeason': 559.37}, {'RoomId': '02-018', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 151.59}, {'RoomId': '02-019', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 57.0, 'PricePeakSeason': 92.91}, {'RoomId': '02-020', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 57.0, 'PricePeakSeason': 92.91}, {'RoomId': '02-021', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 139.5, 'PricePeakSeason': 227.38}, {'RoomId': '02-022', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 151.59}, {'RoomId': '02-023', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 139.5, 'PricePeakSeason': 227.38}, {'RoomId': '02-024', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 57.0, 'PricePeakSeason': 92.91}, {'RoomId': '02-025', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 228.78, 'PricePeakSeason': 372.91}, {'RoomId': '02-026', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 151.59}, {'RoomId': '02-027', 'Floor': '02', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 140.22, 'PricePeakSeason': 228.56}, {'RoomId': '02-028', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 228.78, 'PricePeakSeason': 372.91}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>4092</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Crystal Bay</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>{'Country': 'France', 'City': 'Paris', 'ZipCode': '94559', 'Address': '48740 Cynthia Village Suite 005'}</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>{'OccupancyPeakSeasonWeight': 90, 'OccupancyOffSeasonWeight': 37, 'OccupancyBaseDiscountPercentage': 23, 'ExtraBedChargePercentage': 21, 'MealPlanWeights': {'room_only': {'name': 'Room Only', 'weight': 0.17}, 'room_and_breakfast': {'name': 'Room and Breakfast', 'weight': 0.48}, 'all_inclusive': {'name': 'All Inclusive', 'weight': 0.04}, 'half_board': {'name': 'Half Board', 'weight': 0.19}, 'full_board': {'name': 'Full Board', 'weight': 0.12}}, 'MealPlanPrices': {'Room Only': 1.0, 'Room and Breakfast': 1.15, 'All Inclusive': 2.09, 'Half Board': 1.45, 'Full Board': 1.67}, 'PromotionPriceDiscount': 10}</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>[{'RoomId': '01-001', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 166.5, 'PricePeakSeason': 314.69}, {'RoomId': '01-002', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 218.67, 'PricePeakSeason': 413.29}, {'RoomId': '01-003', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 74.0, 'PricePeakSeason': 139.86}, {'RoomId': '01-004', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 218.67, 'PricePeakSeason': 413.29}, {'RoomId': '01-005', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 111.0, 'PricePeakSeason': 209.79}, {'RoomId': '01-006', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 111.0, 'PricePeakSeason': 209.79}, {'RoomId': '01-007', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 166.5, 'PricePeakSeason': 314.69}, {'RoomId': '01-008', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 111.0, 'PricePeakSeason': 209.79}, {'RoomId': '01-009', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 218.67, 'PricePeakSeason': 413.29}, {'RoomId': '01-010', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 74.0, 'PricePeakSeason': 139.86}, {'RoomId': '01-011', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 111.0, 'PricePeakSeason': 209.79}, {'RoomId': '01-012', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 111.0, 'PricePeakSeason': 209.79}, {'RoomId': '01-013', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 74.0, 'PricePeakSeason': 139.86}, {'RoomId': '01-014', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 166.5, 'PricePeakSeason': 314.69}, {'RoomId': '01-015', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 111.0, 'PricePeakSeason': 209.79}, {'RoomId': '01-016', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 166.5, 'PricePeakSeason': 314.69}, {'RoomId': '01-017', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 74.0, 'PricePeakSeason': 139.86}, {'RoomId': '01-018', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 111.0, 'PricePeakSeason': 209.79}, {'RoomId': '01-019', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 218.67, 'PricePeakSeason': 413.29}, {'RoomId': '01-020', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 111.0, 'PricePeakSeason': 209.79}, {'RoomId': '01-021', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 166.5, 'PricePeakSeason': 314.69}, {'RoomId': '01-022', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 328.0, 'PricePeakSeason': 619.92}, {'RoomId': '01-023', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 328.0, 'PricePeakSeason': 619.92}, {'RoomId': '01-024', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 166.5, 'PricePeakSeason': 314.69}, {'RoomId': '01-025', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 166.5, 'PricePeakSeason': 314.69}, {'RoomId': '01-026', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 218.67, 'PricePeakSeason': 413.29}, {'RoomId': '01-027', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 111.0, 'PricePeakSeason': 209.79}, {'RoomId': '01-028', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 166.5, 'PricePeakSeason': 314.69}, {'RoomId': '01-029', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 111.0, 'PricePeakSeason': 209.79}, {'RoomId': '01-030', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 111.0, 'PricePeakSeason': 209.79}, {'RoomId': '01-031', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 166.5, 'PricePeakSeason': 314.69}, {'RoomId': '01-032', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 74.0, 'PricePeakSeason': 139.86}, {'RoomId': '01-033', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 74.0, 'PricePeakSeason': 139.86}, {'RoomId': '01-034', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 166.5, 'PricePeakSeason': 314.69}, {'RoomId': '01-035', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 111.0, 'PricePeakSeason': 209.79}, {'RoomId': '01-036', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 111.0, 'PricePeakSeason': 209.79}, {'RoomId': '01-037', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 166.5, 'PricePeakSeason': 314.69}, {'RoomId': '01-038', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 111.0, 'PricePeakSeason': 209.79}, {'RoomId': '01-039', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 111.0, 'PricePeakSeason': 209.79}, {'RoomId': '01-040', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 111.0, 'PricePeakSeason': 209.79}, {'RoomId': '01-041', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 111.0, 'PricePeakSeason': 209.79}, {'RoomId': '01-042', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 218.67, 'PricePeakSeason': 413.29}, {'RoomId': '01-043', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 111.0, 'PricePeakSeason': 209.79}, {'RoomId': '01-044', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 218.67, 'PricePeakSeason': 413.29}, {'RoomId': '01-045', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 111.0, 'PricePeakSeason': 209.79}, {'RoomId': '01-046', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 166.5, 'PricePeakSeason': 314.69}, {'RoomId': '01-047', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 218.67, 'PricePeakSeason': 413.29}, {'RoomId': '01-048', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 218.67, 'PricePeakSeason': 413.29}, {'RoomId': '01-049', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 111.0, 'PricePeakSeason': 209.79}, {'RoomId': '01-050', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 145.78, 'PricePeakSeason': 275.52}, {'RoomId': '01-051', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 111.0, 'PricePeakSeason': 209.79}, {'RoomId': '01-052', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 111.0, 'PricePeakSeason': 209.79}, {'RoomId': '01-053', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 111.0, 'PricePeakSeason': 209.79}, {'RoomId': '01-054', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 218.67, 'PricePeakSeason': 413.29}, {'RoomId': '01-055', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 218.67, 'PricePeakSeason': 413.29}, {'RoomId': '01-056', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 111.0, 'PricePeakSeason': 209.79}, {'RoomId': '01-057', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 166.5, 'PricePeakSeason': 314.69}, {'RoomId': '01-058', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 74.0, 'PricePeakSeason': 139.86}, {'RoomId': '01-059', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 111.0, 'PricePeakSeason': 209.79}, {'RoomId': '01-060', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 145.78, 'PricePeakSeason': 275.52}, {'RoomId': '01-061', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 74.0, 'PricePeakSeason': 139.86}, {'RoomId': '01-062', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 218.67, 'PricePeakSeason': 413.29}, {'RoomId': '01-063', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 111.0, 'PricePeakSeason': 209.79}, {'RoomId': '01-064', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 166.5, 'PricePeakSeason': 314.69}, {'RoomId': '01-065', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 111.0, 'PricePeakSeason': 209.79}, {'RoomId': '01-066', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 166.5, 'PricePeakSeason': 314.69}, {'RoomId': '01-067', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 74.0, 'PricePeakSeason': 139.86}, {'RoomId': '01-068', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 218.67, 'PricePeakSeason': 413.29}, {'RoomId': '01-069', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 111.0, 'PricePeakSeason': 209.79}, {'RoomId': '01-070', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 74.0, 'PricePeakSeason': 139.86}, {'RoomId': '01-071', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 166.5, 'PricePeakSeason': 314.69}, {'RoomId': '01-072', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 218.67, 'PricePeakSeason': 413.29}, {'RoomId': '01-073', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 328.0, 'PricePeakSeason': 619.92}, {'RoomId': '01-074', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 74.0, 'PricePeakSeason': 139.86}, {'RoomId': '01-075', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 218.67, 'PricePeakSeason': 413.29}, {'RoomId': '01-076', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 111.0, 'PricePeakSeason': 209.79}, {'RoomId': '01-077', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 328.0, 'PricePeakSeason': 619.92}, {'RoomId': '01-078', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 111.0, 'PricePeakSeason': 209.79}, {'RoomId': '01-079', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 166.5, 'PricePeakSeason': 314.69}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>8060</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Ivory Dunes</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>{'Country': 'France', 'City': 'Nice', 'ZipCode': '17647', 'Address': '78680 Charles Spurs Apt. 805'}</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>{'OccupancyPeakSeasonWeight': 96, 'OccupancyOffSeasonWeight': 26, 'OccupancyBaseDiscountPercentage': 27, 'ExtraBedChargePercentage': 26, 'MealPlanWeights': {'room_only': {'name': 'Room Only', 'weight': 0.18}, 'room_and_breakfast': {'name': 'Room and Breakfast', 'weight': 0.42}, 'all_inclusive': {'name': 'All Inclusive', 'weight': 0.03}, 'half_board': {'name': 'Half Board', 'weight': 0.25}, 'full_board': {'name': 'Full Board', 'weight': 0.12}}, 'MealPlanPrices': {'Room Only': 1.0, 'Room and Breakfast': 1.14, 'All Inclusive': 2.15, 'Half Board': 1.5, 'Full Board': 1.59}, 'PromotionPriceDiscount': 16}</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>[{'RoomId': '01-001', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 112.5, 'PricePeakSeason': 180.0}, {'RoomId': '01-002', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 135.75, 'PricePeakSeason': 217.2}, {'RoomId': '01-003', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 112.5, 'PricePeakSeason': 180.0}, {'RoomId': '01-004', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 112.5, 'PricePeakSeason': 180.0}, {'RoomId': '01-005', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 112.5, 'PricePeakSeason': 180.0}, {'RoomId': '01-006', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 112.5, 'PricePeakSeason': 180.0}, {'RoomId': '01-007', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 112.5, 'PricePeakSeason': 180.0}, {'RoomId': '01-008', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 75.0, 'PricePeakSeason': 120.0}, {'RoomId': '01-009', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 75.0, 'PricePeakSeason': 120.0}, {'RoomId': '01-010', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 112.5, 'PricePeakSeason': 180.0}, {'RoomId': '02-001', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 112.5, 'PricePeakSeason': 180.0}, {'RoomId': '02-002', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 75.0, 'PricePeakSeason': 120.0}, {'RoomId': '02-003', 'Floor': '02', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 135.75, 'PricePeakSeason': 217.2}, {'RoomId': '02-004', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 203.62, 'PricePeakSeason': 325.79}, {'RoomId': '02-005', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 112.5, 'PricePeakSeason': 180.0}, {'RoomId': '02-006', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 75.0, 'PricePeakSeason': 120.0}, {'RoomId': '02-007', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 75.0, 'PricePeakSeason': 120.0}, {'RoomId': '02-008', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 112.5, 'PricePeakSeason': 180.0}, {'RoomId': '02-009', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 112.5, 'PricePeakSeason': 180.0}, {'RoomId': '02-010', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 75.0, 'PricePeakSeason': 120.0}, {'RoomId': '03-001', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 112.5, 'PricePeakSeason': 180.0}, {'RoomId': '03-002', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 112.5, 'PricePeakSeason': 180.0}, {'RoomId': '03-003', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 112.5, 'PricePeakSeason': 180.0}, {'RoomId': '03-004', 'Floor': '03', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 168.75, 'PricePeakSeason': 270.0}, {'RoomId': '03-005', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 112.5, 'PricePeakSeason': 180.0}, {'RoomId': '03-006', 'Floor': '03', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 168.75, 'PricePeakSeason': 270.0}, {'RoomId': '03-007', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 112.5, 'PricePeakSeason': 180.0}, {'RoomId': '03-008', 'Floor': '03', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 135.75, 'PricePeakSeason': 217.2}, {'RoomId': '03-009', 'Floor': '03', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 135.75, 'PricePeakSeason': 217.2}, {'RoomId': '03-010', 'Floor': '03', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 75.0, 'PricePeakSeason': 120.0}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>5906</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Onyx Cliffs</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>{'Country': 'France', 'City': 'Cannes', 'ZipCode': '76851', 'Address': '2045 Rachel Fords'}</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>{'OccupancyPeakSeasonWeight': 89, 'OccupancyOffSeasonWeight': 40, 'OccupancyBaseDiscountPercentage': 20, 'ExtraBedChargePercentage': 25, 'MealPlanWeights': {'room_only': {'name': 'Room Only', 'weight': 0.13}, 'room_and_breakfast': {'name': 'Room and Breakfast', 'weight': 0.5}, 'all_inclusive': {'name': 'All Inclusive', 'weight': 0.03}, 'half_board': {'name': 'Half Board', 'weight': 0.14}, 'full_board': {'name': 'Full Board', 'weight': 0.2}}, 'MealPlanPrices': {'Room Only': 1.0, 'Room and Breakfast': 1.18, 'All Inclusive': 2.01, 'Half Board': 1.32, 'Full Board': 1.59}, 'PromotionPriceDiscount': 12}</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>[{'RoomId': '01-001', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 135.75, 'PricePeakSeason': 203.62}, {'RoomId': '01-002', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 75.0, 'PricePeakSeason': 112.5}, {'RoomId': '01-003', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 150.0, 'PricePeakSeason': 225.0}, {'RoomId': '01-004', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 75.0, 'PricePeakSeason': 112.5}, {'RoomId': '01-005', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 75.0, 'PricePeakSeason': 112.5}, {'RoomId': '01-006', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 271.5, 'PricePeakSeason': 407.25}, {'RoomId': '01-007', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 75.0, 'PricePeakSeason': 112.5}, {'RoomId': '01-008', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 75.0, 'PricePeakSeason': 112.5}, {'RoomId': '01-009', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 75.0, 'PricePeakSeason': 112.5}, {'RoomId': '01-010', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 75.0, 'PricePeakSeason': 112.5}, {'RoomId': '01-011', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 75.0, 'PricePeakSeason': 112.5}, {'RoomId': '01-012', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 135.75, 'PricePeakSeason': 203.62}, {'RoomId': '01-013', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 75.0, 'PricePeakSeason': 112.5}, {'RoomId': '01-014', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 135.75, 'PricePeakSeason': 203.62}, {'RoomId': '01-015', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 75.0, 'PricePeakSeason': 112.5}, {'RoomId': '02-001', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 75.0, 'PricePeakSeason': 112.5}, {'RoomId': '02-002', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 75.0, 'PricePeakSeason': 112.5}, {'RoomId': '02-003', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 75.0, 'PricePeakSeason': 112.5}, {'RoomId': '02-004', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 150.0, 'PricePeakSeason': 225.0}, {'RoomId': '02-005', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 150.0, 'PricePeakSeason': 225.0}, {'RoomId': '02-006', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 75.0, 'PricePeakSeason': 112.5}, {'RoomId': '02-007', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 150.0, 'PricePeakSeason': 225.0}, {'RoomId': '02-008', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 75.0, 'PricePeakSeason': 112.5}, {'RoomId': '02-009', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 135.75, 'PricePeakSeason': 203.62}, {'RoomId': '02-010', 'Floor': '02', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 271.5, 'PricePeakSeason': 407.25}, {'RoomId': '02-011', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 75.0, 'PricePeakSeason': 112.5}, {'RoomId': '02-012', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 75.0, 'PricePeakSeason': 112.5}, {'RoomId': '02-013', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 150.0, 'PricePeakSeason': 225.0}, {'RoomId': '02-014', 'Floor': '02', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 85.07, 'PricePeakSeason': 127.6}, {'RoomId': '03-001', 'Floor': '03', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 150.0, 'PricePeakSeason': 225.0}, {'RoomId': '03-002', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 75.0, 'PricePeakSeason': 112.5}, {'RoomId': '03-003', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 75.0, 'PricePeakSeason': 112.5}, {'RoomId': '03-004', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 75.0, 'PricePeakSeason': 112.5}, {'RoomId': '03-005', 'Floor': '03', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 150.0, 'PricePeakSeason': 225.0}, {'RoomId': '03-006', 'Floor': '03', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 47.0, 'PricePeakSeason': 70.5}, {'RoomId': '03-007', 'Floor': '03', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 47.0, 'PricePeakSeason': 70.5}, {'RoomId': '03-008', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 75.0, 'PricePeakSeason': 112.5}, {'RoomId': '03-009', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 75.0, 'PricePeakSeason': 112.5}, {'RoomId': '03-010', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 75.0, 'PricePeakSeason': 112.5}, {'RoomId': '03-011', 'Floor': '03', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 47.0, 'PricePeakSeason': 70.5}, {'RoomId': '03-012', 'Floor': '03', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 47.0, 'PricePeakSeason': 70.5}, {'RoomId': '03-013', 'Floor': '03', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 135.75, 'PricePeakSeason': 203.62}, {'RoomId': '03-014', 'Floor': '03', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 271.5, 'PricePeakSeason': 407.25}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>3538</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Amber Forest</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>{'Country': 'France', 'City': 'Paris', 'ZipCode': '89900', 'Address': '158 Dickson Summit'}</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>{'OccupancyPeakSeasonWeight': 92, 'OccupancyOffSeasonWeight': 36, 'OccupancyBaseDiscountPercentage': 24, 'ExtraBedChargePercentage': 28, 'MealPlanWeights': {'room_only': {'name': 'Room Only', 'weight': 0.15}, 'room_and_breakfast': {'name': 'Room and Breakfast', 'weight': 0.5}, 'all_inclusive': {'name': 'All Inclusive', 'weight': 0.01}, 'half_board': {'name': 'Half Board', 'weight': 0.24}, 'full_board': {'name': 'Full Board', 'weight': 0.1}}, 'MealPlanPrices': {'Room Only': 1.0, 'Room and Breakfast': 1.14, 'All Inclusive': 2.05, 'Half Board': 1.31, 'Full Board': 1.59}, 'PromotionPriceDiscount': 16}</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>[{'RoomId': '01-001', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 187.85, 'PricePeakSeason': 330.62}, {'RoomId': '01-002', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 149.6}, {'RoomId': '01-003', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 187.85, 'PricePeakSeason': 330.62}, {'RoomId': '01-004', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 149.6}, {'RoomId': '01-005', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 149.6}, {'RoomId': '01-006', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 149.6}, {'RoomId': '01-007', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 147.0, 'PricePeakSeason': 258.72}, {'RoomId': '01-008', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 187.85, 'PricePeakSeason': 330.62}, {'RoomId': '01-009', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 187.85, 'PricePeakSeason': 330.62}, {'RoomId': '01-010', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 149.6}, {'RoomId': '01-011', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 187.85, 'PricePeakSeason': 330.62}, {'RoomId': '01-012', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 149.6}, {'RoomId': '01-013', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 149.6}, {'RoomId': '01-014', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 187.85, 'PricePeakSeason': 330.62}, {'RoomId': '01-015', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 147.0, 'PricePeakSeason': 258.72}, {'RoomId': '01-016', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 51.0, 'PricePeakSeason': 89.76}, {'RoomId': '01-017', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 51.0, 'PricePeakSeason': 89.76}, {'RoomId': '01-018', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 147.0, 'PricePeakSeason': 258.72}, {'RoomId': '01-019', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 147.0, 'PricePeakSeason': 258.72}, {'RoomId': '01-020', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 149.6}, {'RoomId': '01-021', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 324.87, 'PricePeakSeason': 571.77}, {'RoomId': '01-022', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 324.87, 'PricePeakSeason': 571.77}, {'RoomId': '01-023', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 149.6}, {'RoomId': '01-024', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 51.0, 'PricePeakSeason': 89.76}, {'RoomId': '01-025', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 51.0, 'PricePeakSeason': 89.76}, {'RoomId': '01-026', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 147.0, 'PricePeakSeason': 258.72}, {'RoomId': '01-027', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 149.6}, {'RoomId': '01-028', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 149.6}, {'RoomId': '01-029', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 51.0, 'PricePeakSeason': 89.76}, {'RoomId': '01-030', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 149.6}, {'RoomId': '01-031', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 149.6}, {'RoomId': '01-032', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 187.85, 'PricePeakSeason': 330.62}, {'RoomId': '01-033', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 112.71, 'PricePeakSeason': 198.37}, {'RoomId': '01-034', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 51.0, 'PricePeakSeason': 89.76}, {'RoomId': '01-035', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 187.85, 'PricePeakSeason': 330.62}, {'RoomId': '01-036', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 324.87, 'PricePeakSeason': 571.77}, {'RoomId': '01-037', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 147.0, 'PricePeakSeason': 258.72}, {'RoomId': '01-038', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 147.0, 'PricePeakSeason': 258.72}, {'RoomId': '02-001', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 149.6}, {'RoomId': '02-002', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 187.85, 'PricePeakSeason': 330.62}, {'RoomId': '02-003', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 187.85, 'PricePeakSeason': 330.62}, {'RoomId': '02-004', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 51.0, 'PricePeakSeason': 89.76}, {'RoomId': '02-005', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 149.6}, {'RoomId': '02-006', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 149.6}, {'RoomId': '02-007', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 51.0, 'PricePeakSeason': 89.76}, {'RoomId': '02-008', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 147.0, 'PricePeakSeason': 258.72}, {'RoomId': '02-009', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 187.85, 'PricePeakSeason': 330.62}, {'RoomId': '02-010', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 51.0, 'PricePeakSeason': 89.76}, {'RoomId': '02-011', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 149.6}, {'RoomId': '02-012', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 149.6}, {'RoomId': '02-013', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 149.6}, {'RoomId': '02-014', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 149.6}, {'RoomId': '02-015', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 149.6}, {'RoomId': '02-016', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 149.6}, {'RoomId': '02-017', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 51.0, 'PricePeakSeason': 89.76}, {'RoomId': '02-018', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 149.6}, {'RoomId': '02-019', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 147.0, 'PricePeakSeason': 258.72}, {'RoomId': '02-020', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 149.6}, {'RoomId': '02-021', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 149.6}, {'RoomId': '02-022', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 149.6}, {'RoomId': '02-023', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 149.6}, {'RoomId': '02-024', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 51.0, 'PricePeakSeason': 89.76}, {'RoomId': '02-025', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 149.6}, {'RoomId': '02-026', 'Floor': '02', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 112.71, 'PricePeakSeason': 198.37}, {'RoomId': '02-027', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 149.6}, {'RoomId': '02-028', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 187.85, 'PricePeakSeason': 330.62}, {'RoomId': '02-029', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 147.0, 'PricePeakSeason': 258.72}, {'RoomId': '02-030', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 149.6}, {'RoomId': '02-031', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 149.6}, {'RoomId': '02-032', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 149.6}, {'RoomId': '02-033', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 149.6}, {'RoomId': '02-034', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 149.6}, {'RoomId': '02-035', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 149.6}, {'RoomId': '02-036', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 187.85, 'PricePeakSeason': 330.62}, {'RoomId': '02-037', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 149.6}, {'RoomId': '02-038', 'Floor': '02', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 112.71, 'PricePeakSeason': 198.37}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>4445</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Pearl Lagoon</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>{'Country': 'France', 'City': 'Nice', 'ZipCode': '20758', 'Address': '26025 Pham Way'}</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>{'OccupancyPeakSeasonWeight': 94, 'OccupancyOffSeasonWeight': 21, 'OccupancyBaseDiscountPercentage': 28, 'ExtraBedChargePercentage': 22, 'MealPlanWeights': {'room_only': {'name': 'Room Only', 'weight': 0.15}, 'room_and_breakfast': {'name': 'Room and Breakfast', 'weight': 0.5}, 'all_inclusive': {'name': 'All Inclusive', 'weight': 0.01}, 'half_board': {'name': 'Half Board', 'weight': 0.2}, 'full_board': {'name': 'Full Board', 'weight': 0.14}}, 'MealPlanPrices': {'Room Only': 1.0, 'Room and Breakfast': 1.16, 'All Inclusive': 2.13, 'Half Board': 1.4, 'Full Board': 1.64}, 'PromotionPriceDiscount': 10}</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>[{'RoomId': '01-001', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 69.0, 'PricePeakSeason': 120.06}, {'RoomId': '01-002', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 107.18, 'PricePeakSeason': 186.49}, {'RoomId': '01-003', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 118.0, 'PricePeakSeason': 205.32}, {'RoomId': '01-004', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 46.0, 'PricePeakSeason': 80.04}, {'RoomId': '01-005', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 69.0, 'PricePeakSeason': 120.06}, {'RoomId': '01-006', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 107.18, 'PricePeakSeason': 186.49}, {'RoomId': '01-007', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 69.0, 'PricePeakSeason': 120.06}, {'RoomId': '01-008', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 69.0, 'PricePeakSeason': 120.06}, {'RoomId': '01-009', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 69.0, 'PricePeakSeason': 120.06}, {'RoomId': '01-010', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 69.0, 'PricePeakSeason': 120.06}, {'RoomId': '01-011', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 118.0, 'PricePeakSeason': 205.32}, {'RoomId': '01-012', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 118.0, 'PricePeakSeason': 205.32}, {'RoomId': '01-013', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 118.0, 'PricePeakSeason': 205.32}, {'RoomId': '01-014', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 274.94, 'PricePeakSeason': 478.4}, {'RoomId': '01-015', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 69.0, 'PricePeakSeason': 120.06}, {'RoomId': '01-016', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 46.0, 'PricePeakSeason': 80.04}, {'RoomId': '01-017', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 160.77, 'PricePeakSeason': 279.74}, {'RoomId': '01-018', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 69.0, 'PricePeakSeason': 120.06}, {'RoomId': '01-019', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 160.77, 'PricePeakSeason': 279.74}, {'RoomId': '01-020', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 46.0, 'PricePeakSeason': 80.04}, {'RoomId': '01-021', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 46.0, 'PricePeakSeason': 80.04}, {'RoomId': '01-022', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 274.94, 'PricePeakSeason': 478.4}, {'RoomId': '01-023', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 69.0, 'PricePeakSeason': 120.06}, {'RoomId': '01-024', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 46.0, 'PricePeakSeason': 80.04}, {'RoomId': '01-025', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 118.0, 'PricePeakSeason': 205.32}, {'RoomId': '01-026', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 160.77, 'PricePeakSeason': 279.74}, {'RoomId': '01-027', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 69.0, 'PricePeakSeason': 120.06}, {'RoomId': '01-028', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 118.0, 'PricePeakSeason': 205.32}, {'RoomId': '01-029', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 107.18, 'PricePeakSeason': 186.49}, {'RoomId': '01-030', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 274.94, 'PricePeakSeason': 478.4}, {'RoomId': '01-031', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 69.0, 'PricePeakSeason': 120.06}, {'RoomId': '01-032', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 107.18, 'PricePeakSeason': 186.49}, {'RoomId': '01-033', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 118.0, 'PricePeakSeason': 205.32}, {'RoomId': '01-034', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 118.0, 'PricePeakSeason': 205.32}, {'RoomId': '01-035', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 160.77, 'PricePeakSeason': 279.74}, {'RoomId': '01-036', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 69.0, 'PricePeakSeason': 120.06}, {'RoomId': '02-001', 'Floor': '02', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 274.94, 'PricePeakSeason': 478.4}, {'RoomId': '02-002', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 160.77, 'PricePeakSeason': 279.74}, {'RoomId': '02-003', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 46.0, 'PricePeakSeason': 80.04}, {'RoomId': '02-004', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 118.0, 'PricePeakSeason': 205.32}, {'RoomId': '02-005', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 69.0, 'PricePeakSeason': 120.06}, {'RoomId': '02-006', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 69.0, 'PricePeakSeason': 120.06}, {'RoomId': '02-007', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 69.0, 'PricePeakSeason': 120.06}, {'RoomId': '02-008', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 69.0, 'PricePeakSeason': 120.06}, {'RoomId': '02-009', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 69.0, 'PricePeakSeason': 120.06}, {'RoomId': '02-010', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 69.0, 'PricePeakSeason': 120.06}, {'RoomId': '02-011', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 118.0, 'PricePeakSeason': 205.32}, {'RoomId': '02-012', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 46.0, 'PricePeakSeason': 80.04}, {'RoomId': '02-013', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 46.0, 'PricePeakSeason': 80.04}, {'RoomId': '02-014', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 46.0, 'PricePeakSeason': 80.04}, {'RoomId': '02-015', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 69.0, 'PricePeakSeason': 120.06}, {'RoomId': '02-016', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 118.0, 'PricePeakSeason': 205.32}, {'RoomId': '02-017', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 46.0, 'PricePeakSeason': 80.04}, {'RoomId': '02-018', 'Floor': '02', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 274.94, 'PricePeakSeason': 478.4}, {'RoomId': '02-019', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 160.77, 'PricePeakSeason': 279.74}, {'RoomId': '02-020', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 69.0, 'PricePeakSeason': 120.06}, {'RoomId': '02-021', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 69.0, 'PricePeakSeason': 120.06}, {'RoomId': '02-022', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 69.0, 'PricePeakSeason': 120.06}, {'RoomId': '02-023', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 69.0, 'PricePeakSeason': 120.06}, {'RoomId': '02-024', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 69.0, 'PricePeakSeason': 120.06}, {'RoomId': '02-025', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 69.0, 'PricePeakSeason': 120.06}, {'RoomId': '02-026', 'Floor': '02', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 274.94, 'PricePeakSeason': 478.4}, {'RoomId': '02-027', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 69.0, 'PricePeakSeason': 120.06}, {'RoomId': '02-028', 'Floor': '02', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 107.18, 'PricePeakSeason': 186.49}, {'RoomId': '02-029', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 160.77, 'PricePeakSeason': 279.74}, {'RoomId': '02-030', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 69.0, 'PricePeakSeason': 120.06}, {'RoomId': '02-031', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 69.0, 'PricePeakSeason': 120.06}, {'RoomId': '02-032', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 46.0, 'PricePeakSeason': 80.04}, {'RoomId': '02-033', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 69.0, 'PricePeakSeason': 120.06}, {'RoomId': '02-034', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 118.0, 'PricePeakSeason': 205.32}, {'RoomId': '02-035', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 69.0, 'PricePeakSeason': 120.06}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2931</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Celestial Heights</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>{'Country': 'France', 'City': 'Cannes', 'ZipCode': '96846', 'Address': '2160 Walker Viaduct'}</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>{'OccupancyPeakSeasonWeight': 100, 'OccupancyOffSeasonWeight': 31, 'OccupancyBaseDiscountPercentage': 21, 'ExtraBedChargePercentage': 22, 'MealPlanWeights': {'room_only': {'name': 'Room Only', 'weight': 0.12}, 'room_and_breakfast': {'name': 'Room and Breakfast', 'weight': 0.3}, 'all_inclusive': {'name': 'All Inclusive', 'weight': 0.1}, 'half_board': {'name': 'Half Board', 'weight': 0.22}, 'full_board': {'name': 'Full Board', 'weight': 0.26}}, 'MealPlanPrices': {'Room Only': 1.0, 'Room and Breakfast': 1.12, 'All Inclusive': 2.19, 'Half Board': 1.33, 'Full Board': 1.59}, 'PromotionPriceDiscount': 20}</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>[{'RoomId': '01-001', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 95.0, 'PricePeakSeason': 147.25}, {'RoomId': '01-002', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 95.0, 'PricePeakSeason': 147.25}, {'RoomId': '01-003', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 146.0, 'PricePeakSeason': 226.3}, {'RoomId': '01-004', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 146.0, 'PricePeakSeason': 226.3}, {'RoomId': '01-005', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 95.0, 'PricePeakSeason': 147.25}, {'RoomId': '01-006', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 240.9, 'PricePeakSeason': 373.4}, {'RoomId': '01-007', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 95.0, 'PricePeakSeason': 147.25}, {'RoomId': '01-008', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 146.0, 'PricePeakSeason': 226.3}, {'RoomId': '01-009', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 95.0, 'PricePeakSeason': 147.25}, {'RoomId': '01-010', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 95.0, 'PricePeakSeason': 147.25}, {'RoomId': '01-011', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 156.75, 'PricePeakSeason': 242.96}, {'RoomId': '01-012', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 50.0, 'PricePeakSeason': 77.5}, {'RoomId': '01-013', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 95.0, 'PricePeakSeason': 147.25}, {'RoomId': '01-014', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 95.0, 'PricePeakSeason': 147.25}, {'RoomId': '01-015', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 146.0, 'PricePeakSeason': 226.3}, {'RoomId': '01-016', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 50.0, 'PricePeakSeason': 77.5}, {'RoomId': '01-017', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 156.75, 'PricePeakSeason': 242.96}, {'RoomId': '01-018', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 95.0, 'PricePeakSeason': 147.25}, {'RoomId': '01-019', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 50.0, 'PricePeakSeason': 77.5}, {'RoomId': '01-020', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 95.0, 'PricePeakSeason': 147.25}, {'RoomId': '01-021', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 95.0, 'PricePeakSeason': 147.25}, {'RoomId': '01-022', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 146.0, 'PricePeakSeason': 226.3}, {'RoomId': '01-023', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 50.0, 'PricePeakSeason': 77.5}, {'RoomId': '01-024', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 82.5, 'PricePeakSeason': 127.88}, {'RoomId': '01-025', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 156.75, 'PricePeakSeason': 242.96}, {'RoomId': '01-026', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 156.75, 'PricePeakSeason': 242.96}, {'RoomId': '01-027', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 82.5, 'PricePeakSeason': 127.88}, {'RoomId': '01-028', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 50.0, 'PricePeakSeason': 77.5}, {'RoomId': '01-029', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 156.75, 'PricePeakSeason': 242.96}, {'RoomId': '01-030', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 156.75, 'PricePeakSeason': 242.96}, {'RoomId': '01-031', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 82.5, 'PricePeakSeason': 127.88}, {'RoomId': '01-032', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 95.0, 'PricePeakSeason': 147.25}, {'RoomId': '01-033', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 82.5, 'PricePeakSeason': 127.88}, {'RoomId': '01-034', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 95.0, 'PricePeakSeason': 147.25}, {'RoomId': '01-035', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 50.0, 'PricePeakSeason': 77.5}, {'RoomId': '01-036', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 95.0, 'PricePeakSeason': 147.25}, {'RoomId': '01-037', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 50.0, 'PricePeakSeason': 77.5}, {'RoomId': '01-038', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 156.75, 'PricePeakSeason': 242.96}, {'RoomId': '01-039', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 95.0, 'PricePeakSeason': 147.25}, {'RoomId': '01-040', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 156.75, 'PricePeakSeason': 242.96}, {'RoomId': '01-041', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 95.0, 'PricePeakSeason': 147.25}, {'RoomId': '01-042', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 146.0, 'PricePeakSeason': 226.3}, {'RoomId': '01-043', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 95.0, 'PricePeakSeason': 147.25}, {'RoomId': '01-044', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 240.9, 'PricePeakSeason': 373.4}, {'RoomId': '01-045', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 95.0, 'PricePeakSeason': 147.25}, {'RoomId': '01-046', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 95.0, 'PricePeakSeason': 147.25}, {'RoomId': '01-047', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 156.75, 'PricePeakSeason': 242.96}, {'RoomId': '01-048', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 95.0, 'PricePeakSeason': 147.25}, {'RoomId': '01-049', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 95.0, 'PricePeakSeason': 147.25}, {'RoomId': '01-050', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 50.0, 'PricePeakSeason': 77.5}, {'RoomId': '01-051', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 95.0, 'PricePeakSeason': 147.25}, {'RoomId': '01-052', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 82.5, 'PricePeakSeason': 127.88}, {'RoomId': '01-053', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 95.0, 'PricePeakSeason': 147.25}, {'RoomId': '01-054', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 146.0, 'PricePeakSeason': 226.3}, {'RoomId': '01-055', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 240.9, 'PricePeakSeason': 373.4}, {'RoomId': '01-056', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 95.0, 'PricePeakSeason': 147.25}, {'RoomId': '01-057', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 95.0, 'PricePeakSeason': 147.25}, {'RoomId': '01-058', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 95.0, 'PricePeakSeason': 147.25}, {'RoomId': '01-059', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 146.0, 'PricePeakSeason': 226.3}, {'RoomId': '01-060', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 95.0, 'PricePeakSeason': 147.25}, {'RoomId': '01-061', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 50.0, 'PricePeakSeason': 77.5}, {'RoomId': '01-062', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 156.75, 'PricePeakSeason': 242.96}, {'RoomId': '01-063', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 156.75, 'PricePeakSeason': 242.96}, {'RoomId': '01-064', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 50.0, 'PricePeakSeason': 77.5}, {'RoomId': '01-065', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 95.0, 'PricePeakSeason': 147.25}, {'RoomId': '01-066', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 240.9, 'PricePeakSeason': 373.4}, {'RoomId': '01-067', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 156.75, 'PricePeakSeason': 242.96}, {'RoomId': '01-068', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 95.0, 'PricePeakSeason': 147.25}, {'RoomId': '01-069', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 156.75, 'PricePeakSeason': 242.96}, {'RoomId': '01-070', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 146.0, 'PricePeakSeason': 226.3}, {'RoomId': '01-071', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 95.0, 'PricePeakSeason': 147.25}, {'RoomId': '01-072', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 156.75, 'PricePeakSeason': 242.96}, {'RoomId': '01-073', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 156.75, 'PricePeakSeason': 242.96}, {'RoomId': '01-074', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 95.0, 'PricePeakSeason': 147.25}, {'RoomId': '01-075', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 240.9, 'PricePeakSeason': 373.4}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>0519</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Aurora Suites</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>{'Country': 'France', 'City': 'Nice', 'ZipCode': '60833', 'Address': '3303 Murphy Way Apt. 458'}</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>{'OccupancyPeakSeasonWeight': 97, 'OccupancyOffSeasonWeight': 37, 'OccupancyBaseDiscountPercentage': 21, 'ExtraBedChargePercentage': 27, 'MealPlanWeights': {'room_only': {'name': 'Room Only', 'weight': 0.17}, 'room_and_breakfast': {'name': 'Room and Breakfast', 'weight': 0.35}, 'all_inclusive': {'name': 'All Inclusive', 'weight': 0.09}, 'half_board': {'name': 'Half Board', 'weight': 0.26}, 'full_board': {'name': 'Full Board', 'weight': 0.13}}, 'MealPlanPrices': {'Room Only': 1.0, 'Room and Breakfast': 1.2, 'All Inclusive': 2.2, 'Half Board': 1.44, 'Full Board': 1.65}, 'PromotionPriceDiscount': 17}</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>[{'RoomId': '01-001', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 123.0, 'PricePeakSeason': 186.96}, {'RoomId': '01-002', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 51.0, 'PricePeakSeason': 77.52}, {'RoomId': '01-003', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 76.5, 'PricePeakSeason': 116.28}, {'RoomId': '01-004', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 123.0, 'PricePeakSeason': 186.96}, {'RoomId': '01-005', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 76.5, 'PricePeakSeason': 116.28}, {'RoomId': '01-006', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 51.0, 'PricePeakSeason': 77.52}, {'RoomId': '01-007', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 191.25, 'PricePeakSeason': 290.7}, {'RoomId': '01-008', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 191.25, 'PricePeakSeason': 290.7}, {'RoomId': '01-009', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 76.5, 'PricePeakSeason': 116.28}, {'RoomId': '01-010', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 76.5, 'PricePeakSeason': 116.28}, {'RoomId': '01-011', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 51.0, 'PricePeakSeason': 77.52}, {'RoomId': '01-012', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 191.25, 'PricePeakSeason': 290.7}, {'RoomId': '01-013', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 51.0, 'PricePeakSeason': 77.52}, {'RoomId': '01-014', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 51.0, 'PricePeakSeason': 77.52}, {'RoomId': '01-015', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 76.5, 'PricePeakSeason': 116.28}, {'RoomId': '01-016', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 76.5, 'PricePeakSeason': 116.28}, {'RoomId': '01-017', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 123.0, 'PricePeakSeason': 186.96}, {'RoomId': '01-018', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 51.0, 'PricePeakSeason': 77.52}, {'RoomId': '02-001', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 76.5, 'PricePeakSeason': 116.28}, {'RoomId': '02-002', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 51.0, 'PricePeakSeason': 77.52}, {'RoomId': '02-003', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 76.5, 'PricePeakSeason': 116.28}, {'RoomId': '02-004', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 76.5, 'PricePeakSeason': 116.28}, {'RoomId': '02-005', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 51.0, 'PricePeakSeason': 77.52}, {'RoomId': '02-006', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 76.5, 'PricePeakSeason': 116.28}, {'RoomId': '02-007', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 76.5, 'PricePeakSeason': 116.28}, {'RoomId': '02-008', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 76.5, 'PricePeakSeason': 116.28}, {'RoomId': '02-009', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 76.5, 'PricePeakSeason': 116.28}, {'RoomId': '02-010', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 76.5, 'PricePeakSeason': 116.28}, {'RoomId': '02-011', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 76.5, 'PricePeakSeason': 116.28}, {'RoomId': '02-012', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 51.0, 'PricePeakSeason': 77.52}, {'RoomId': '02-013', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 76.5, 'PricePeakSeason': 116.28}, {'RoomId': '02-014', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 76.5, 'PricePeakSeason': 116.28}, {'RoomId': '02-015', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 76.5, 'PricePeakSeason': 116.28}, {'RoomId': '02-016', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 76.5, 'PricePeakSeason': 116.28}, {'RoomId': '02-017', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 76.5, 'PricePeakSeason': 116.28}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>3667</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Stellar Hotel</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>{'Country': 'France', 'City': 'Cannes', 'ZipCode': '52887', 'Address': '14294 Daniel Mews Suite 569'}</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>{'OccupancyPeakSeasonWeight': 86, 'OccupancyOffSeasonWeight': 33, 'OccupancyBaseDiscountPercentage': 22, 'ExtraBedChargePercentage': 24, 'MealPlanWeights': {'room_only': {'name': 'Room Only', 'weight': 0.22}, 'room_and_breakfast': {'name': 'Room and Breakfast', 'weight': 0.54}, 'all_inclusive': {'name': 'All Inclusive', 'weight': 0.01}, 'half_board': {'name': 'Half Board', 'weight': 0.12}, 'full_board': {'name': 'Full Board', 'weight': 0.11}}, 'MealPlanPrices': {'Room Only': 1.0, 'Room and Breakfast': 1.2, 'All Inclusive': 2.13, 'Half Board': 1.34, 'Full Board': 1.52}, 'PromotionPriceDiscount': 14}</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>[{'RoomId': '01-001', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 138.6}, {'RoomId': '01-002', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 60.0, 'PricePeakSeason': 92.4}, {'RoomId': '01-003', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 137.7, 'PricePeakSeason': 212.06}, {'RoomId': '01-004', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 60.0, 'PricePeakSeason': 92.4}, {'RoomId': '01-005', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 206.55, 'PricePeakSeason': 318.09}, {'RoomId': '01-006', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 138.6}, {'RoomId': '01-007', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 137.7, 'PricePeakSeason': 212.06}, {'RoomId': '01-008', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 138.6}, {'RoomId': '01-009', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 137.7, 'PricePeakSeason': 212.06}, {'RoomId': '01-010', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 137.7, 'PricePeakSeason': 212.06}, {'RoomId': '01-011', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 135.0, 'PricePeakSeason': 207.9}, {'RoomId': '01-012', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 135.0, 'PricePeakSeason': 207.9}, {'RoomId': '01-013', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 135.0, 'PricePeakSeason': 207.9}, {'RoomId': '01-014', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 138.6}, {'RoomId': '01-015', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 91.8, 'PricePeakSeason': 141.37}, {'RoomId': '01-016', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 137.7, 'PricePeakSeason': 212.06}, {'RoomId': '01-017', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 138.6}, {'RoomId': '01-018', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 138.6}, {'RoomId': '01-019', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 91.8, 'PricePeakSeason': 141.37}, {'RoomId': '01-020', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 91.8, 'PricePeakSeason': 141.37}, {'RoomId': '01-021', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 135.0, 'PricePeakSeason': 207.9}, {'RoomId': '01-022', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 137.7, 'PricePeakSeason': 212.06}, {'RoomId': '01-023', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 138.6}, {'RoomId': '01-024', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 135.0, 'PricePeakSeason': 207.9}, {'RoomId': '01-025', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 206.55, 'PricePeakSeason': 318.09}, {'RoomId': '01-026', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 91.8, 'PricePeakSeason': 141.37}, {'RoomId': '01-027', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 60.0, 'PricePeakSeason': 92.4}, {'RoomId': '01-028', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 138.6}, {'RoomId': '01-029', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 60.0, 'PricePeakSeason': 92.4}, {'RoomId': '01-030', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 137.7, 'PricePeakSeason': 212.06}, {'RoomId': '01-031', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 135.0, 'PricePeakSeason': 207.9}, {'RoomId': '01-032', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 135.0, 'PricePeakSeason': 207.9}, {'RoomId': '01-033', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 135.0, 'PricePeakSeason': 207.9}, {'RoomId': '01-034', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 60.0, 'PricePeakSeason': 92.4}, {'RoomId': '01-035', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 135.0, 'PricePeakSeason': 207.9}, {'RoomId': '01-036', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 60.0, 'PricePeakSeason': 92.4}, {'RoomId': '01-037', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 138.6}, {'RoomId': '01-038', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 60.0, 'PricePeakSeason': 92.4}, {'RoomId': '01-039', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 206.55, 'PricePeakSeason': 318.09}, {'RoomId': '01-040', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 135.0, 'PricePeakSeason': 207.9}, {'RoomId': '01-041', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 137.7, 'PricePeakSeason': 212.06}, {'RoomId': '01-042', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 137.7, 'PricePeakSeason': 212.06}, {'RoomId': '01-043', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 138.6}, {'RoomId': '01-044', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 138.6}, {'RoomId': '01-045', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 137.7, 'PricePeakSeason': 212.06}, {'RoomId': '01-046', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 138.6}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>6814</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Lunar Residences</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>{'Country': 'France', 'City': 'Cannes', 'ZipCode': '67534', 'Address': '9340 Smith Valley'}</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>{'OccupancyPeakSeasonWeight': 76, 'OccupancyOffSeasonWeight': 20, 'OccupancyBaseDiscountPercentage': 29, 'ExtraBedChargePercentage': 21, 'MealPlanWeights': {'room_only': {'name': 'Room Only', 'weight': 0.11}, 'room_and_breakfast': {'name': 'Room and Breakfast', 'weight': 0.46}, 'all_inclusive': {'name': 'All Inclusive', 'weight': 0.09}, 'half_board': {'name': 'Half Board', 'weight': 0.13}, 'full_board': {'name': 'Full Board', 'weight': 0.21}}, 'MealPlanPrices': {'Room Only': 1.0, 'Room and Breakfast': 1.11, 'All Inclusive': 2.02, 'Half Board': 1.49, 'Full Board': 1.54}, 'PromotionPriceDiscount': 22}</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>[{'RoomId': '01-001', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 174.84}, {'RoomId': '01-002', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 174.84}, {'RoomId': '01-003', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 139.5, 'PricePeakSeason': 262.26}, {'RoomId': '01-004', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 62.0, 'PricePeakSeason': 116.56}, {'RoomId': '01-005', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 174.84}, {'RoomId': '01-006', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 174.84}, {'RoomId': '01-007', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 126.48, 'PricePeakSeason': 237.78}, {'RoomId': '01-008', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 174.84}, {'RoomId': '01-009', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 189.72, 'PricePeakSeason': 356.67}, {'RoomId': '01-010', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 174.84}, {'RoomId': '01-011', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 174.84}, {'RoomId': '01-012', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 174.84}, {'RoomId': '01-013', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 174.84}, {'RoomId': '01-014', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 174.84}, {'RoomId': '01-015', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 174.84}, {'RoomId': '01-016', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 189.72, 'PricePeakSeason': 356.67}, {'RoomId': '01-017', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 174.84}, {'RoomId': '01-018', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 189.72, 'PricePeakSeason': 356.67}, {'RoomId': '01-019', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 174.84}, {'RoomId': '01-020', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 189.72, 'PricePeakSeason': 356.67}, {'RoomId': '01-021', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 174.84}, {'RoomId': '01-022', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 174.84}, {'RoomId': '01-023', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 189.72, 'PricePeakSeason': 356.67}, {'RoomId': '01-024', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 174.84}, {'RoomId': '01-025', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 174.84}, {'RoomId': '01-026', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 174.84}, {'RoomId': '01-027', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 174.84}, {'RoomId': '01-028', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 62.0, 'PricePeakSeason': 116.56}, {'RoomId': '01-029', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 189.72, 'PricePeakSeason': 356.67}, {'RoomId': '01-030', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 174.84}, {'RoomId': '01-031', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 174.84}, {'RoomId': '01-032', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 139.5, 'PricePeakSeason': 262.26}, {'RoomId': '01-033', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 174.84}, {'RoomId': '01-034', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 62.0, 'PricePeakSeason': 116.56}, {'RoomId': '01-035', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 189.72, 'PricePeakSeason': 356.67}, {'RoomId': '01-036', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 174.84}, {'RoomId': '01-037', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 139.5, 'PricePeakSeason': 262.26}, {'RoomId': '01-038', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 189.72, 'PricePeakSeason': 356.67}, {'RoomId': '01-039', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 284.58, 'PricePeakSeason': 535.01}, {'RoomId': '01-040', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 174.84}, {'RoomId': '01-041', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 174.84}, {'RoomId': '01-042', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 62.0, 'PricePeakSeason': 116.56}, {'RoomId': '01-043', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 139.5, 'PricePeakSeason': 262.26}, {'RoomId': '01-044', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 174.84}, {'RoomId': '01-045', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 126.48, 'PricePeakSeason': 237.78}, {'RoomId': '01-046', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 174.84}, {'RoomId': '01-047', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 139.5, 'PricePeakSeason': 262.26}, {'RoomId': '01-048', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 189.72, 'PricePeakSeason': 356.67}, {'RoomId': '01-049', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 174.84}, {'RoomId': '01-050', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 174.84}, {'RoomId': '01-051', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 174.84}, {'RoomId': '01-052', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 189.72, 'PricePeakSeason': 356.67}, {'RoomId': '01-053', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 174.84}, {'RoomId': '01-054', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 126.48, 'PricePeakSeason': 237.78}, {'RoomId': '01-055', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 174.84}, {'RoomId': '01-056', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 189.72, 'PricePeakSeason': 356.67}, {'RoomId': '01-057', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 174.84}, {'RoomId': '01-058', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 139.5, 'PricePeakSeason': 262.26}, {'RoomId': '01-059', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 174.84}, {'RoomId': '01-060', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 174.84}, {'RoomId': '01-061', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 174.84}, {'RoomId': '01-062', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 174.84}, {'RoomId': '01-063', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 139.5, 'PricePeakSeason': 262.26}, {'RoomId': '01-064', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 62.0, 'PricePeakSeason': 116.56}, {'RoomId': '01-065', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 62.0, 'PricePeakSeason': 116.56}, {'RoomId': '01-066', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 174.84}, {'RoomId': '01-067', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 174.84}, {'RoomId': '01-068', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 93.0, 'PricePeakSeason': 174.84}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>9275</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Solar Plaza</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>{'Country': 'France', 'City': 'Paris', 'ZipCode': '71076', 'Address': '6159 Alvarado Crossing'}</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>{'OccupancyPeakSeasonWeight': 77, 'OccupancyOffSeasonWeight': 40, 'OccupancyBaseDiscountPercentage': 29, 'ExtraBedChargePercentage': 24, 'MealPlanWeights': {'room_only': {'name': 'Room Only', 'weight': 0.12}, 'room_and_breakfast': {'name': 'Room and Breakfast', 'weight': 0.48}, 'all_inclusive': {'name': 'All Inclusive', 'weight': 0.07}, 'half_board': {'name': 'Half Board', 'weight': 0.21}, 'full_board': {'name': 'Full Board', 'weight': 0.12}}, 'MealPlanPrices': {'Room Only': 1.0, 'Room and Breakfast': 1.18, 'All Inclusive': 2.14, 'Half Board': 1.43, 'Full Board': 1.57}, 'PromotionPriceDiscount': 15}</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>[{'RoomId': '01-001', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 235.62, 'PricePeakSeason': 452.39}, {'RoomId': '01-002', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 57.0, 'PricePeakSeason': 109.44}, {'RoomId': '01-003', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 235.62, 'PricePeakSeason': 452.39}, {'RoomId': '01-004', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 57.0, 'PricePeakSeason': 109.44}, {'RoomId': '01-005', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 235.62, 'PricePeakSeason': 452.39}, {'RoomId': '01-006', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 190.08}, {'RoomId': '01-007', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 235.62, 'PricePeakSeason': 452.39}, {'RoomId': '01-008', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 190.08}, {'RoomId': '01-009', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 190.08}, {'RoomId': '01-010', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 190.08}, {'RoomId': '01-011', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 235.62, 'PricePeakSeason': 452.39}, {'RoomId': '01-012', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 57.0, 'PricePeakSeason': 109.44}, {'RoomId': '01-013', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 190.08}, {'RoomId': '01-014', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 148.5, 'PricePeakSeason': 285.12}, {'RoomId': '01-015', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 190.08}, {'RoomId': '01-016', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 235.62, 'PricePeakSeason': 452.39}, {'RoomId': '01-017', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 190.08}, {'RoomId': '01-018', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 235.62, 'PricePeakSeason': 452.39}, {'RoomId': '01-019', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 148.5, 'PricePeakSeason': 285.12}, {'RoomId': '01-020', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 190.08}, {'RoomId': '01-021', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 235.62, 'PricePeakSeason': 452.39}, {'RoomId': '01-022', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 235.62, 'PricePeakSeason': 452.39}, {'RoomId': '01-023', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 148.5, 'PricePeakSeason': 285.12}, {'RoomId': '01-024', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 235.62, 'PricePeakSeason': 452.39}, {'RoomId': '01-025', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 148.5, 'PricePeakSeason': 285.12}, {'RoomId': '01-026', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 190.08}, {'RoomId': '01-027', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 190.08}, {'RoomId': '01-028', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 135.66, 'PricePeakSeason': 260.47}, {'RoomId': '01-029', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 148.5, 'PricePeakSeason': 285.12}, {'RoomId': '01-030', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 190.08}, {'RoomId': '01-031', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 235.62, 'PricePeakSeason': 452.39}, {'RoomId': '01-032', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 57.0, 'PricePeakSeason': 109.44}, {'RoomId': '01-033', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 57.0, 'PricePeakSeason': 109.44}, {'RoomId': '01-034', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 353.43, 'PricePeakSeason': 678.59}, {'RoomId': '01-035', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 235.62, 'PricePeakSeason': 452.39}, {'RoomId': '01-036', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 190.08}, {'RoomId': '01-037', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 135.66, 'PricePeakSeason': 260.47}, {'RoomId': '02-001', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 190.08}, {'RoomId': '02-002', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 190.08}, {'RoomId': '02-003', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 190.08}, {'RoomId': '02-004', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 190.08}, {'RoomId': '02-005', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 235.62, 'PricePeakSeason': 452.39}, {'RoomId': '02-006', 'Floor': '02', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 135.66, 'PricePeakSeason': 260.47}, {'RoomId': '02-007', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 190.08}, {'RoomId': '02-008', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 57.0, 'PricePeakSeason': 109.44}, {'RoomId': '02-009', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 235.62, 'PricePeakSeason': 452.39}, {'RoomId': '02-010', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 190.08}, {'RoomId': '02-011', 'Floor': '02', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 135.66, 'PricePeakSeason': 260.47}, {'RoomId': '02-012', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 148.5, 'PricePeakSeason': 285.12}, {'RoomId': '02-013', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 57.0, 'PricePeakSeason': 109.44}, {'RoomId': '02-014', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 235.62, 'PricePeakSeason': 452.39}, {'RoomId': '02-015', 'Floor': '02', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 135.66, 'PricePeakSeason': 260.47}, {'RoomId': '02-016', 'Floor': '02', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 135.66, 'PricePeakSeason': 260.47}, {'RoomId': '02-017', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 57.0, 'PricePeakSeason': 109.44}, {'RoomId': '02-018', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 190.08}, {'RoomId': '02-019', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 57.0, 'PricePeakSeason': 109.44}, {'RoomId': '02-020', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 148.5, 'PricePeakSeason': 285.12}, {'RoomId': '02-021', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 190.08}, {'RoomId': '02-022', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 235.62, 'PricePeakSeason': 452.39}, {'RoomId': '02-023', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 235.62, 'PricePeakSeason': 452.39}, {'RoomId': '02-024', 'Floor': '02', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 353.43, 'PricePeakSeason': 678.59}, {'RoomId': '02-025', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 235.62, 'PricePeakSeason': 452.39}, {'RoomId': '02-026', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 235.62, 'PricePeakSeason': 452.39}, {'RoomId': '02-027', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 148.5, 'PricePeakSeason': 285.12}, {'RoomId': '02-028', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 235.62, 'PricePeakSeason': 452.39}, {'RoomId': '02-029', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 190.08}, {'RoomId': '02-030', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 57.0, 'PricePeakSeason': 109.44}, {'RoomId': '02-031', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 190.08}, {'RoomId': '02-032', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 190.08}, {'RoomId': '02-033', 'Floor': '02', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 135.66, 'PricePeakSeason': 260.47}, {'RoomId': '02-034', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 148.5, 'PricePeakSeason': 285.12}, {'RoomId': '02-035', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 235.62, 'PricePeakSeason': 452.39}, {'RoomId': '02-036', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 99.0, 'PricePeakSeason': 190.08}, {'RoomId': '02-037', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 57.0, 'PricePeakSeason': 109.44}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>0617</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Silk Road Hotel</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>{'Country': 'France', 'City': 'Cannes', 'ZipCode': '94840', 'Address': '465 Terry Plaza Apt. 366'}</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>{'OccupancyPeakSeasonWeight': 87, 'OccupancyOffSeasonWeight': 30, 'OccupancyBaseDiscountPercentage': 28, 'ExtraBedChargePercentage': 20, 'MealPlanWeights': {'room_only': {'name': 'Room Only', 'weight': 0.11}, 'room_and_breakfast': {'name': 'Room and Breakfast', 'weight': 0.45}, 'all_inclusive': {'name': 'All Inclusive', 'weight': 0.06}, 'half_board': {'name': 'Half Board', 'weight': 0.19}, 'full_board': {'name': 'Full Board', 'weight': 0.19}}, 'MealPlanPrices': {'Room Only': 1.0, 'Room and Breakfast': 1.2, 'All Inclusive': 2.02, 'Half Board': 1.49, 'Full Board': 1.6}, 'PromotionPriceDiscount': 11}</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>[{'RoomId': '01-001', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 123.75, 'PricePeakSeason': 193.05}, {'RoomId': '01-002', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 179.03, 'PricePeakSeason': 279.29}, {'RoomId': '01-003', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 128.7}, {'RoomId': '01-004', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 55.0, 'PricePeakSeason': 85.8}, {'RoomId': '01-005', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 55.0, 'PricePeakSeason': 85.8}, {'RoomId': '01-006', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 268.54, 'PricePeakSeason': 418.92}, {'RoomId': '01-007', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 55.0, 'PricePeakSeason': 85.8}, {'RoomId': '01-008', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 119.35, 'PricePeakSeason': 186.19}, {'RoomId': '01-009', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 55.0, 'PricePeakSeason': 85.8}, {'RoomId': '01-010', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 128.7}, {'RoomId': '01-011', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 179.03, 'PricePeakSeason': 279.29}, {'RoomId': '01-012', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 55.0, 'PricePeakSeason': 85.8}, {'RoomId': '01-013', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 55.0, 'PricePeakSeason': 85.8}, {'RoomId': '01-014', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 128.7}, {'RoomId': '01-015', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 55.0, 'PricePeakSeason': 85.8}, {'RoomId': '01-016', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 128.7}, {'RoomId': '01-017', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 128.7}, {'RoomId': '01-018', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 119.35, 'PricePeakSeason': 186.19}, {'RoomId': '01-019', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 55.0, 'PricePeakSeason': 85.8}, {'RoomId': '01-020', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 128.7}, {'RoomId': '01-021', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 123.75, 'PricePeakSeason': 193.05}, {'RoomId': '02-001', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 128.7}, {'RoomId': '02-002', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 128.7}, {'RoomId': '02-003', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 128.7}, {'RoomId': '02-004', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 128.7}, {'RoomId': '02-005', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 55.0, 'PricePeakSeason': 85.8}, {'RoomId': '02-006', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 55.0, 'PricePeakSeason': 85.8}, {'RoomId': '02-007', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 55.0, 'PricePeakSeason': 85.8}, {'RoomId': '02-008', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 128.7}, {'RoomId': '02-009', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 128.7}, {'RoomId': '02-010', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 128.7}, {'RoomId': '02-011', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 128.7}, {'RoomId': '02-012', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 128.7}, {'RoomId': '02-013', 'Floor': '02', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 268.54, 'PricePeakSeason': 418.92}, {'RoomId': '02-014', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 128.7}, {'RoomId': '02-015', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 128.7}, {'RoomId': '02-016', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 123.75, 'PricePeakSeason': 193.05}, {'RoomId': '02-017', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 128.7}, {'RoomId': '02-018', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 55.0, 'PricePeakSeason': 85.8}, {'RoomId': '02-019', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 123.75, 'PricePeakSeason': 193.05}, {'RoomId': '02-020', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 128.7}, {'RoomId': '03-001', 'Floor': '03', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 123.75, 'PricePeakSeason': 193.05}, {'RoomId': '03-002', 'Floor': '03', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 268.54, 'PricePeakSeason': 418.92}, {'RoomId': '03-003', 'Floor': '03', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 179.03, 'PricePeakSeason': 279.29}, {'RoomId': '03-004', 'Floor': '03', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 123.75, 'PricePeakSeason': 193.05}, {'RoomId': '03-005', 'Floor': '03', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 179.03, 'PricePeakSeason': 279.29}, {'RoomId': '03-006', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 128.7}, {'RoomId': '03-007', 'Floor': '03', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 179.03, 'PricePeakSeason': 279.29}, {'RoomId': '03-008', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 128.7}, {'RoomId': '03-009', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 128.7}, {'RoomId': '03-010', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 128.7}, {'RoomId': '03-011', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 128.7}, {'RoomId': '03-012', 'Floor': '03', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 123.75, 'PricePeakSeason': 193.05}, {'RoomId': '03-013', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 128.7}, {'RoomId': '03-014', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 128.7}, {'RoomId': '03-015', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 128.7}, {'RoomId': '03-016', 'Floor': '03', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 179.03, 'PricePeakSeason': 279.29}, {'RoomId': '03-017', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 128.7}, {'RoomId': '03-018', 'Floor': '03', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 123.75, 'PricePeakSeason': 193.05}, {'RoomId': '03-019', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 128.7}, {'RoomId': '03-020', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 82.5, 'PricePeakSeason': 128.7}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>8434</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Savoy London</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>{'Country': 'France', 'City': 'Paris', 'ZipCode': '89278', 'Address': '946 Kevin Fords'}</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>{'OccupancyPeakSeasonWeight': 80, 'OccupancyOffSeasonWeight': 39, 'OccupancyBaseDiscountPercentage': 22, 'ExtraBedChargePercentage': 28, 'MealPlanWeights': {'room_only': {'name': 'Room Only', 'weight': 0.1}, 'room_and_breakfast': {'name': 'Room and Breakfast', 'weight': 0.47000000000000003}, 'all_inclusive': {'name': 'All Inclusive', 'weight': 0.06}, 'half_board': {'name': 'Half Board', 'weight': 0.19}, 'full_board': {'name': 'Full Board', 'weight': 0.18}}, 'MealPlanPrices': {'Room Only': 1.0, 'Room and Breakfast': 1.12, 'All Inclusive': 2.07, 'Half Board': 1.33, 'Full Board': 1.51}, 'PromotionPriceDiscount': 20}</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>[{'RoomId': '01-001', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 138.55}, {'RoomId': '01-002', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 138.55}, {'RoomId': '01-003', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 211.65, 'PricePeakSeason': 344.99}, {'RoomId': '01-004', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 211.65, 'PricePeakSeason': 344.99}, {'RoomId': '01-005', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 211.65, 'PricePeakSeason': 344.99}, {'RoomId': '01-006', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 145.0, 'PricePeakSeason': 236.35}, {'RoomId': '01-007', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 138.55}, {'RoomId': '01-008', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 138.55}, {'RoomId': '01-009', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 138.55}, {'RoomId': '01-010', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 211.65, 'PricePeakSeason': 344.99}, {'RoomId': '01-011', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 138.55}, {'RoomId': '01-012', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 211.65, 'PricePeakSeason': 344.99}, {'RoomId': '01-013', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 138.55}, {'RoomId': '01-014', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 145.0, 'PricePeakSeason': 236.35}, {'RoomId': '01-015', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 109.56, 'PricePeakSeason': 178.58}, {'RoomId': '01-016', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 109.56, 'PricePeakSeason': 178.58}, {'RoomId': '01-017', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 44.0, 'PricePeakSeason': 71.72}, {'RoomId': '01-018', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 109.56, 'PricePeakSeason': 178.58}, {'RoomId': '01-019', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 44.0, 'PricePeakSeason': 71.72}, {'RoomId': '02-001', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 44.0, 'PricePeakSeason': 71.72}, {'RoomId': '02-002', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 145.0, 'PricePeakSeason': 236.35}, {'RoomId': '02-003', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 138.55}, {'RoomId': '02-004', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 145.0, 'PricePeakSeason': 236.35}, {'RoomId': '02-005', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 138.55}, {'RoomId': '02-006', 'Floor': '02', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 109.56, 'PricePeakSeason': 178.58}, {'RoomId': '02-007', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 44.0, 'PricePeakSeason': 71.72}, {'RoomId': '02-008', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 211.65, 'PricePeakSeason': 344.99}, {'RoomId': '02-009', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 138.55}, {'RoomId': '02-010', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 138.55}, {'RoomId': '02-011', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 211.65, 'PricePeakSeason': 344.99}, {'RoomId': '02-012', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 138.55}, {'RoomId': '02-013', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 138.55}, {'RoomId': '02-014', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 145.0, 'PricePeakSeason': 236.35}, {'RoomId': '02-015', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 138.55}, {'RoomId': '02-016', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 138.55}, {'RoomId': '02-017', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 138.55}, {'RoomId': '02-018', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 85.0, 'PricePeakSeason': 138.55}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>9414</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Plaza New York</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>{'Country': 'France', 'City': 'Nice', 'ZipCode': '56847', 'Address': '7738 Leon Underpass Apt. 148'}</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>{'OccupancyPeakSeasonWeight': 90, 'OccupancyOffSeasonWeight': 37, 'OccupancyBaseDiscountPercentage': 27, 'ExtraBedChargePercentage': 23, 'MealPlanWeights': {'room_only': {'name': 'Room Only', 'weight': 0.1}, 'room_and_breakfast': {'name': 'Room and Breakfast', 'weight': 0.31}, 'all_inclusive': {'name': 'All Inclusive', 'weight': 0.03}, 'half_board': {'name': 'Half Board', 'weight': 0.29}, 'full_board': {'name': 'Full Board', 'weight': 0.27}}, 'MealPlanPrices': {'Room Only': 1.0, 'Room and Breakfast': 1.11, 'All Inclusive': 2.2, 'Half Board': 1.39, 'Full Board': 1.63}, 'PromotionPriceDiscount': 15}</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>[{'RoomId': '01-001', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 49.0, 'PricePeakSeason': 78.4}, {'RoomId': '01-002', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 128.0, 'PricePeakSeason': 204.8}, {'RoomId': '01-003', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 128.0, 'PricePeakSeason': 204.8}, {'RoomId': '01-004', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 107.31, 'PricePeakSeason': 171.7}, {'RoomId': '01-005', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 160.97, 'PricePeakSeason': 257.55}, {'RoomId': '01-006', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 73.5, 'PricePeakSeason': 117.6}, {'RoomId': '01-007', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 128.0, 'PricePeakSeason': 204.8}, {'RoomId': '01-008', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 160.97, 'PricePeakSeason': 257.55}, {'RoomId': '01-009', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 160.97, 'PricePeakSeason': 257.55}, {'RoomId': '01-010', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 160.97, 'PricePeakSeason': 257.55}, {'RoomId': '01-011', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 160.97, 'PricePeakSeason': 257.55}, {'RoomId': '01-012', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 73.5, 'PricePeakSeason': 117.6}, {'RoomId': '01-013', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 73.5, 'PricePeakSeason': 117.6}, {'RoomId': '01-014', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 49.0, 'PricePeakSeason': 78.4}, {'RoomId': '01-015', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 49.0, 'PricePeakSeason': 78.4}, {'RoomId': '01-016', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 73.5, 'PricePeakSeason': 117.6}, {'RoomId': '01-017', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 49.0, 'PricePeakSeason': 78.4}, {'RoomId': '01-018', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 73.5, 'PricePeakSeason': 117.6}, {'RoomId': '01-019', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 49.0, 'PricePeakSeason': 78.4}, {'RoomId': '01-020', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 128.0, 'PricePeakSeason': 204.8}, {'RoomId': '01-021', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 128.0, 'PricePeakSeason': 204.8}, {'RoomId': '01-022', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 160.97, 'PricePeakSeason': 257.55}, {'RoomId': '01-023', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 73.5, 'PricePeakSeason': 117.6}, {'RoomId': '01-024', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 49.0, 'PricePeakSeason': 78.4}, {'RoomId': '01-025', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 73.5, 'PricePeakSeason': 117.6}, {'RoomId': '01-026', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 73.5, 'PricePeakSeason': 117.6}, {'RoomId': '01-027', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 49.0, 'PricePeakSeason': 78.4}, {'RoomId': '01-028', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 73.5, 'PricePeakSeason': 117.6}, {'RoomId': '01-029', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 73.5, 'PricePeakSeason': 117.6}, {'RoomId': '01-030', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 128.0, 'PricePeakSeason': 204.8}, {'RoomId': '01-031', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 73.5, 'PricePeakSeason': 117.6}, {'RoomId': '01-032', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 49.0, 'PricePeakSeason': 78.4}, {'RoomId': '01-033', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 128.0, 'PricePeakSeason': 204.8}, {'RoomId': '01-034', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 73.5, 'PricePeakSeason': 117.6}, {'RoomId': '01-035', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 160.97, 'PricePeakSeason': 257.55}, {'RoomId': '01-036', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 73.5, 'PricePeakSeason': 117.6}, {'RoomId': '01-037', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 160.97, 'PricePeakSeason': 257.55}, {'RoomId': '01-038', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 128.0, 'PricePeakSeason': 204.8}, {'RoomId': '01-039', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 73.5, 'PricePeakSeason': 117.6}, {'RoomId': '01-040', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 73.5, 'PricePeakSeason': 117.6}, {'RoomId': '01-041', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 49.0, 'PricePeakSeason': 78.4}, {'RoomId': '01-042', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 73.5, 'PricePeakSeason': 117.6}, {'RoomId': '01-043', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 107.31, 'PricePeakSeason': 171.7}, {'RoomId': '01-044', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 160.97, 'PricePeakSeason': 257.55}, {'RoomId': '01-045', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 73.5, 'PricePeakSeason': 117.6}, {'RoomId': '01-046', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 73.5, 'PricePeakSeason': 117.6}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>4010</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Ritz Paris</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>{'Country': 'France', 'City': 'Paris', 'ZipCode': '87513', 'Address': '34332 Brandon Mountains Apt. 769'}</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>{'OccupancyPeakSeasonWeight': 78, 'OccupancyOffSeasonWeight': 24, 'OccupancyBaseDiscountPercentage': 26, 'ExtraBedChargePercentage': 26, 'MealPlanWeights': {'room_only': {'name': 'Room Only', 'weight': 0.14}, 'room_and_breakfast': {'name': 'Room and Breakfast', 'weight': 0.47}, 'all_inclusive': {'name': 'All Inclusive', 'weight': 0.06}, 'half_board': {'name': 'Half Board', 'weight': 0.23}, 'full_board': {'name': 'Full Board', 'weight': 0.1}}, 'MealPlanPrices': {'Room Only': 1.0, 'Room and Breakfast': 1.13, 'All Inclusive': 2.1, 'Half Board': 1.36, 'Full Board': 1.69}, 'PromotionPriceDiscount': 22}</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>[{'RoomId': '01-001', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 189.0, 'PricePeakSeason': 366.66}, {'RoomId': '01-002', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 56.0, 'PricePeakSeason': 108.64}, {'RoomId': '01-003', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 174.6}, {'RoomId': '01-004', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 174.6}, {'RoomId': '01-005', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 174.6}, {'RoomId': '01-006', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 174.6}, {'RoomId': '01-007', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 143.0, 'PricePeakSeason': 277.42}, {'RoomId': '01-008', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 174.6}, {'RoomId': '01-009', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 56.0, 'PricePeakSeason': 108.64}, {'RoomId': '01-010', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 174.6}, {'RoomId': '01-011', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 174.6}, {'RoomId': '01-012', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 174.6}, {'RoomId': '01-013', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 143.0, 'PricePeakSeason': 277.42}, {'RoomId': '01-014', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 189.0, 'PricePeakSeason': 366.66}, {'RoomId': '01-015', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 174.6}, {'RoomId': '01-016', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 174.6}, {'RoomId': '01-017', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 56.0, 'PricePeakSeason': 108.64}, {'RoomId': '01-018', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 174.6}, {'RoomId': '01-019', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 143.0, 'PricePeakSeason': 277.42}, {'RoomId': '01-020', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 56.0, 'PricePeakSeason': 108.64}, {'RoomId': '01-021', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 143.0, 'PricePeakSeason': 277.42}, {'RoomId': '01-022', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 189.0, 'PricePeakSeason': 366.66}, {'RoomId': '01-023', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 143.0, 'PricePeakSeason': 277.42}, {'RoomId': '01-024', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 189.0, 'PricePeakSeason': 366.66}, {'RoomId': '01-025', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 174.6}, {'RoomId': '01-026', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 143.0, 'PricePeakSeason': 277.42}, {'RoomId': '01-027', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 56.0, 'PricePeakSeason': 108.64}, {'RoomId': '01-028', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 174.6}, {'RoomId': '01-029', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 56.0, 'PricePeakSeason': 108.64}, {'RoomId': '01-030', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 143.0, 'PricePeakSeason': 277.42}, {'RoomId': '01-031', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 143.0, 'PricePeakSeason': 277.42}, {'RoomId': '01-032', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 174.6}, {'RoomId': '01-033', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 56.0, 'PricePeakSeason': 108.64}, {'RoomId': '01-034', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 174.6}, {'RoomId': '01-035', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 174.6}, {'RoomId': '01-036', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 143.0, 'PricePeakSeason': 277.42}, {'RoomId': '01-037', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 174.6}, {'RoomId': '01-038', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 56.0, 'PricePeakSeason': 108.64}, {'RoomId': '01-039', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 174.6}, {'RoomId': '01-040', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 56.0, 'PricePeakSeason': 108.64}, {'RoomId': '01-041', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 174.6}, {'RoomId': '01-042', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 143.0, 'PricePeakSeason': 277.42}, {'RoomId': '01-043', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 174.6}, {'RoomId': '01-044', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 56.0, 'PricePeakSeason': 108.64}, {'RoomId': '01-045', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 174.6}, {'RoomId': '01-046', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 56.0, 'PricePeakSeason': 108.64}, {'RoomId': '01-047', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 56.0, 'PricePeakSeason': 108.64}, {'RoomId': '01-048', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 174.6}, {'RoomId': '01-049', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 174.6}, {'RoomId': '01-050', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 143.0, 'PricePeakSeason': 277.42}, {'RoomId': '01-051', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 189.0, 'PricePeakSeason': 366.66}, {'RoomId': '01-052', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 56.0, 'PricePeakSeason': 108.64}, {'RoomId': '01-053', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 189.0, 'PricePeakSeason': 366.66}, {'RoomId': '01-054', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 174.6}, {'RoomId': '01-055', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 117.6, 'PricePeakSeason': 228.14}, {'RoomId': '01-056', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 56.0, 'PricePeakSeason': 108.64}, {'RoomId': '01-057', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 143.0, 'PricePeakSeason': 277.42}, {'RoomId': '01-058', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 300.3, 'PricePeakSeason': 582.58}, {'RoomId': '01-059', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 174.6}, {'RoomId': '01-060', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 174.6}, {'RoomId': '01-061', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 143.0, 'PricePeakSeason': 277.42}, {'RoomId': '01-062', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 189.0, 'PricePeakSeason': 366.66}, {'RoomId': '01-063', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 174.6}, {'RoomId': '01-064', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 174.6}, {'RoomId': '01-065', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 174.6}, {'RoomId': '01-066', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 174.6}, {'RoomId': '01-067', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 174.6}, {'RoomId': '01-068', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 174.6}, {'RoomId': '01-069', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 174.6}, {'RoomId': '01-070', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 174.6}, {'RoomId': '01-071', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 117.6, 'PricePeakSeason': 228.14}, {'RoomId': '01-072', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 143.0, 'PricePeakSeason': 277.42}, {'RoomId': '01-073', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 143.0, 'PricePeakSeason': 277.42}, {'RoomId': '01-074', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 189.0, 'PricePeakSeason': 366.66}, {'RoomId': '01-075', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 189.0, 'PricePeakSeason': 366.66}, {'RoomId': '01-076', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 174.6}, {'RoomId': '01-077', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 174.6}, {'RoomId': '01-078', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 90.0, 'PricePeakSeason': 174.6}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2012</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Danieli Venice</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>{'Country': 'France', 'City': 'Nice', 'ZipCode': '25986', 'Address': '6320 Kimberly Forges Apt. 870'}</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>{'OccupancyPeakSeasonWeight': 81, 'OccupancyOffSeasonWeight': 31, 'OccupancyBaseDiscountPercentage': 27, 'ExtraBedChargePercentage': 22, 'MealPlanWeights': {'room_only': {'name': 'Room Only', 'weight': 0.1}, 'room_and_breakfast': {'name': 'Room and Breakfast', 'weight': 0.45}, 'all_inclusive': {'name': 'All Inclusive', 'weight': 0.07}, 'half_board': {'name': 'Half Board', 'weight': 0.23}, 'full_board': {'name': 'Full Board', 'weight': 0.15}}, 'MealPlanPrices': {'Room Only': 1.0, 'Room and Breakfast': 1.2, 'All Inclusive': 2.06, 'Half Board': 1.43, 'Full Board': 1.58}, 'PromotionPriceDiscount': 19}</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>[{'RoomId': '01-001', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 343.69, 'PricePeakSeason': 646.14}, {'RoomId': '01-002', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 65.0, 'PricePeakSeason': 122.2}, {'RoomId': '01-003', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 65.0, 'PricePeakSeason': 122.2}, {'RoomId': '01-004', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 65.0, 'PricePeakSeason': 122.2}, {'RoomId': '01-005', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 152.75, 'PricePeakSeason': 287.17}, {'RoomId': '01-006', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 343.69, 'PricePeakSeason': 646.14}, {'RoomId': '01-007', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 65.0, 'PricePeakSeason': 122.2}, {'RoomId': '01-008', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.5, 'PricePeakSeason': 183.3}, {'RoomId': '01-009', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.5, 'PricePeakSeason': 183.3}, {'RoomId': '01-010', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.5, 'PricePeakSeason': 183.3}, {'RoomId': '01-011', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 229.12, 'PricePeakSeason': 430.75}, {'RoomId': '01-012', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.5, 'PricePeakSeason': 183.3}, {'RoomId': '01-013', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.5, 'PricePeakSeason': 183.3}, {'RoomId': '01-014', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.5, 'PricePeakSeason': 183.3}, {'RoomId': '01-015', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 229.12, 'PricePeakSeason': 430.75}, {'RoomId': '01-016', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.5, 'PricePeakSeason': 183.3}, {'RoomId': '01-017', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 343.69, 'PricePeakSeason': 646.14}, {'RoomId': '01-018', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.5, 'PricePeakSeason': 183.3}, {'RoomId': '01-019', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 229.12, 'PricePeakSeason': 430.75}, {'RoomId': '01-020', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 65.0, 'PricePeakSeason': 122.2}, {'RoomId': '01-021', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 229.12, 'PricePeakSeason': 430.75}, {'RoomId': '01-022', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 152.75, 'PricePeakSeason': 287.17}, {'RoomId': '01-023', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.5, 'PricePeakSeason': 183.3}, {'RoomId': '01-024', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.5, 'PricePeakSeason': 183.3}, {'RoomId': '01-025', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.5, 'PricePeakSeason': 183.3}, {'RoomId': '01-026', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.5, 'PricePeakSeason': 183.3}, {'RoomId': '02-001', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.5, 'PricePeakSeason': 183.3}, {'RoomId': '02-002', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 65.0, 'PricePeakSeason': 122.2}, {'RoomId': '02-003', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.5, 'PricePeakSeason': 183.3}, {'RoomId': '02-004', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.5, 'PricePeakSeason': 183.3}, {'RoomId': '02-005', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 229.12, 'PricePeakSeason': 430.75}, {'RoomId': '02-006', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.5, 'PricePeakSeason': 183.3}, {'RoomId': '02-007', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.5, 'PricePeakSeason': 183.3}, {'RoomId': '02-008', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 229.12, 'PricePeakSeason': 430.75}, {'RoomId': '02-009', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 229.12, 'PricePeakSeason': 430.75}, {'RoomId': '02-010', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.5, 'PricePeakSeason': 183.3}, {'RoomId': '02-011', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 229.12, 'PricePeakSeason': 430.75}, {'RoomId': '02-012', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.5, 'PricePeakSeason': 183.3}, {'RoomId': '02-013', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.5, 'PricePeakSeason': 183.3}, {'RoomId': '02-014', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.5, 'PricePeakSeason': 183.3}, {'RoomId': '02-015', 'Floor': '02', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 152.75, 'PricePeakSeason': 287.17}, {'RoomId': '02-016', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.5, 'PricePeakSeason': 183.3}, {'RoomId': '02-017', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.5, 'PricePeakSeason': 183.3}, {'RoomId': '02-018', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.5, 'PricePeakSeason': 183.3}, {'RoomId': '02-019', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 65.0, 'PricePeakSeason': 122.2}, {'RoomId': '02-020', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 65.0, 'PricePeakSeason': 122.2}, {'RoomId': '02-021', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.5, 'PricePeakSeason': 183.3}, {'RoomId': '02-022', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 65.0, 'PricePeakSeason': 122.2}, {'RoomId': '02-023', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.5, 'PricePeakSeason': 183.3}, {'RoomId': '02-024', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.5, 'PricePeakSeason': 183.3}, {'RoomId': '02-025', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 229.12, 'PricePeakSeason': 430.75}, {'RoomId': '03-001', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.5, 'PricePeakSeason': 183.3}, {'RoomId': '03-002', 'Floor': '03', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 152.75, 'PricePeakSeason': 287.17}, {'RoomId': '03-003', 'Floor': '03', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 146.25, 'PricePeakSeason': 274.95}, {'RoomId': '03-004', 'Floor': '03', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 146.25, 'PricePeakSeason': 274.95}, {'RoomId': '03-005', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.5, 'PricePeakSeason': 183.3}, {'RoomId': '03-006', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.5, 'PricePeakSeason': 183.3}, {'RoomId': '03-007', 'Floor': '03', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 229.12, 'PricePeakSeason': 430.75}, {'RoomId': '03-008', 'Floor': '03', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 229.12, 'PricePeakSeason': 430.75}, {'RoomId': '03-009', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.5, 'PricePeakSeason': 183.3}, {'RoomId': '03-010', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.5, 'PricePeakSeason': 183.3}, {'RoomId': '03-011', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.5, 'PricePeakSeason': 183.3}, {'RoomId': '03-012', 'Floor': '03', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 65.0, 'PricePeakSeason': 122.2}, {'RoomId': '03-013', 'Floor': '03', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 229.12, 'PricePeakSeason': 430.75}, {'RoomId': '03-014', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.5, 'PricePeakSeason': 183.3}, {'RoomId': '03-015', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.5, 'PricePeakSeason': 183.3}, {'RoomId': '03-016', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.5, 'PricePeakSeason': 183.3}, {'RoomId': '03-017', 'Floor': '03', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 229.12, 'PricePeakSeason': 430.75}, {'RoomId': '03-018', 'Floor': '03', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 229.12, 'PricePeakSeason': 430.75}, {'RoomId': '03-019', 'Floor': '03', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 65.0, 'PricePeakSeason': 122.2}, {'RoomId': '03-020', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.5, 'PricePeakSeason': 183.3}, {'RoomId': '03-021', 'Floor': '03', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 343.69, 'PricePeakSeason': 646.14}, {'RoomId': '03-022', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 97.5, 'PricePeakSeason': 183.3}, {'RoomId': '03-023', 'Floor': '03', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 343.69, 'PricePeakSeason': 646.14}, {'RoomId': '03-024', 'Floor': '03', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 343.69, 'PricePeakSeason': 646.14}, {'RoomId': '03-025', 'Floor': '03', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 152.75, 'PricePeakSeason': 287.17}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2632</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Raffles Singapore</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>{'Country': 'France', 'City': 'Cannes', 'ZipCode': '73561', 'Address': '72788 Dodson Mills'}</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>{'OccupancyPeakSeasonWeight': 77, 'OccupancyOffSeasonWeight': 33, 'OccupancyBaseDiscountPercentage': 25, 'ExtraBedChargePercentage': 22, 'MealPlanWeights': {'room_only': {'name': 'Room Only', 'weight': 0.15}, 'room_and_breakfast': {'name': 'Room and Breakfast', 'weight': 0.43}, 'all_inclusive': {'name': 'All Inclusive', 'weight': 0.09}, 'half_board': {'name': 'Half Board', 'weight': 0.22}, 'full_board': {'name': 'Full Board', 'weight': 0.11}}, 'MealPlanPrices': {'Room Only': 1.0, 'Room and Breakfast': 1.18, 'All Inclusive': 2.2, 'Half Board': 1.49, 'Full Board': 1.7}, 'PromotionPriceDiscount': 17}</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>[{'RoomId': '01-001', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 132.75, 'PricePeakSeason': 234.97}, {'RoomId': '01-002', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 88.5, 'PricePeakSeason': 156.65}, {'RoomId': '01-003', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 88.5, 'PricePeakSeason': 156.65}, {'RoomId': '01-004', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 88.5, 'PricePeakSeason': 156.65}, {'RoomId': '01-005', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 130.39, 'PricePeakSeason': 230.79}, {'RoomId': '01-006', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 195.59, 'PricePeakSeason': 346.19}, {'RoomId': '01-007', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 132.75, 'PricePeakSeason': 234.97}, {'RoomId': '01-008', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 88.5, 'PricePeakSeason': 156.65}, {'RoomId': '01-009', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 132.75, 'PricePeakSeason': 234.97}, {'RoomId': '01-010', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 195.59, 'PricePeakSeason': 346.19}, {'RoomId': '01-011', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 195.59, 'PricePeakSeason': 346.19}, {'RoomId': '01-012', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 293.38, 'PricePeakSeason': 519.28}, {'RoomId': '01-013', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 88.5, 'PricePeakSeason': 156.65}, {'RoomId': '01-014', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 59.0, 'PricePeakSeason': 104.43}, {'RoomId': '01-015', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 195.59, 'PricePeakSeason': 346.19}, {'RoomId': '01-016', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 195.59, 'PricePeakSeason': 346.19}, {'RoomId': '01-017', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 59.0, 'PricePeakSeason': 104.43}, {'RoomId': '01-018', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 88.5, 'PricePeakSeason': 156.65}, {'RoomId': '01-019', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 132.75, 'PricePeakSeason': 234.97}, {'RoomId': '01-020', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 195.59, 'PricePeakSeason': 346.19}, {'RoomId': '01-021', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 293.38, 'PricePeakSeason': 519.28}, {'RoomId': '01-022', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 59.0, 'PricePeakSeason': 104.43}, {'RoomId': '01-023', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 88.5, 'PricePeakSeason': 156.65}, {'RoomId': '01-024', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 132.75, 'PricePeakSeason': 234.97}, {'RoomId': '01-025', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 88.5, 'PricePeakSeason': 156.65}, {'RoomId': '01-026', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 130.39, 'PricePeakSeason': 230.79}, {'RoomId': '01-027', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 88.5, 'PricePeakSeason': 156.65}, {'RoomId': '01-028', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 88.5, 'PricePeakSeason': 156.65}, {'RoomId': '01-029', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 130.39, 'PricePeakSeason': 230.79}, {'RoomId': '01-030', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 88.5, 'PricePeakSeason': 156.65}, {'RoomId': '01-031', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 88.5, 'PricePeakSeason': 156.65}, {'RoomId': '01-032', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 130.39, 'PricePeakSeason': 230.79}, {'RoomId': '01-033', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 195.59, 'PricePeakSeason': 346.19}, {'RoomId': '01-034', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 132.75, 'PricePeakSeason': 234.97}, {'RoomId': '01-035', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 195.59, 'PricePeakSeason': 346.19}, {'RoomId': '01-036', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 88.5, 'PricePeakSeason': 156.65}, {'RoomId': '01-037', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 293.38, 'PricePeakSeason': 519.28}, {'RoomId': '01-038', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 195.59, 'PricePeakSeason': 346.19}, {'RoomId': '01-039', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 88.5, 'PricePeakSeason': 156.65}, {'RoomId': '01-040', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 132.75, 'PricePeakSeason': 234.97}, {'RoomId': '01-041', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 293.38, 'PricePeakSeason': 519.28}, {'RoomId': '01-042', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 132.75, 'PricePeakSeason': 234.97}, {'RoomId': '01-043', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 195.59, 'PricePeakSeason': 346.19}, {'RoomId': '01-044', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 130.39, 'PricePeakSeason': 230.79}, {'RoomId': '01-045', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 88.5, 'PricePeakSeason': 156.65}, {'RoomId': '01-046', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 195.59, 'PricePeakSeason': 346.19}, {'RoomId': '01-047', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 195.59, 'PricePeakSeason': 346.19}, {'RoomId': '01-048', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 88.5, 'PricePeakSeason': 156.65}, {'RoomId': '01-049', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 88.5, 'PricePeakSeason': 156.65}, {'RoomId': '01-050', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 195.59, 'PricePeakSeason': 346.19}, {'RoomId': '01-051', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 132.75, 'PricePeakSeason': 234.97}, {'RoomId': '01-052', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 59.0, 'PricePeakSeason': 104.43}, {'RoomId': '01-053', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 59.0, 'PricePeakSeason': 104.43}, {'RoomId': '01-054', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 88.5, 'PricePeakSeason': 156.65}, {'RoomId': '01-055', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 88.5, 'PricePeakSeason': 156.65}, {'RoomId': '01-056', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 195.59, 'PricePeakSeason': 346.19}, {'RoomId': '01-057', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 130.39, 'PricePeakSeason': 230.79}, {'RoomId': '01-058', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 88.5, 'PricePeakSeason': 156.65}, {'RoomId': '01-059', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 59.0, 'PricePeakSeason': 104.43}, {'RoomId': '01-060', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 88.5, 'PricePeakSeason': 156.65}, {'RoomId': '01-061', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 88.5, 'PricePeakSeason': 156.65}, {'RoomId': '01-062', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 195.59, 'PricePeakSeason': 346.19}, {'RoomId': '01-063', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 130.39, 'PricePeakSeason': 230.79}, {'RoomId': '01-064', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 88.5, 'PricePeakSeason': 156.65}, {'RoomId': '01-065', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 195.59, 'PricePeakSeason': 346.19}, {'RoomId': '01-066', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 130.39, 'PricePeakSeason': 230.79}, {'RoomId': '01-067', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 88.5, 'PricePeakSeason': 156.65}, {'RoomId': '01-068', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 88.5, 'PricePeakSeason': 156.65}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>1458</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Peninsula Hong Kong</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>{'Country': 'France', 'City': 'Paris', 'ZipCode': '80802', 'Address': '727 Green Gateway Suite 873'}</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>{'OccupancyPeakSeasonWeight': 90, 'OccupancyOffSeasonWeight': 21, 'OccupancyBaseDiscountPercentage': 27, 'ExtraBedChargePercentage': 25, 'MealPlanWeights': {'room_only': {'name': 'Room Only', 'weight': 0.19}, 'room_and_breakfast': {'name': 'Room and Breakfast', 'weight': 0.43}, 'all_inclusive': {'name': 'All Inclusive', 'weight': 0.05}, 'half_board': {'name': 'Half Board', 'weight': 0.11}, 'full_board': {'name': 'Full Board', 'weight': 0.22}}, 'MealPlanPrices': {'Room Only': 1.0, 'Room and Breakfast': 1.11, 'All Inclusive': 2.11, 'Half Board': 1.32, 'Full Board': 1.56}, 'PromotionPriceDiscount': 19}</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>[{'RoomId': '01-001', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.5, 'PricePeakSeason': 141.75}, {'RoomId': '01-002', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 155.92, 'PricePeakSeason': 233.88}, {'RoomId': '01-003', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 63.0, 'PricePeakSeason': 94.5}, {'RoomId': '01-004', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 63.0, 'PricePeakSeason': 94.5}, {'RoomId': '01-005', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.5, 'PricePeakSeason': 141.75}, {'RoomId': '01-006', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.5, 'PricePeakSeason': 141.75}, {'RoomId': '01-007', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 141.75, 'PricePeakSeason': 212.62}, {'RoomId': '01-008', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 141.75, 'PricePeakSeason': 212.62}, {'RoomId': '01-009', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.5, 'PricePeakSeason': 141.75}, {'RoomId': '01-010', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.5, 'PricePeakSeason': 141.75}, {'RoomId': '01-011', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.5, 'PricePeakSeason': 141.75}, {'RoomId': '01-012', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.5, 'PricePeakSeason': 141.75}, {'RoomId': '01-013', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 155.92, 'PricePeakSeason': 233.88}, {'RoomId': '01-014', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.5, 'PricePeakSeason': 141.75}, {'RoomId': '01-015', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 63.0, 'PricePeakSeason': 94.5}, {'RoomId': '01-016', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.5, 'PricePeakSeason': 141.75}, {'RoomId': '01-017', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.5, 'PricePeakSeason': 141.75}, {'RoomId': '01-018', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.5, 'PricePeakSeason': 141.75}, {'RoomId': '01-019', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 63.0, 'PricePeakSeason': 94.5}, {'RoomId': '01-020', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.5, 'PricePeakSeason': 141.75}, {'RoomId': '01-021', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 141.75, 'PricePeakSeason': 212.62}, {'RoomId': '01-022', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 233.89, 'PricePeakSeason': 350.83}, {'RoomId': '01-023', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 155.92, 'PricePeakSeason': 233.88}, {'RoomId': '01-024', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 63.0, 'PricePeakSeason': 94.5}, {'RoomId': '01-025', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.5, 'PricePeakSeason': 141.75}, {'RoomId': '01-026', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.5, 'PricePeakSeason': 141.75}, {'RoomId': '01-027', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 141.75, 'PricePeakSeason': 212.62}, {'RoomId': '01-028', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.5, 'PricePeakSeason': 141.75}, {'RoomId': '01-029', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.5, 'PricePeakSeason': 141.75}, {'RoomId': '01-030', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 233.89, 'PricePeakSeason': 350.83}, {'RoomId': '01-031', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.5, 'PricePeakSeason': 141.75}, {'RoomId': '01-032', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 63.0, 'PricePeakSeason': 94.5}, {'RoomId': '01-033', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 63.0, 'PricePeakSeason': 94.5}, {'RoomId': '01-034', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 141.75, 'PricePeakSeason': 212.62}, {'RoomId': '01-035', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.5, 'PricePeakSeason': 141.75}, {'RoomId': '01-036', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 155.92, 'PricePeakSeason': 233.88}, {'RoomId': '01-037', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.5, 'PricePeakSeason': 141.75}, {'RoomId': '01-038', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.5, 'PricePeakSeason': 141.75}, {'RoomId': '01-039', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 141.75, 'PricePeakSeason': 212.62}, {'RoomId': '01-040', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 141.75, 'PricePeakSeason': 212.62}, {'RoomId': '01-041', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 63.0, 'PricePeakSeason': 94.5}, {'RoomId': '01-042', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.5, 'PricePeakSeason': 141.75}, {'RoomId': '01-043', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 63.0, 'PricePeakSeason': 94.5}, {'RoomId': '01-044', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 63.0, 'PricePeakSeason': 94.5}, {'RoomId': '01-045', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.5, 'PricePeakSeason': 141.75}, {'RoomId': '01-046', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 94.5, 'PricePeakSeason': 141.75}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2960</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Adlon Berlin</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>{'Country': 'France', 'City': 'Cannes', 'ZipCode': '36493', 'Address': '43455 Devon Fort Suite 231'}</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>{'OccupancyPeakSeasonWeight': 98, 'OccupancyOffSeasonWeight': 39, 'OccupancyBaseDiscountPercentage': 27, 'ExtraBedChargePercentage': 24, 'MealPlanWeights': {'room_only': {'name': 'Room Only', 'weight': 0.13}, 'room_and_breakfast': {'name': 'Room and Breakfast', 'weight': 0.47}, 'all_inclusive': {'name': 'All Inclusive', 'weight': 0.03}, 'half_board': {'name': 'Half Board', 'weight': 0.18}, 'full_board': {'name': 'Full Board', 'weight': 0.19}}, 'MealPlanPrices': {'Room Only': 1.0, 'Room and Breakfast': 1.14, 'All Inclusive': 2.02, 'Half Board': 1.34, 'Full Board': 1.54}, 'PromotionPriceDiscount': 10}</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>[{'RoomId': '01-001', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 181.26, 'PricePeakSeason': 299.08}, {'RoomId': '01-002', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 120.84, 'PricePeakSeason': 199.39}, {'RoomId': '01-003', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 188.1}, {'RoomId': '01-004', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 188.1}, {'RoomId': '01-005', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 271.89, 'PricePeakSeason': 448.62}, {'RoomId': '01-006', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 76.0, 'PricePeakSeason': 125.4}, {'RoomId': '01-007', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 181.26, 'PricePeakSeason': 299.08}, {'RoomId': '01-008', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 171.0, 'PricePeakSeason': 282.15}, {'RoomId': '01-009', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 76.0, 'PricePeakSeason': 125.4}, {'RoomId': '01-010', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 181.26, 'PricePeakSeason': 299.08}, {'RoomId': '01-011', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 181.26, 'PricePeakSeason': 299.08}, {'RoomId': '01-012', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 188.1}, {'RoomId': '01-013', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 181.26, 'PricePeakSeason': 299.08}, {'RoomId': '01-014', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 76.0, 'PricePeakSeason': 125.4}, {'RoomId': '01-015', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 188.1}, {'RoomId': '01-016', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 76.0, 'PricePeakSeason': 125.4}, {'RoomId': '01-017', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 181.26, 'PricePeakSeason': 299.08}, {'RoomId': '01-018', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 76.0, 'PricePeakSeason': 125.4}, {'RoomId': '01-019', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 271.89, 'PricePeakSeason': 448.62}, {'RoomId': '01-020', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 171.0, 'PricePeakSeason': 282.15}, {'RoomId': '01-021', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 171.0, 'PricePeakSeason': 282.15}, {'RoomId': '02-001', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 171.0, 'PricePeakSeason': 282.15}, {'RoomId': '02-002', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 76.0, 'PricePeakSeason': 125.4}, {'RoomId': '02-003', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 188.1}, {'RoomId': '02-004', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 181.26, 'PricePeakSeason': 299.08}, {'RoomId': '02-005', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 76.0, 'PricePeakSeason': 125.4}, {'RoomId': '02-006', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 171.0, 'PricePeakSeason': 282.15}, {'RoomId': '02-007', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 188.1}, {'RoomId': '02-008', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 181.26, 'PricePeakSeason': 299.08}, {'RoomId': '02-009', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 188.1}, {'RoomId': '02-010', 'Floor': '02', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 271.89, 'PricePeakSeason': 448.62}, {'RoomId': '02-011', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 188.1}, {'RoomId': '02-012', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 76.0, 'PricePeakSeason': 125.4}, {'RoomId': '02-013', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 188.1}, {'RoomId': '02-014', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 188.1}, {'RoomId': '02-015', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 188.1}, {'RoomId': '02-016', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 188.1}, {'RoomId': '02-017', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 188.1}, {'RoomId': '02-018', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 181.26, 'PricePeakSeason': 299.08}, {'RoomId': '02-019', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 76.0, 'PricePeakSeason': 125.4}, {'RoomId': '02-020', 'Floor': '02', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 271.89, 'PricePeakSeason': 448.62}, {'RoomId': '02-021', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 188.1}, {'RoomId': '03-001', 'Floor': '03', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 76.0, 'PricePeakSeason': 125.4}, {'RoomId': '03-002', 'Floor': '03', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 76.0, 'PricePeakSeason': 125.4}, {'RoomId': '03-003', 'Floor': '03', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 76.0, 'PricePeakSeason': 125.4}, {'RoomId': '03-004', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 188.1}, {'RoomId': '03-005', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 188.1}, {'RoomId': '03-006', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 188.1}, {'RoomId': '03-007', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 188.1}, {'RoomId': '03-008', 'Floor': '03', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 76.0, 'PricePeakSeason': 125.4}, {'RoomId': '03-009', 'Floor': '03', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 76.0, 'PricePeakSeason': 125.4}, {'RoomId': '03-010', 'Floor': '03', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 181.26, 'PricePeakSeason': 299.08}, {'RoomId': '03-011', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 188.1}, {'RoomId': '03-012', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 188.1}, {'RoomId': '03-013', 'Floor': '03', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 171.0, 'PricePeakSeason': 282.15}, {'RoomId': '03-014', 'Floor': '03', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 120.84, 'PricePeakSeason': 199.39}, {'RoomId': '03-015', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 188.1}, {'RoomId': '03-016', 'Floor': '03', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 171.0, 'PricePeakSeason': 282.15}, {'RoomId': '03-017', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 188.1}, {'RoomId': '03-018', 'Floor': '03', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 76.0, 'PricePeakSeason': 125.4}, {'RoomId': '03-019', 'Floor': '03', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 114.0, 'PricePeakSeason': 188.1}, {'RoomId': '03-020', 'Floor': '03', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 171.0, 'PricePeakSeason': 282.15}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>3127</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Imperial Vienna</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>{'Country': 'France', 'City': 'Paris', 'ZipCode': '54878', 'Address': '8760 Marissa Loaf Apt. 967'}</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>{'OccupancyPeakSeasonWeight': 75, 'OccupancyOffSeasonWeight': 34, 'OccupancyBaseDiscountPercentage': 22, 'ExtraBedChargePercentage': 20, 'MealPlanWeights': {'room_only': {'name': 'Room Only', 'weight': 0.17}, 'room_and_breakfast': {'name': 'Room and Breakfast', 'weight': 0.47000000000000003}, 'all_inclusive': {'name': 'All Inclusive', 'weight': 0.01}, 'half_board': {'name': 'Half Board', 'weight': 0.17}, 'full_board': {'name': 'Full Board', 'weight': 0.18}}, 'MealPlanPrices': {'Room Only': 1.0, 'Room and Breakfast': 1.16, 'All Inclusive': 2.01, 'Half Board': 1.42, 'Full Board': 1.51}, 'PromotionPriceDiscount': 30}</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>[{'RoomId': '01-001', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 120.0, 'PricePeakSeason': 186.0}, {'RoomId': '01-002', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 80.0, 'PricePeakSeason': 124.0}, {'RoomId': '01-003', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 80.0, 'PricePeakSeason': 124.0}, {'RoomId': '01-004', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 313.2, 'PricePeakSeason': 485.46}, {'RoomId': '01-005', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 180.0, 'PricePeakSeason': 279.0}, {'RoomId': '01-006', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 80.0, 'PricePeakSeason': 124.0}, {'RoomId': '01-007', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 120.0, 'PricePeakSeason': 186.0}, {'RoomId': '01-008', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 80.0, 'PricePeakSeason': 124.0}, {'RoomId': '01-009', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 120.0, 'PricePeakSeason': 186.0}, {'RoomId': '01-010', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 313.2, 'PricePeakSeason': 485.46}, {'RoomId': '01-011', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 208.8, 'PricePeakSeason': 323.64}, {'RoomId': '01-012', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 120.0, 'PricePeakSeason': 186.0}, {'RoomId': '01-013', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 120.0, 'PricePeakSeason': 186.0}, {'RoomId': '01-014', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 120.0, 'PricePeakSeason': 186.0}, {'RoomId': '01-015', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 208.8, 'PricePeakSeason': 323.64}, {'RoomId': '01-016', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 120.0, 'PricePeakSeason': 186.0}, {'RoomId': '01-017', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 120.0, 'PricePeakSeason': 186.0}, {'RoomId': '01-018', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 80.0, 'PricePeakSeason': 124.0}, {'RoomId': '01-019', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 208.8, 'PricePeakSeason': 323.64}, {'RoomId': '01-020', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 120.0, 'PricePeakSeason': 186.0}, {'RoomId': '01-021', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 208.8, 'PricePeakSeason': 323.64}, {'RoomId': '01-022', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 139.2, 'PricePeakSeason': 215.76}, {'RoomId': '01-023', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 80.0, 'PricePeakSeason': 124.0}, {'RoomId': '01-024', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 80.0, 'PricePeakSeason': 124.0}, {'RoomId': '01-025', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 180.0, 'PricePeakSeason': 279.0}, {'RoomId': '01-026', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 120.0, 'PricePeakSeason': 186.0}, {'RoomId': '01-027', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 208.8, 'PricePeakSeason': 323.64}, {'RoomId': '01-028', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 120.0, 'PricePeakSeason': 186.0}, {'RoomId': '01-029', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 313.2, 'PricePeakSeason': 485.46}, {'RoomId': '01-030', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 208.8, 'PricePeakSeason': 323.64}, {'RoomId': '01-031', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 208.8, 'PricePeakSeason': 323.64}, {'RoomId': '01-032', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 313.2, 'PricePeakSeason': 485.46}, {'RoomId': '01-033', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 120.0, 'PricePeakSeason': 186.0}, {'RoomId': '01-034', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 208.8, 'PricePeakSeason': 323.64}, {'RoomId': '01-035', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 80.0, 'PricePeakSeason': 124.0}, {'RoomId': '01-036', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 80.0, 'PricePeakSeason': 124.0}, {'RoomId': '01-037', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 180.0, 'PricePeakSeason': 279.0}, {'RoomId': '01-038', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 80.0, 'PricePeakSeason': 124.0}, {'RoomId': '01-039', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 80.0, 'PricePeakSeason': 124.0}, {'RoomId': '01-040', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 208.8, 'PricePeakSeason': 323.64}, {'RoomId': '01-041', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 120.0, 'PricePeakSeason': 186.0}, {'RoomId': '01-042', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 139.2, 'PricePeakSeason': 215.76}, {'RoomId': '01-043', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 120.0, 'PricePeakSeason': 186.0}, {'RoomId': '01-044', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 80.0, 'PricePeakSeason': 124.0}, {'RoomId': '01-045', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 80.0, 'PricePeakSeason': 124.0}, {'RoomId': '01-046', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 120.0, 'PricePeakSeason': 186.0}, {'RoomId': '01-047', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 180.0, 'PricePeakSeason': 279.0}, {'RoomId': '01-048', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 80.0, 'PricePeakSeason': 124.0}, {'RoomId': '01-049', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 208.8, 'PricePeakSeason': 323.64}, {'RoomId': '01-050', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 208.8, 'PricePeakSeason': 323.64}, {'RoomId': '01-051', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 208.8, 'PricePeakSeason': 323.64}, {'RoomId': '01-052', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 180.0, 'PricePeakSeason': 279.0}, {'RoomId': '01-053', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 80.0, 'PricePeakSeason': 124.0}, {'RoomId': '01-054', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 120.0, 'PricePeakSeason': 186.0}, {'RoomId': '01-055', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 208.8, 'PricePeakSeason': 323.64}, {'RoomId': '01-056', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 80.0, 'PricePeakSeason': 124.0}, {'RoomId': '01-057', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 180.0, 'PricePeakSeason': 279.0}, {'RoomId': '01-058', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 139.2, 'PricePeakSeason': 215.76}, {'RoomId': '01-059', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 120.0, 'PricePeakSeason': 186.0}, {'RoomId': '01-060', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 120.0, 'PricePeakSeason': 186.0}, {'RoomId': '01-061', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 120.0, 'PricePeakSeason': 186.0}, {'RoomId': '01-062', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 80.0, 'PricePeakSeason': 124.0}, {'RoomId': '01-063', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 208.8, 'PricePeakSeason': 323.64}, {'RoomId': '01-064', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 120.0, 'PricePeakSeason': 186.0}, {'RoomId': '01-065', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 120.0, 'PricePeakSeason': 186.0}, {'RoomId': '01-066', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 120.0, 'PricePeakSeason': 186.0}, {'RoomId': '01-067', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 120.0, 'PricePeakSeason': 186.0}, {'RoomId': '01-068', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 208.8, 'PricePeakSeason': 323.64}, {'RoomId': '01-069', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 139.2, 'PricePeakSeason': 215.76}, {'RoomId': '01-070', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 208.8, 'PricePeakSeason': 323.64}, {'RoomId': '01-071', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 120.0, 'PricePeakSeason': 186.0}, {'RoomId': '01-072', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 120.0, 'PricePeakSeason': 186.0}, {'RoomId': '01-073', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 180.0, 'PricePeakSeason': 279.0}, {'RoomId': '01-074', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 208.8, 'PricePeakSeason': 323.64}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2474</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Cipriani Venice</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>{'Country': 'France', 'City': 'Cannes', 'ZipCode': '01273', 'Address': '6688 Tracy Groves Suite 706'}</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>{'OccupancyPeakSeasonWeight': 100, 'OccupancyOffSeasonWeight': 29, 'OccupancyBaseDiscountPercentage': 28, 'ExtraBedChargePercentage': 30, 'MealPlanWeights': {'room_only': {'name': 'Room Only', 'weight': 0.11}, 'room_and_breakfast': {'name': 'Room and Breakfast', 'weight': 0.45}, 'all_inclusive': {'name': 'All Inclusive', 'weight': 0.02}, 'half_board': {'name': 'Half Board', 'weight': 0.21}, 'full_board': {'name': 'Full Board', 'weight': 0.21}}, 'MealPlanPrices': {'Room Only': 1.0, 'Room and Breakfast': 1.19, 'All Inclusive': 2.16, 'Half Board': 1.36, 'Full Board': 1.65}, 'PromotionPriceDiscount': 26}</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>[{'RoomId': '01-001', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 165.12}, {'RoomId': '01-002', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 147.0, 'PricePeakSeason': 252.84}, {'RoomId': '01-003', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 182.4, 'PricePeakSeason': 313.73}, {'RoomId': '01-004', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 165.12}, {'RoomId': '01-005', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 182.4, 'PricePeakSeason': 313.73}, {'RoomId': '01-006', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 279.3, 'PricePeakSeason': 480.4}, {'RoomId': '01-007', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 182.4, 'PricePeakSeason': 313.73}, {'RoomId': '01-008', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 165.12}, {'RoomId': '01-009', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 165.12}, {'RoomId': '01-010', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 182.4, 'PricePeakSeason': 313.73}, {'RoomId': '01-011', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 147.0, 'PricePeakSeason': 252.84}, {'RoomId': '01-012', 'Floor': '01', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 59.0, 'PricePeakSeason': 101.48}, {'RoomId': '01-013', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 165.12}, {'RoomId': '01-014', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 112.1, 'PricePeakSeason': 192.81}, {'RoomId': '01-015', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 147.0, 'PricePeakSeason': 252.84}, {'RoomId': '01-016', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 165.12}, {'RoomId': '01-017', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 182.4, 'PricePeakSeason': 313.73}, {'RoomId': '01-018', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 112.1, 'PricePeakSeason': 192.81}, {'RoomId': '01-019', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 165.12}, {'RoomId': '01-020', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 165.12}, {'RoomId': '01-021', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 165.12}, {'RoomId': '01-022', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 165.12}, {'RoomId': '01-023', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 182.4, 'PricePeakSeason': 313.73}, {'RoomId': '01-024', 'Floor': '01', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 279.3, 'PricePeakSeason': 480.4}, {'RoomId': '01-025', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 182.4, 'PricePeakSeason': 313.73}, {'RoomId': '01-026', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 182.4, 'PricePeakSeason': 313.73}, {'RoomId': '01-027', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 165.12}, {'RoomId': '01-028', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 165.12}, {'RoomId': '01-029', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 182.4, 'PricePeakSeason': 313.73}, {'RoomId': '01-030', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 182.4, 'PricePeakSeason': 313.73}, {'RoomId': '01-031', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 165.12}, {'RoomId': '01-032', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 165.12}, {'RoomId': '01-033', 'Floor': '01', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 182.4, 'PricePeakSeason': 313.73}, {'RoomId': '01-034', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 165.12}, {'RoomId': '01-035', 'Floor': '01', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 112.1, 'PricePeakSeason': 192.81}, {'RoomId': '01-036', 'Floor': '01', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 147.0, 'PricePeakSeason': 252.84}, {'RoomId': '01-037', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 165.12}, {'RoomId': '01-038', 'Floor': '01', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 165.12}, {'RoomId': '02-001', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 165.12}, {'RoomId': '02-002', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 165.12}, {'RoomId': '02-003', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 165.12}, {'RoomId': '02-004', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 147.0, 'PricePeakSeason': 252.84}, {'RoomId': '02-005', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 147.0, 'PricePeakSeason': 252.84}, {'RoomId': '02-006', 'Floor': '02', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 112.1, 'PricePeakSeason': 192.81}, {'RoomId': '02-007', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 165.12}, {'RoomId': '02-008', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 165.12}, {'RoomId': '02-009', 'Floor': '02', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 112.1, 'PricePeakSeason': 192.81}, {'RoomId': '02-010', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 165.12}, {'RoomId': '02-011', 'Floor': '02', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 279.3, 'PricePeakSeason': 480.4}, {'RoomId': '02-012', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 147.0, 'PricePeakSeason': 252.84}, {'RoomId': '02-013', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 165.12}, {'RoomId': '02-014', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 165.12}, {'RoomId': '02-015', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 59.0, 'PricePeakSeason': 101.48}, {'RoomId': '02-016', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 147.0, 'PricePeakSeason': 252.84}, {'RoomId': '02-017', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 165.12}, {'RoomId': '02-018', 'Floor': '02', 'Category': 'Premium', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 112.1, 'PricePeakSeason': 192.81}, {'RoomId': '02-019', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 59.0, 'PricePeakSeason': 101.48}, {'RoomId': '02-020', 'Floor': '02', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 279.3, 'PricePeakSeason': 480.4}, {'RoomId': '02-021', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 147.0, 'PricePeakSeason': 252.84}, {'RoomId': '02-022', 'Floor': '02', 'Category': 'Standard', 'Type': 'Single', 'Guests': 1, 'PriceOffSeason': 59.0, 'PricePeakSeason': 101.48}, {'RoomId': '02-023', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 147.0, 'PricePeakSeason': 252.84}, {'RoomId': '02-024', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 165.12}, {'RoomId': '02-025', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 147.0, 'PricePeakSeason': 252.84}, {'RoomId': '02-026', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 182.4, 'PricePeakSeason': 313.73}, {'RoomId': '02-027', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 182.4, 'PricePeakSeason': 313.73}, {'RoomId': '02-028', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 182.4, 'PricePeakSeason': 313.73}, {'RoomId': '02-029', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 165.12}, {'RoomId': '02-030', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 147.0, 'PricePeakSeason': 252.84}, {'RoomId': '02-031', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 147.0, 'PricePeakSeason': 252.84}, {'RoomId': '02-032', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 182.4, 'PricePeakSeason': 313.73}, {'RoomId': '02-033', 'Floor': '02', 'Category': 'Standard', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 96.0, 'PricePeakSeason': 165.12}, {'RoomId': '02-034', 'Floor': '02', 'Category': 'Standard', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 147.0, 'PricePeakSeason': 252.84}, {'RoomId': '02-035', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 182.4, 'PricePeakSeason': 313.73}, {'RoomId': '02-036', 'Floor': '02', 'Category': 'Premium', 'Type': 'Triple', 'Guests': 3, 'PriceOffSeason': 279.3, 'PricePeakSeason': 480.4}, {'RoomId': '02-037', 'Floor': '02', 'Category': 'Premium', 'Type': 'Double', 'Guests': 2, 'PriceOffSeason': 182.4, 'PricePeakSeason': 313.73}]</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>